<commit_message>
add Aragón and Madrid hospitalized data by provinces 2020.05.27
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C50F932-20AA-43A1-9FA9-20E5DAE6D9DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B48368A-F5A4-49A5-A8BF-BB588323DDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9456" yWindow="2832" windowWidth="19368" windowHeight="6720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10620" yWindow="3252" windowWidth="17280" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4212" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1052"/>
+  <dimension ref="A1:J1112"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -26604,6 +26604,1434 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1053" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1053" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1053" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1053" s="3">
+        <v>11</v>
+      </c>
+      <c r="D1053" s="3">
+        <v>5</v>
+      </c>
+      <c r="E1053" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1053" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1053" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1053" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1054" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1054" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1054" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1054" s="3">
+        <v>35</v>
+      </c>
+      <c r="D1054" s="4"/>
+      <c r="E1054" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1054" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1054" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1054" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1055" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1055" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1055" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1055" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1055" s="3"/>
+      <c r="E1055" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1055" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1055" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1055" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1056" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1056" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1056" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1056" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1056" s="3"/>
+      <c r="E1056" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1056" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1056" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1056" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1057" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1057" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1057" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1057" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1057" s="4"/>
+      <c r="E1057" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1057" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1057" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1057" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1058" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1058" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1058" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1058" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1058" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1058" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1058" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1058" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1058" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1059" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1059" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1059" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1059" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1059" s="4"/>
+      <c r="E1059" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1059" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1059" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1059" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1060" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1060" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1060" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1060" s="3">
+        <v>17</v>
+      </c>
+      <c r="D1060" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1060" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1060" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1060" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1060" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1061" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1061" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1061" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1061" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1061" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1061" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1061" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1061" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1061" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1062" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1062" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1062" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1062" s="4"/>
+      <c r="D1062" s="4"/>
+      <c r="E1062" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1062" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1062" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1062" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1063" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1063" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1063" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1063" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1063" s="3"/>
+      <c r="E1063" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1063" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1063" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1063" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1064" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1064" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1064" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1064" s="3">
+        <v>12</v>
+      </c>
+      <c r="D1064" s="3"/>
+      <c r="E1064" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1064" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1064" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1064" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1065" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1065" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1065" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1065" s="3"/>
+      <c r="D1065" s="4"/>
+      <c r="E1065" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1065" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1065" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1065" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1066" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1066" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1066" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1066" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1066" s="6"/>
+      <c r="E1066" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1066" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1066" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1066" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1067" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1067" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1067" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1067" s="3"/>
+      <c r="D1067" s="6"/>
+      <c r="E1067" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1067" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1067" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1067" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1068" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1068" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1068" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1068" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1068" s="6"/>
+      <c r="E1068" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1068" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1068" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1068" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1069" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1069" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1069" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1069" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1069" s="6"/>
+      <c r="E1069" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1069" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1069" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1069" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1070" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1070" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1070" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1070" s="3"/>
+      <c r="D1070" s="6"/>
+      <c r="E1070" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1070" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1070" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1070" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1071" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1071" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1071" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1071" s="3"/>
+      <c r="D1071" s="6"/>
+      <c r="E1071" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1071" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1071" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1071" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1072" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1072" s="2">
+        <v>43977</v>
+      </c>
+      <c r="B1072" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1072" s="3"/>
+      <c r="D1072" s="4"/>
+      <c r="E1072" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1072" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1072" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1072" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1073" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1073" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1073" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1073" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1073" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1073" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1073" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1073" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1073" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1074" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1074" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1074" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1074" s="3">
+        <v>34</v>
+      </c>
+      <c r="D1074" s="4"/>
+      <c r="E1074" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1074" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1074" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1074" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1075" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1075" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1075" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1075" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1075" s="3"/>
+      <c r="E1075" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1075" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1075" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1075" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1076" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1076" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1076" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1076" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1076" s="3"/>
+      <c r="E1076" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1076" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1076" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1076" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1077" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1077" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1077" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1077" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1077" s="4"/>
+      <c r="E1077" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1077" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1077" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1077" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1078" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1078" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1078" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1078" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1078" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1078" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1078" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1078" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1078" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1079" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1079" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1079" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1079" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1079" s="4"/>
+      <c r="E1079" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1079" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1079" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1079" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1080" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1080" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1080" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1080" s="3">
+        <v>14</v>
+      </c>
+      <c r="D1080" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1080" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1080" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1080" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1080" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1081" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1081" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1081" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1081" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1081" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1081" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1081" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1081" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1081" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1082" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1082" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1082" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1082" s="4"/>
+      <c r="D1082" s="4"/>
+      <c r="E1082" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1082" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1082" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1082" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1083" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1083" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1083" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1083" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1083" s="3"/>
+      <c r="E1083" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1083" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1083" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1083" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1084" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1084" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1084" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1084" s="3">
+        <v>13</v>
+      </c>
+      <c r="D1084" s="3"/>
+      <c r="E1084" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1084" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1084" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1084" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1085" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1085" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1085" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1085" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1085" s="4"/>
+      <c r="E1085" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1085" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1085" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1085" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1086" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1086" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1086" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1086" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1086" s="6"/>
+      <c r="E1086" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1086" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1086" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1086" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1087" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1087" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1087" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1087" s="3"/>
+      <c r="D1087" s="6"/>
+      <c r="E1087" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1087" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1087" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1087" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1088" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1088" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1088" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1088" s="3"/>
+      <c r="D1088" s="6"/>
+      <c r="E1088" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1088" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1088" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1088" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1089" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1089" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1089" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1089" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1089" s="6"/>
+      <c r="E1089" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1089" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1089" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1089" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1090" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1090" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1090" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1090" s="3"/>
+      <c r="D1090" s="6"/>
+      <c r="E1090" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1090" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1090" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1090" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1091" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1091" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1091" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1091" s="3"/>
+      <c r="D1091" s="6"/>
+      <c r="E1091" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1091" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1091" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1091" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1092" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1092" s="2">
+        <v>43978</v>
+      </c>
+      <c r="B1092" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1092" s="3"/>
+      <c r="D1092" s="4"/>
+      <c r="E1092" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1092" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1092" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1092" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1093" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1093" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1093" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1093" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1093" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1093" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1093" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1093" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1093" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1094" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1094" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1094" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1094" s="3">
+        <v>30</v>
+      </c>
+      <c r="D1094" s="4"/>
+      <c r="E1094" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1094" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1094" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1094" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1095" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1095" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1095" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1095" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1095" s="3"/>
+      <c r="E1095" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1095" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1095" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1095" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1096" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1096" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1096" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1096" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1096" s="3"/>
+      <c r="E1096" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1096" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1096" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1096" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1097" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1097" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1097" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1097" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1097" s="4"/>
+      <c r="E1097" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1097" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1097" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1097" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1098" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1098" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1098" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1098" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1098" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1098" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1098" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1098" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1098" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1099" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1099" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1099" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1099" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1099" s="4"/>
+      <c r="E1099" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1099" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1099" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1099" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1100" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1100" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1100" s="3">
+        <v>12</v>
+      </c>
+      <c r="D1100" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1100" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1100" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1100" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1100" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1101" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1101" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1101" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1101" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1101" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1101" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1101" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1101" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1102" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1102" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1102" s="4"/>
+      <c r="D1102" s="4"/>
+      <c r="E1102" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1102" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1102" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1102" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1103" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1103" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1103" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1103" s="3"/>
+      <c r="E1103" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1103" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1103" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1103" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1104" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1104" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1104" s="3">
+        <v>12</v>
+      </c>
+      <c r="D1104" s="3"/>
+      <c r="E1104" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1104" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1104" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1104" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1105" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1105" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1105" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1105" s="4"/>
+      <c r="E1105" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1105" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1105" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1105" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1106" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1106" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1106" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1106" s="6"/>
+      <c r="E1106" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1106" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1106" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1106" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1107" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1107" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1107" s="3"/>
+      <c r="D1107" s="6"/>
+      <c r="E1107" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1107" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1107" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1107" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1108" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1108" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1108" s="3"/>
+      <c r="D1108" s="6"/>
+      <c r="E1108" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1108" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1108" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1108" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1109" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1109" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1109" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1109" s="6"/>
+      <c r="E1109" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1109" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1109" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1109" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1110" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1110" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1110" s="3"/>
+      <c r="D1110" s="6"/>
+      <c r="E1110" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1110" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1110" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1110" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1111" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1111" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1111" s="3"/>
+      <c r="D1111" s="6"/>
+      <c r="E1111" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1111" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1111" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1111" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1112" s="2">
+        <v>43979</v>
+      </c>
+      <c r="B1112" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1112" s="3"/>
+      <c r="D1112" s="4"/>
+      <c r="E1112" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1112" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1112" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1112" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.05.28
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B48368A-F5A4-49A5-A8BF-BB588323DDA0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A518CA-17BF-45E0-B8F3-EB0C9E839218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10620" yWindow="3252" windowWidth="17280" windowHeight="6480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4464" yWindow="1596" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4452" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4532" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1112"/>
+  <dimension ref="A1:J1132"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -28032,6 +28032,480 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1113" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1113" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1113" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1113" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1113" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1113" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1113" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1113" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1114" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1114" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1114" s="3">
+        <v>30</v>
+      </c>
+      <c r="D1114" s="4"/>
+      <c r="E1114" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1114" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1114" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1114" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1115" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1115" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1115" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1115" s="3"/>
+      <c r="E1115" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1115" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1115" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1115" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1116" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1116" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1116" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1116" s="3"/>
+      <c r="E1116" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1116" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1116" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1116" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1117" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1117" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1117" s="3"/>
+      <c r="D1117" s="4"/>
+      <c r="E1117" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1117" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1117" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1117" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1118" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1118" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1118" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1118" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1118" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1118" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1118" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1118" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1119" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1119" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1119" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1119" s="4"/>
+      <c r="E1119" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1119" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1119" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1119" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1120" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1120" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1120" s="3">
+        <v>11</v>
+      </c>
+      <c r="D1120" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1120" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1120" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1120" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1120" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1121" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1121" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1121" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1121" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1121" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1121" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1121" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1121" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1122" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1122" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1122" s="4"/>
+      <c r="D1122" s="4"/>
+      <c r="E1122" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1122" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1122" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1122" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1123" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1123" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1123" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1123" s="3"/>
+      <c r="E1123" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1123" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1123" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1123" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1124" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1124" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1124" s="3">
+        <v>10</v>
+      </c>
+      <c r="D1124" s="3"/>
+      <c r="E1124" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1124" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1124" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1124" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1125" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1125" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1125" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1125" s="4"/>
+      <c r="E1125" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1125" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1125" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1125" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1126" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1126" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1126" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1126" s="6"/>
+      <c r="E1126" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1126" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1126" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1126" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1127" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1127" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1127" s="3"/>
+      <c r="D1127" s="6"/>
+      <c r="E1127" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1127" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1127" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1127" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1128" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1128" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1128" s="3"/>
+      <c r="D1128" s="6"/>
+      <c r="E1128" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1128" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1128" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1128" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1129" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1129" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1129" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1129" s="6"/>
+      <c r="E1129" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1129" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1129" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1129" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1130" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1130" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1130" s="3"/>
+      <c r="D1130" s="6"/>
+      <c r="E1130" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1130" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1130" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1130" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1131" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1131" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1131" s="3"/>
+      <c r="D1131" s="6"/>
+      <c r="E1131" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1131" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1131" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1131" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1132" s="2">
+        <v>43980</v>
+      </c>
+      <c r="B1132" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1132" s="3"/>
+      <c r="D1132" s="4"/>
+      <c r="E1132" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1132" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1132" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1132" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update data and charts Spain provinces 2020.05.29
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13A518CA-17BF-45E0-B8F3-EB0C9E839218}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C04BF-53EA-43D1-BD08-51FFA0CEA6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4464" yWindow="1596" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9852" yWindow="1956" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4532" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4612" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,9 +550,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1132"/>
+  <dimension ref="A1:J1152"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A1127" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1149" sqref="C1149"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28506,6 +28508,478 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1133" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1133" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1133" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1133" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1133" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1133" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1133" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1133" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1134" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1134" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1134" s="3">
+        <v>28</v>
+      </c>
+      <c r="D1134" s="4"/>
+      <c r="E1134" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1134" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1134" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1134" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1135" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1135" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1135" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1135" s="3"/>
+      <c r="E1135" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1135" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1135" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1135" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1136" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1136" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1136" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1136" s="3"/>
+      <c r="E1136" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1136" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1136" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1136" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1137" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1137" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1137" s="3"/>
+      <c r="D1137" s="4"/>
+      <c r="E1137" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1137" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1137" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1137" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1138" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1138" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1138" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1138" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1138" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1138" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1138" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1138" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1139" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1139" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1139" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1139" s="4"/>
+      <c r="E1139" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1139" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1139" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1139" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1140" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1140" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1140" s="3">
+        <v>10</v>
+      </c>
+      <c r="D1140" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1140" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1140" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1140" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1140" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1141" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1141" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1141" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1141" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1141" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1141" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1141" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1141" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1142" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1142" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1142" s="4"/>
+      <c r="D1142" s="4"/>
+      <c r="E1142" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1142" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1142" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1142" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1143" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1143" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1143" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1143" s="3"/>
+      <c r="E1143" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1143" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1143" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1143" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1144" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1144" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1144" s="3">
+        <v>10</v>
+      </c>
+      <c r="D1144" s="3"/>
+      <c r="E1144" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1144" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1144" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1144" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1145" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1145" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1145" s="3"/>
+      <c r="D1145" s="4"/>
+      <c r="E1145" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1145" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1145" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1145" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1146" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1146" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1146" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1146" s="6"/>
+      <c r="E1146" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1146" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1146" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1146" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1147" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1147" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1147" s="3"/>
+      <c r="D1147" s="6"/>
+      <c r="E1147" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1147" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1147" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1147" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1148" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1148" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1148" s="3"/>
+      <c r="D1148" s="6"/>
+      <c r="E1148" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1148" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1148" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1148" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1149" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1149" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1149" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1149" s="6"/>
+      <c r="E1149" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1149" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1149" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1149" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1150" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1150" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1150" s="3"/>
+      <c r="D1150" s="6"/>
+      <c r="E1150" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1150" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1150" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1150" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1151" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1151" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1151" s="3"/>
+      <c r="D1151" s="6"/>
+      <c r="E1151" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1151" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1151" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1151" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1152" s="2">
+        <v>43981</v>
+      </c>
+      <c r="B1152" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1152" s="3"/>
+      <c r="D1152" s="4"/>
+      <c r="E1152" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1152" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1152" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1152" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data and charts 2020.05.30. Add Ourense data. Remove unwanted process Madrid variables
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C16C04BF-53EA-43D1-BD08-51FFA0CEA6D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520048B1-435B-46AB-A28A-18FCDB115F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9852" yWindow="1956" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10392" yWindow="1692" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4612" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4692" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,11 +550,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1152"/>
+  <dimension ref="A1:J1172"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1127" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1149" sqref="C1149"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -28980,6 +28978,478 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1153" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1153" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1153" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1153" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1153" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1153" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1153" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1153" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1154" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1154" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1154" s="3">
+        <v>29</v>
+      </c>
+      <c r="D1154" s="4"/>
+      <c r="E1154" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1154" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1154" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1154" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1155" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1155" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1155" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1155" s="3"/>
+      <c r="E1155" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1155" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1155" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1155" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1156" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1156" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1156" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1156" s="3"/>
+      <c r="E1156" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1156" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1156" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1156" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1157" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1157" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1157" s="3"/>
+      <c r="D1157" s="4"/>
+      <c r="E1157" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1157" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1157" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1157" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1158" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1158" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1158" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1158" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1158" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1158" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1158" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1158" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1159" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1159" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1159" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1159" s="4"/>
+      <c r="E1159" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1159" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1159" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1159" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1160" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1160" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1160" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1160" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1160" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1160" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1160" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1160" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1161" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1161" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1161" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1161" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1161" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1161" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1161" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1161" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1162" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1162" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1162" s="4"/>
+      <c r="D1162" s="4"/>
+      <c r="E1162" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1162" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1162" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1162" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1163" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1163" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1163" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1163" s="3"/>
+      <c r="E1163" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1163" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1163" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1163" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1164" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1164" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1164" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1164" s="3"/>
+      <c r="E1164" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1164" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1164" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1164" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1165" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1165" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1165" s="3"/>
+      <c r="D1165" s="4"/>
+      <c r="E1165" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1165" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1165" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1165" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1166" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1166" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1166" s="3"/>
+      <c r="D1166" s="6"/>
+      <c r="E1166" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1166" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1166" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1166" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1167" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1167" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1167" s="3"/>
+      <c r="D1167" s="6"/>
+      <c r="E1167" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1167" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1167" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1167" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1168" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1168" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1168" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1168" s="6"/>
+      <c r="E1168" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1168" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1168" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1168" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1169" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1169" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1169" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1169" s="6"/>
+      <c r="E1169" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1169" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1169" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1169" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1170" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1170" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1170" s="3"/>
+      <c r="D1170" s="6"/>
+      <c r="E1170" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1170" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1170" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1170" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1171" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1171" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1171" s="3"/>
+      <c r="D1171" s="6"/>
+      <c r="E1171" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1171" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1171" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1171" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1172" s="2">
+        <v>43982</v>
+      </c>
+      <c r="B1172" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1172" s="3"/>
+      <c r="D1172" s="4"/>
+      <c r="E1172" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1172" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1172" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1172" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces charts and data 2020.05.31
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{520048B1-435B-46AB-A28A-18FCDB115F3E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88958254-38F2-4FA7-AC75-9BA3D542882E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10392" yWindow="1692" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9372" yWindow="2088" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4692" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4772" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1172"/>
+  <dimension ref="A1:J1192"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -29450,6 +29450,478 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1173" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1173" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1173" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1173" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1173" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1173" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1173" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1173" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1174" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1174" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1174" s="3">
+        <v>24</v>
+      </c>
+      <c r="D1174" s="4"/>
+      <c r="E1174" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1174" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1174" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1174" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1175" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1175" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1175" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1175" s="3"/>
+      <c r="E1175" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1175" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1175" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1175" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1176" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1176" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1176" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1176" s="3"/>
+      <c r="E1176" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1176" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1176" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1176" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1177" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1177" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1177" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1177" s="4"/>
+      <c r="E1177" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1177" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1177" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1177" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1178" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1178" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1178" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1178" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1178" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1178" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1178" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1178" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1179" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1179" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1179" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1179" s="4"/>
+      <c r="E1179" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1179" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1179" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1179" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1180" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1180" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1180" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1180" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1180" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1180" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1180" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1180" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1181" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1181" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1181" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1181" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1181" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1181" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1181" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1181" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1182" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1182" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1182" s="4"/>
+      <c r="D1182" s="4"/>
+      <c r="E1182" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1182" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1182" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1182" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1183" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1183" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1183" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1183" s="3"/>
+      <c r="E1183" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1183" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1183" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1183" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1184" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1184" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1184" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1184" s="3"/>
+      <c r="E1184" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1184" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1184" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1184" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1185" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1185" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1185" s="3"/>
+      <c r="D1185" s="4"/>
+      <c r="E1185" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1185" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1185" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1185" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1186" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1186" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1186" s="3"/>
+      <c r="D1186" s="6"/>
+      <c r="E1186" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1186" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1186" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1186" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1187" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1187" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1187" s="3"/>
+      <c r="D1187" s="6"/>
+      <c r="E1187" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1187" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1187" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1187" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1188" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1188" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1188" s="3"/>
+      <c r="D1188" s="6"/>
+      <c r="E1188" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1188" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1188" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1188" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1189" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1189" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1189" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1189" s="6"/>
+      <c r="E1189" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1189" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1189" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1189" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1190" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1190" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1190" s="3"/>
+      <c r="D1190" s="6"/>
+      <c r="E1190" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1190" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1190" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1190" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1191" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1191" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1191" s="3"/>
+      <c r="D1191" s="6"/>
+      <c r="E1191" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1191" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1191" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1191" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1192" s="2">
+        <v>43983</v>
+      </c>
+      <c r="B1192" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1192" s="3"/>
+      <c r="D1192" s="4"/>
+      <c r="E1192" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1192" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1192" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1192" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.01
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88958254-38F2-4FA7-AC75-9BA3D542882E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A79A4-C621-4B4A-8B14-17E6B5DA4C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9372" yWindow="2088" windowWidth="17280" windowHeight="9828" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5136" yWindow="3216" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4772" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4852" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1192"/>
+  <dimension ref="A1:J1212"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -29922,6 +29922,480 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1193" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1193" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1193" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1193" s="3">
+        <v>5</v>
+      </c>
+      <c r="E1193" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1193" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1193" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1193" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1194" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1194" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1194" s="3">
+        <v>22</v>
+      </c>
+      <c r="D1194" s="4"/>
+      <c r="E1194" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1194" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1194" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1194" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1195" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1195" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1195" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1195" s="3"/>
+      <c r="E1195" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1195" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1195" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1195" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1196" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1196" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1196" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1196" s="3"/>
+      <c r="E1196" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1196" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1196" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1196" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1197" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1197" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1197" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1197" s="4"/>
+      <c r="E1197" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1197" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1197" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1197" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1198" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1198" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1198" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1198" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1198" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1198" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1198" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1198" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1199" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1199" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1199" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1199" s="4"/>
+      <c r="E1199" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1199" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1199" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1199" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1200" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1200" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1200" s="3">
+        <v>10</v>
+      </c>
+      <c r="D1200" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1200" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1200" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1200" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1200" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1201" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1201" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1201" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1201" s="4">
+        <v>2</v>
+      </c>
+      <c r="E1201" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1201" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1201" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1201" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1202" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1202" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1202" s="4"/>
+      <c r="D1202" s="4"/>
+      <c r="E1202" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1202" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1202" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1202" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1203" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1203" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1203" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1203" s="3"/>
+      <c r="E1203" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1203" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1203" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1203" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1204" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1204" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1204" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1204" s="3"/>
+      <c r="E1204" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1204" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1204" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1204" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1205" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1205" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1205" s="3"/>
+      <c r="D1205" s="4"/>
+      <c r="E1205" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1205" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1205" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1205" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1206" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1206" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1206" s="3"/>
+      <c r="D1206" s="6"/>
+      <c r="E1206" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1206" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1206" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1206" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1207" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1207" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1207" s="3"/>
+      <c r="D1207" s="6"/>
+      <c r="E1207" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1207" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1207" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1207" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1208" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1208" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1208" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1208" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1208" s="6"/>
+      <c r="E1208" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1208" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1208" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1208" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1209" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1209" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1209" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1209" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1209" s="6"/>
+      <c r="E1209" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1209" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1209" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1209" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1210" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1210" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1210" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1210" s="3"/>
+      <c r="D1210" s="6"/>
+      <c r="E1210" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1210" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1210" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1210" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1211" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1211" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1211" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1211" s="3"/>
+      <c r="D1211" s="6"/>
+      <c r="E1211" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1211" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1211" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1211" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1212" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1212" s="2">
+        <v>43984</v>
+      </c>
+      <c r="B1212" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1212" s="3"/>
+      <c r="D1212" s="4"/>
+      <c r="E1212" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1212" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1212" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1212" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts and Euskadi hospitalized 2020.06.02
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD3A79A4-C621-4B4A-8B14-17E6B5DA4C35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7CB297-7077-41AB-9125-5C0B0D242B9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5136" yWindow="3216" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5892" yWindow="3252" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4852" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1212"/>
+  <dimension ref="A1:J1232"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -30396,6 +30396,478 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1213" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1213" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1213" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1213" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1213" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1213" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1213" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1213" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1213" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1214" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1214" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1214" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1214" s="3">
+        <v>31</v>
+      </c>
+      <c r="D1214" s="4"/>
+      <c r="E1214" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1214" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1214" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1214" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1215" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1215" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1215" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1215" s="3"/>
+      <c r="E1215" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1215" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1215" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1215" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1216" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1216" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1216" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1216" s="3"/>
+      <c r="E1216" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1216" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1216" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1216" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1217" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1217" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1217" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1217" s="4"/>
+      <c r="E1217" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1217" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1217" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1217" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1218" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1218" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1218" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1218" s="3"/>
+      <c r="E1218" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1218" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1218" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1218" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1219" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1219" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1219" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1219" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1219" s="4"/>
+      <c r="E1219" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1219" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1219" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1219" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1220" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1220" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1220" s="3">
+        <v>11</v>
+      </c>
+      <c r="D1220" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1220" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1220" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1220" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1220" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1221" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1221" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1221" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1221" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1221" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1221" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1221" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1221" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1221" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1222" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1222" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1222" s="4"/>
+      <c r="D1222" s="4"/>
+      <c r="E1222" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1222" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1222" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1222" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1223" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1223" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1223" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1223" s="3"/>
+      <c r="E1223" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1223" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1223" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1223" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1224" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1224" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1224" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1224" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1224" s="3"/>
+      <c r="E1224" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1224" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1224" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1224" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1225" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1225" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1225" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1225" s="3"/>
+      <c r="D1225" s="4"/>
+      <c r="E1225" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1225" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1225" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1225" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1226" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1226" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1226" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1226" s="3"/>
+      <c r="D1226" s="6"/>
+      <c r="E1226" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1226" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1226" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1226" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1227" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1227" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1227" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1227" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1227" s="6"/>
+      <c r="E1227" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1227" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1227" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1227" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1228" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1228" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1228" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1228" s="3"/>
+      <c r="D1228" s="6"/>
+      <c r="E1228" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1228" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1228" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1228" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1229" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1229" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1229" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1229" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1229" s="6"/>
+      <c r="E1229" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1229" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1229" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1229" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1230" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1230" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1230" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1230" s="3"/>
+      <c r="D1230" s="6"/>
+      <c r="E1230" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1230" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1230" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1230" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1231" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1231" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1231" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1231" s="3"/>
+      <c r="D1231" s="6"/>
+      <c r="E1231" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1231" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1231" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1231" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1232" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1232" s="2">
+        <v>43985</v>
+      </c>
+      <c r="B1232" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1232" s="3"/>
+      <c r="D1232" s="4"/>
+      <c r="E1232" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1232" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1232" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1232" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.02. Fix Uniprovinciales minus 1 day after May 21
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F7CB297-7077-41AB-9125-5C0B0D242B9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8D071-4D20-436F-90BA-40D77DD9375B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5892" yWindow="3252" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7884" yWindow="3216" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4932" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5012" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1232"/>
+  <dimension ref="A1:J1252"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -30868,6 +30868,482 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1233" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1233" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1233" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1233" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1233" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1233" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1233" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1233" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1233" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1234" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1234" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1234" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1234" s="3">
+        <v>27</v>
+      </c>
+      <c r="D1234" s="4"/>
+      <c r="E1234" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1234" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1234" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1234" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1235" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1235" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1235" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1235" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1235" s="3"/>
+      <c r="E1235" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1235" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1235" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1235" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1236" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1236" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1236" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1236" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1236" s="3"/>
+      <c r="E1236" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1236" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1236" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1236" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1237" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1237" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1237" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1237" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1237" s="4"/>
+      <c r="E1237" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1237" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1237" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1237" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1238" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1238" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1238" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1238" s="3"/>
+      <c r="E1238" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1238" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1238" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1238" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1239" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1239" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1239" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1239" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1239" s="4"/>
+      <c r="E1239" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1239" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1239" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1239" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1240" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1240" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1240" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1240" s="3">
+        <v>11</v>
+      </c>
+      <c r="D1240" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1240" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1240" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1240" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1240" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1241" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1241" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1241" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1241" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1241" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1241" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1241" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1241" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1241" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1242" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1242" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1242" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1242" s="4"/>
+      <c r="D1242" s="4"/>
+      <c r="E1242" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1242" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1242" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1242" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1243" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1243" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1243" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1243" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1243" s="3"/>
+      <c r="E1243" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1243" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1243" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1243" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1244" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1244" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1244" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1244" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1244" s="3"/>
+      <c r="E1244" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1244" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1244" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1244" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1245" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1245" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1245" s="3"/>
+      <c r="D1245" s="4"/>
+      <c r="E1245" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1245" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1245" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1245" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1246" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1246" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1246" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1246" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1246" s="6"/>
+      <c r="E1246" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1246" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1246" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1246" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1247" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1247" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1247" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1247" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1247" s="6"/>
+      <c r="E1247" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1247" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1247" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1247" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1248" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1248" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1248" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1248" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1248" s="6"/>
+      <c r="E1248" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1248" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1248" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1248" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1249" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1249" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1249" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1249" s="6"/>
+      <c r="E1249" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1249" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1249" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1249" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1250" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1250" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1250" s="3"/>
+      <c r="D1250" s="6"/>
+      <c r="E1250" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1250" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1250" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1250" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1251" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1251" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1251" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1251" s="3"/>
+      <c r="D1251" s="6"/>
+      <c r="E1251" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1251" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1251" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1251" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1252" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1252" s="2">
+        <v>43986</v>
+      </c>
+      <c r="B1252" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1252" s="3"/>
+      <c r="D1252" s="4"/>
+      <c r="E1252" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1252" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1252" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1252" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces and Euskadi hospitalized data and charts 2020.06.05
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4AD8D071-4D20-436F-90BA-40D77DD9375B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF21FC2D-ED5A-41F2-B783-AB81640226A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7884" yWindow="3216" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10236" yWindow="2124" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5012" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5092" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1252"/>
+  <dimension ref="A1:J1272"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -31344,6 +31344,476 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1253" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1253" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1253" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1253" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1253" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1253" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1253" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1253" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1253" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1254" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1254" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1254" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1254" s="3">
+        <v>29</v>
+      </c>
+      <c r="D1254" s="4"/>
+      <c r="E1254" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1254" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1254" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1254" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1255" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1255" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1255" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1255" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1255" s="3"/>
+      <c r="E1255" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1255" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1255" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1255" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1256" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1256" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1256" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1256" s="3"/>
+      <c r="E1256" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1256" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1256" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1256" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1257" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1257" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1257" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1257" s="4"/>
+      <c r="E1257" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1257" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1257" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1257" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1258" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1258" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1258" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1258" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1258" s="3"/>
+      <c r="E1258" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1258" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1258" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1258" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1259" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1259" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1259" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1259" s="4"/>
+      <c r="E1259" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1259" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1259" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1259" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1260" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1260" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1260" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1260" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1260" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1260" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1260" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1260" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1261" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1261" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1261" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1261" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1261" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1261" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1261" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1261" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1261" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1262" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1262" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1262" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1262" s="4"/>
+      <c r="D1262" s="4"/>
+      <c r="E1262" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1262" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1262" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1262" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1263" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1263" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1263" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1263" s="3"/>
+      <c r="E1263" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1263" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1263" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1263" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1264" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1264" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1264" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1264" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1264" s="3"/>
+      <c r="E1264" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1264" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1264" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1264" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1265" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1265" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1265" s="3"/>
+      <c r="D1265" s="4"/>
+      <c r="E1265" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1265" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1265" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1265" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1266" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1266" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1266" s="3"/>
+      <c r="D1266" s="6"/>
+      <c r="E1266" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1266" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1266" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1266" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1267" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1267" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1267" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1267" s="3"/>
+      <c r="D1267" s="6"/>
+      <c r="E1267" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1267" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1267" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1267" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1268" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1268" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1268" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1268" s="3"/>
+      <c r="D1268" s="6"/>
+      <c r="E1268" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1268" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1268" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1268" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1269" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1269" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1269" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1269" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1269" s="6"/>
+      <c r="E1269" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1269" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1269" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1269" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1270" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1270" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1270" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1270" s="3"/>
+      <c r="D1270" s="6"/>
+      <c r="E1270" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1270" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1270" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1270" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1271" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1271" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1271" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1271" s="3"/>
+      <c r="D1271" s="6"/>
+      <c r="E1271" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1271" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1271" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1271" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1272" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1272" s="2">
+        <v>43987</v>
+      </c>
+      <c r="B1272" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1272" s="3"/>
+      <c r="D1272" s="4"/>
+      <c r="E1272" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1272" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1272" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1272" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.05
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF21FC2D-ED5A-41F2-B783-AB81640226A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50CB45A-4BA8-4274-B441-74D6147D0822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10236" yWindow="2124" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2844" yWindow="5364" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5092" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1272"/>
+  <dimension ref="A1:J1292"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -31814,6 +31814,480 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1273" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1273" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1273" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1273" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1273" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1273" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1273" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1273" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1273" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1274" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1274" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1274" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1274" s="3">
+        <v>33</v>
+      </c>
+      <c r="D1274" s="4"/>
+      <c r="E1274" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1274" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1274" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1274" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1275" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1275" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1275" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1275" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1275" s="3"/>
+      <c r="E1275" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1275" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1275" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1275" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1276" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1276" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1276" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1276" s="3"/>
+      <c r="E1276" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1276" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1276" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1276" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1277" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1277" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1277" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1277" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1277" s="4"/>
+      <c r="E1277" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1277" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1277" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1277" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1278" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1278" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1278" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1278" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1278" s="3"/>
+      <c r="E1278" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1278" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1278" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1278" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1279" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1279" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1279" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1279" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1279" s="4"/>
+      <c r="E1279" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1279" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1279" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1279" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1280" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1280" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1280" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1280" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1280" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1280" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1280" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1280" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1281" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1281" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1281" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1281" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1281" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1281" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1281" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1281" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1281" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1282" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1282" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1282" s="4"/>
+      <c r="D1282" s="4"/>
+      <c r="E1282" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1282" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1282" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1282" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1283" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1283" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1283" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1283" s="3"/>
+      <c r="E1283" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1283" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1283" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1283" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1284" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1284" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1284" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1284" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1284" s="3"/>
+      <c r="E1284" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1284" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1284" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1284" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1285" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1285" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1285" s="3"/>
+      <c r="D1285" s="4"/>
+      <c r="E1285" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1285" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1285" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1285" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1286" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1286" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1286" s="3"/>
+      <c r="D1286" s="6"/>
+      <c r="E1286" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1286" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1286" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1286" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1287" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1287" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1287" s="3"/>
+      <c r="D1287" s="6"/>
+      <c r="E1287" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1287" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1287" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1287" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1288" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1288" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1288" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1288" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1288" s="6"/>
+      <c r="E1288" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1288" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1288" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1288" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1289" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1289" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1289" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1289" s="6"/>
+      <c r="E1289" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1289" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1289" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1289" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1290" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1290" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1290" s="3"/>
+      <c r="D1290" s="6"/>
+      <c r="E1290" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1290" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1290" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1290" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1291" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1291" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1291" s="3"/>
+      <c r="D1291" s="6"/>
+      <c r="E1291" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1291" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1291" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1291" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1292" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1292" s="2">
+        <v>43988</v>
+      </c>
+      <c r="B1292" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1292" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1292" s="4"/>
+      <c r="E1292" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1292" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1292" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1292" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain charts and provinces 2020.06.06
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C50CB45A-4BA8-4274-B441-74D6147D0822}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513762E4-1101-4B57-A14C-F400CC3F3849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2844" yWindow="5364" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9420" yWindow="3228" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1292"/>
+  <dimension ref="A1:J1312"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -32288,6 +32288,476 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1293" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1293" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1293" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1293" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1293" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1293" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1293" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1293" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1293" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1294" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1294" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1294" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1294" s="3">
+        <v>26</v>
+      </c>
+      <c r="D1294" s="4"/>
+      <c r="E1294" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1294" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1294" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1294" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1295" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1295" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1295" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1295" s="3"/>
+      <c r="E1295" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1295" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1295" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1295" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1296" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1296" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1296" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1296" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1296" s="3"/>
+      <c r="E1296" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1296" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1296" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1296" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1297" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1297" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1297" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1297" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1297" s="4"/>
+      <c r="E1297" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1297" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1297" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1297" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1298" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1298" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1298" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1298" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1298" s="3"/>
+      <c r="E1298" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1298" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1298" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1298" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1299" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1299" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1299" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1299" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1299" s="4"/>
+      <c r="E1299" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1299" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1299" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1299" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1300" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1300" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1300" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1300" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1300" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1300" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1300" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1300" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1300" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1301" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1301" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1301" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1301" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1301" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1301" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1301" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1301" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1302" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1302" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1302" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1302" s="4"/>
+      <c r="D1302" s="4"/>
+      <c r="E1302" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1302" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1302" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1302" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1303" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1303" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1303" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1303" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1303" s="3"/>
+      <c r="E1303" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1303" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1303" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1303" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1304" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1304" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1304" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1304" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1304" s="3"/>
+      <c r="E1304" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1304" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1304" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1304" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1305" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1305" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1305" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1305" s="3"/>
+      <c r="D1305" s="4"/>
+      <c r="E1305" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1305" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1305" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1305" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1306" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1306" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1306" s="3"/>
+      <c r="D1306" s="6"/>
+      <c r="E1306" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1306" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1306" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1306" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1307" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1307" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1307" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1307" s="3"/>
+      <c r="D1307" s="6"/>
+      <c r="E1307" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1307" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1307" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1307" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1308" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1308" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1308" s="3"/>
+      <c r="D1308" s="6"/>
+      <c r="E1308" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1308" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1308" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1308" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1309" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1309" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1309" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1309" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1309" s="6"/>
+      <c r="E1309" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1309" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1309" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1309" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1310" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1310" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1310" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1310" s="3"/>
+      <c r="D1310" s="6"/>
+      <c r="E1310" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1310" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1310" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1310" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1311" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1311" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1311" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1311" s="3"/>
+      <c r="D1311" s="6"/>
+      <c r="E1311" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1311" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1311" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1311" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1312" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1312" s="2">
+        <v>43989</v>
+      </c>
+      <c r="B1312" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1312" s="3"/>
+      <c r="D1312" s="4"/>
+      <c r="E1312" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1312" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1312" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1312" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.07. Complete C. Valenciana
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{513762E4-1101-4B57-A14C-F400CC3F3849}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B8A6F0-FFF0-4A72-A8E0-CF09058306A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="3228" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5472" yWindow="1308" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5252" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5332" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1312"/>
+  <dimension ref="A1:J1332"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -32758,6 +32758,480 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1313" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1313" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1313" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1313" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1313" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1313" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1313" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1313" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1313" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1314" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1314" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1314" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1314" s="3">
+        <v>28</v>
+      </c>
+      <c r="D1314" s="4"/>
+      <c r="E1314" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1314" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1314" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1314" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1315" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1315" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1315" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1315" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1315" s="3"/>
+      <c r="E1315" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1315" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1315" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1315" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1316" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1316" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1316" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1316" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1316" s="3"/>
+      <c r="E1316" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1316" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1316" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1316" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1317" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1317" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1317" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1317" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1317" s="4"/>
+      <c r="E1317" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1317" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1317" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1317" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1318" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1318" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1318" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1318" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1318" s="3"/>
+      <c r="E1318" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1318" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1318" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1318" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1319" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1319" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1319" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1319" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1319" s="4"/>
+      <c r="E1319" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1319" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1319" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1319" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1320" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1320" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1320" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1320" s="3">
+        <v>10</v>
+      </c>
+      <c r="D1320" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1320" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1320" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1320" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1320" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1321" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1321" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1321" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1321" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1321" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1321" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1321" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1321" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1321" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1322" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1322" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1322" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1322" s="4"/>
+      <c r="D1322" s="4"/>
+      <c r="E1322" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1322" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1322" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1322" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1323" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1323" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1323" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1323" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1323" s="3"/>
+      <c r="E1323" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1323" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1323" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1323" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1324" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1324" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1324" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1324" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1324" s="3"/>
+      <c r="E1324" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1324" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1324" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1324" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1325" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1325" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1325" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1325" s="3"/>
+      <c r="D1325" s="4"/>
+      <c r="E1325" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1325" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1325" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1325" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1326" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1326" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1326" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1326" s="3"/>
+      <c r="D1326" s="6"/>
+      <c r="E1326" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1326" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1326" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1326" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1327" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1327" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1327" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1327" s="3"/>
+      <c r="D1327" s="6"/>
+      <c r="E1327" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1327" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1327" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1327" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1328" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1328" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1328" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1328" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1328" s="6">
+        <v>1</v>
+      </c>
+      <c r="E1328" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1328" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1328" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1328" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1329" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1329" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1329" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1329" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1329" s="6"/>
+      <c r="E1329" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1329" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1329" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1329" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1330" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1330" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1330" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1330" s="3"/>
+      <c r="D1330" s="6"/>
+      <c r="E1330" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1330" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1330" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1330" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1331" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1331" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1331" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1331" s="3"/>
+      <c r="D1331" s="6"/>
+      <c r="E1331" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1331" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1331" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1331" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1332" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1332" s="2">
+        <v>43990</v>
+      </c>
+      <c r="B1332" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1332" s="3"/>
+      <c r="D1332" s="4"/>
+      <c r="E1332" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1332" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1332" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1332" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.08
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1B8A6F0-FFF0-4A72-A8E0-CF09058306A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39BE84E-4085-4A84-BAFD-F6CCB470160F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5472" yWindow="1308" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8388" yWindow="3804" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5332" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5412" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1332"/>
+  <dimension ref="A1:J1352"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -33232,6 +33232,474 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1333" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1333" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1333" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1333" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1333" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1333" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1333" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1333" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1333" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1334" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1334" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1334" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1334" s="3">
+        <v>31</v>
+      </c>
+      <c r="D1334" s="4"/>
+      <c r="E1334" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1334" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1334" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1334" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1335" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1335" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1335" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1335" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1335" s="3"/>
+      <c r="E1335" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1335" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1335" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1335" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1336" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1336" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1336" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1336" s="3"/>
+      <c r="D1336" s="3"/>
+      <c r="E1336" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1336" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1336" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1336" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1337" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1337" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1337" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1337" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1337" s="4"/>
+      <c r="E1337" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1337" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1337" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1337" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1338" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1338" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1338" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1338" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1338" s="3"/>
+      <c r="E1338" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1338" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1338" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1338" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1339" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1339" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1339" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1339" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1339" s="4"/>
+      <c r="E1339" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1339" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1339" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1339" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1340" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1340" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1340" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1340" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1340" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1340" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1340" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1340" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1340" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1341" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1341" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1341" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1341" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1341" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1341" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1341" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1341" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1341" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1342" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1342" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1342" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1342" s="4"/>
+      <c r="D1342" s="4"/>
+      <c r="E1342" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1342" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1342" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1342" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1343" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1343" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1343" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1343" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1343" s="3"/>
+      <c r="E1343" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1343" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1343" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1343" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1344" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1344" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1344" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1344" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1344" s="3"/>
+      <c r="E1344" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1344" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1344" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1344" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1345" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1345" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1345" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1345" s="3"/>
+      <c r="D1345" s="4"/>
+      <c r="E1345" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1345" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1345" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1345" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1346" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1346" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1346" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1346" s="3"/>
+      <c r="D1346" s="6"/>
+      <c r="E1346" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1346" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1346" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1346" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1347" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1347" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1347" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1347" s="3"/>
+      <c r="D1347" s="6"/>
+      <c r="E1347" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1347" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1347" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1347" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1348" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1348" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1348" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1348" s="3"/>
+      <c r="D1348" s="6"/>
+      <c r="E1348" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1348" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1348" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1348" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1349" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1349" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1349" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1349" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1349" s="6"/>
+      <c r="E1349" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1349" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1349" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1349" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1350" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1350" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1350" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1350" s="3"/>
+      <c r="D1350" s="6"/>
+      <c r="E1350" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1350" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1350" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1350" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1351" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1351" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1351" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1351" s="3"/>
+      <c r="D1351" s="6"/>
+      <c r="E1351" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1351" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1351" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1351" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1352" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1352" s="2">
+        <v>43991</v>
+      </c>
+      <c r="B1352" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1352" s="3"/>
+      <c r="D1352" s="4"/>
+      <c r="E1352" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1352" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1352" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1352" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.09
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F39BE84E-4085-4A84-BAFD-F6CCB470160F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA41036F-5699-4C52-93E5-4A9C8BE0C754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8388" yWindow="3804" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7512" yWindow="4440" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5412" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1352"/>
+  <dimension ref="A1:J1372"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -33700,6 +33700,470 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1353" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1353" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1353" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1353" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1353" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1353" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1353" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1353" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1353" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1354" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1354" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1354" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1354" s="3">
+        <v>29</v>
+      </c>
+      <c r="D1354" s="4"/>
+      <c r="E1354" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1354" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1354" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1354" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1355" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1355" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1355" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1355" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1355" s="3"/>
+      <c r="E1355" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1355" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1355" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1355" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1356" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1356" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1356" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1356" s="3"/>
+      <c r="D1356" s="3"/>
+      <c r="E1356" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1356" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1356" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1356" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1357" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1357" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1357" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1357" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1357" s="4"/>
+      <c r="E1357" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1357" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1357" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1357" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1358" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1358" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1358" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1358" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1358" s="3"/>
+      <c r="E1358" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1358" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1358" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1358" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1359" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1359" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1359" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1359" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1359" s="4"/>
+      <c r="E1359" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1359" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1359" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1359" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1360" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1360" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1360" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1360" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1360" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1360" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1360" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1360" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1360" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1361" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1361" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1361" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1361" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1361" s="4"/>
+      <c r="E1361" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1361" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1361" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1361" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1362" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1362" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1362" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1362" s="4"/>
+      <c r="D1362" s="4"/>
+      <c r="E1362" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1362" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1362" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1362" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1363" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1363" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1363" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1363" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1363" s="3"/>
+      <c r="E1363" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1363" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1363" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1363" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1364" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1364" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1364" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1364" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1364" s="3"/>
+      <c r="E1364" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1364" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1364" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1364" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1365" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1365" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1365" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1365" s="3"/>
+      <c r="D1365" s="4"/>
+      <c r="E1365" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1365" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1365" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1365" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1366" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1366" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1366" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1366" s="3"/>
+      <c r="D1366" s="6"/>
+      <c r="E1366" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1366" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1366" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1366" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1367" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1367" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1367" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1367" s="3"/>
+      <c r="D1367" s="6"/>
+      <c r="E1367" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1367" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1367" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1367" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1368" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1368" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1368" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1368" s="3"/>
+      <c r="D1368" s="6"/>
+      <c r="E1368" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1368" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1368" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1368" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1369" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1369" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1369" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1369" s="3"/>
+      <c r="D1369" s="6"/>
+      <c r="E1369" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1369" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1369" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1369" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1370" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1370" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1370" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1370" s="3"/>
+      <c r="D1370" s="6"/>
+      <c r="E1370" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1370" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1370" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1370" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1371" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1371" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1371" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1371" s="3"/>
+      <c r="D1371" s="6"/>
+      <c r="E1371" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1371" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1371" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1371" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1372" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1372" s="2">
+        <v>43992</v>
+      </c>
+      <c r="B1372" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1372" s="3"/>
+      <c r="D1372" s="4"/>
+      <c r="E1372" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1372" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1372" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1372" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data and charts and Euskadi hospitalized 2020.06.10
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA41036F-5699-4C52-93E5-4A9C8BE0C754}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB72881-7909-42BF-BDCB-F86D41CB84CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7512" yWindow="4440" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9264" yWindow="5652" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5492" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5572" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1372"/>
+  <dimension ref="A1:J1392"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -34164,6 +34164,470 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1373" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1373" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1373" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1373" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1373" s="3">
+        <v>4</v>
+      </c>
+      <c r="E1373" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1373" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1373" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1373" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1374" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1374" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1374" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1374" s="3">
+        <v>24</v>
+      </c>
+      <c r="D1374" s="4"/>
+      <c r="E1374" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1374" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1374" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1374" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1375" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1375" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1375" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1375" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1375" s="3"/>
+      <c r="E1375" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1375" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1375" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1375" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1376" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1376" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1376" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1376" s="3"/>
+      <c r="D1376" s="3"/>
+      <c r="E1376" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1376" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1376" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1376" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1377" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1377" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1377" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1377" s="3"/>
+      <c r="D1377" s="4"/>
+      <c r="E1377" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1377" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1377" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1377" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1378" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1378" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1378" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1378" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1378" s="3"/>
+      <c r="E1378" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1378" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1378" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1378" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1379" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1379" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1379" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1379" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1379" s="4"/>
+      <c r="E1379" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1379" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1379" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1379" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1380" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1380" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1380" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1380" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1380" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1380" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1380" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1380" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1380" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1381" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1381" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1381" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1381" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1381" s="4"/>
+      <c r="E1381" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1381" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1381" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1381" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1382" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1382" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1382" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1382" s="4"/>
+      <c r="D1382" s="4"/>
+      <c r="E1382" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1382" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1382" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1382" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1383" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1383" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1383" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1383" s="3"/>
+      <c r="E1383" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1383" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1383" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1383" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1384" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1384" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1384" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1384" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1384" s="3"/>
+      <c r="E1384" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1384" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1384" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1384" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1385" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1385" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1385" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1385" s="3"/>
+      <c r="D1385" s="4"/>
+      <c r="E1385" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1385" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1385" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1385" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1386" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1386" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1386" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1386" s="3"/>
+      <c r="D1386" s="6"/>
+      <c r="E1386" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1386" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1386" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1386" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1387" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1387" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1387" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1387" s="3"/>
+      <c r="D1387" s="6"/>
+      <c r="E1387" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1387" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1387" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1387" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1388" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1388" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1388" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1388" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1388" s="6"/>
+      <c r="E1388" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1388" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1388" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1388" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1389" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1389" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1389" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1389" s="3"/>
+      <c r="D1389" s="6"/>
+      <c r="E1389" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1389" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1389" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1389" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1390" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1390" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1390" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1390" s="3"/>
+      <c r="D1390" s="6"/>
+      <c r="E1390" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1390" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1390" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1390" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1391" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1391" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1391" s="3"/>
+      <c r="D1391" s="6"/>
+      <c r="E1391" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1391" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1391" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1391" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1392" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1392" s="2">
+        <v>43993</v>
+      </c>
+      <c r="B1392" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1392" s="3"/>
+      <c r="D1392" s="4"/>
+      <c r="E1392" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1392" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1392" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1392" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.11
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FB72881-7909-42BF-BDCB-F86D41CB84CA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277AAD0D-9382-410A-BB97-8F42ED370B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9264" yWindow="5652" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10668" yWindow="2580" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5572" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5652" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1392"/>
+  <dimension ref="A1:J1412"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -34628,6 +34628,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1393" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1393" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1393" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1393" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1393" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1393" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1393" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1393" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1393" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1394" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1394" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1394" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1394" s="3">
+        <v>22</v>
+      </c>
+      <c r="D1394" s="4"/>
+      <c r="E1394" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1394" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1394" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1394" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1395" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1395" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1395" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1395" s="3"/>
+      <c r="E1395" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1395" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1395" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1395" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1396" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1396" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1396" s="3"/>
+      <c r="D1396" s="3"/>
+      <c r="E1396" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1396" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1396" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1396" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1397" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1397" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1397" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1397" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1397" s="4"/>
+      <c r="E1397" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1397" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1397" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1397" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1398" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1398" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1398" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1398" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1398" s="3"/>
+      <c r="E1398" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1398" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1398" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1398" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1399" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1399" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1399" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1399" s="3"/>
+      <c r="D1399" s="4"/>
+      <c r="E1399" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1399" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1399" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1399" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1400" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1400" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1400" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1400" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1400" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1400" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1400" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1400" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1400" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1401" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1401" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1401" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1401" s="4"/>
+      <c r="E1401" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1401" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1401" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1401" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1402" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1402" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1402" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1402" s="4"/>
+      <c r="D1402" s="4"/>
+      <c r="E1402" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1402" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1402" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1402" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1403" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1403" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1403" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1403" s="3"/>
+      <c r="D1403" s="3"/>
+      <c r="E1403" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1403" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1403" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1403" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1404" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1404" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1404" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1404" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1404" s="3"/>
+      <c r="E1404" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1404" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1404" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1404" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1405" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1405" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1405" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1405" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1405" s="4"/>
+      <c r="E1405" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1405" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1405" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1405" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1406" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1406" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1406" s="3"/>
+      <c r="D1406" s="6"/>
+      <c r="E1406" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1406" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1406" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1406" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1407" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1407" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1407" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1407" s="3"/>
+      <c r="D1407" s="6"/>
+      <c r="E1407" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1407" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1407" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1407" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1408" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1408" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1408" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1408" s="3"/>
+      <c r="D1408" s="6"/>
+      <c r="E1408" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1408" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1408" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1408" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1409" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1409" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1409" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1409" s="3"/>
+      <c r="D1409" s="6"/>
+      <c r="E1409" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1409" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1409" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1409" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1410" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1410" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1410" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1410" s="3"/>
+      <c r="D1410" s="6"/>
+      <c r="E1410" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1410" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1410" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1410" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1411" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1411" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1411" s="3"/>
+      <c r="D1411" s="6"/>
+      <c r="E1411" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1411" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1411" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1411" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1412" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1412" s="2">
+        <v>43994</v>
+      </c>
+      <c r="B1412" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1412" s="3"/>
+      <c r="D1412" s="4"/>
+      <c r="E1412" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1412" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1412" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1412" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.12
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{277AAD0D-9382-410A-BB97-8F42ED370B9B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C1FA2F-F119-4145-AA02-FBC7C4838C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10668" yWindow="2580" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9780" yWindow="4920" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5652" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5732" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1412"/>
+  <dimension ref="A1:J1432"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -35090,6 +35090,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1413" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1413" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1413" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1413" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1413" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1413" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1413" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1413" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1413" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1414" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1414" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1414" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1414" s="3">
+        <v>20</v>
+      </c>
+      <c r="D1414" s="4"/>
+      <c r="E1414" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1414" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1414" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1414" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1415" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1415" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1415" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1415" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1415" s="3"/>
+      <c r="E1415" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1415" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1415" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1415" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1416" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1416" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1416" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1416" s="3"/>
+      <c r="D1416" s="3"/>
+      <c r="E1416" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1416" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1416" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1416" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1417" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1417" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1417" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1417" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1417" s="4"/>
+      <c r="E1417" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1417" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1417" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1417" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1418" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1418" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1418" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1418" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1418" s="3"/>
+      <c r="E1418" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1418" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1418" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1418" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1419" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1419" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1419" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1419" s="3"/>
+      <c r="D1419" s="4"/>
+      <c r="E1419" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1419" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1419" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1419" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1420" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1420" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1420" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1420" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1420" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1420" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1420" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1420" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1420" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1421" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1421" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1421" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1421" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1421" s="4"/>
+      <c r="E1421" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1421" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1421" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1421" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1422" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1422" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1422" s="4"/>
+      <c r="D1422" s="4"/>
+      <c r="E1422" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1422" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1422" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1422" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1423" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1423" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1423" s="3"/>
+      <c r="D1423" s="3"/>
+      <c r="E1423" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1423" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1423" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1423" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1424" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1424" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1424" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1424" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1424" s="3"/>
+      <c r="E1424" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1424" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1424" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1424" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1425" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1425" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1425" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1425" s="3"/>
+      <c r="D1425" s="4"/>
+      <c r="E1425" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1425" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1425" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1425" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1426" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1426" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1426" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1426" s="3"/>
+      <c r="D1426" s="6"/>
+      <c r="E1426" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1426" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1426" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1426" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1427" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1427" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1427" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1427" s="3"/>
+      <c r="D1427" s="6"/>
+      <c r="E1427" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1427" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1427" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1427" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1428" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1428" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1428" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1428" s="3"/>
+      <c r="D1428" s="6"/>
+      <c r="E1428" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1428" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1428" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1428" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1429" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1429" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1429" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1429" s="3"/>
+      <c r="D1429" s="6"/>
+      <c r="E1429" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1429" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1429" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1429" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1430" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1430" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1430" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1430" s="3"/>
+      <c r="D1430" s="6"/>
+      <c r="E1430" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1430" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1430" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1430" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1431" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1431" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1431" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1431" s="3"/>
+      <c r="D1431" s="6"/>
+      <c r="E1431" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1431" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1431" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1431" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1432" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1432" s="2">
+        <v>43995</v>
+      </c>
+      <c r="B1432" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1432" s="3"/>
+      <c r="D1432" s="4"/>
+      <c r="E1432" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1432" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1432" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1432" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.13
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C1FA2F-F119-4145-AA02-FBC7C4838C67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEF5759-79BA-427E-B29D-47254BD56798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9780" yWindow="4920" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10200" yWindow="3816" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5732" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5812" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1432"/>
+  <dimension ref="A1:J1452"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -35550,6 +35550,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1433" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1433" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1433" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1433" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1433" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1433" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1433" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1433" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1433" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1434" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1434" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1434" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1434" s="3">
+        <v>18</v>
+      </c>
+      <c r="D1434" s="4"/>
+      <c r="E1434" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1434" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1434" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1434" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1435" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1435" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1435" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1435" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1435" s="3"/>
+      <c r="E1435" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1435" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1435" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1435" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1436" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1436" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1436" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1436" s="3"/>
+      <c r="D1436" s="3"/>
+      <c r="E1436" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1436" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1436" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1436" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1437" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1437" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1437" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1437" s="3"/>
+      <c r="D1437" s="4"/>
+      <c r="E1437" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1437" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1437" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1437" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1438" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1438" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1438" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1438" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1438" s="3"/>
+      <c r="E1438" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1438" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1438" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1438" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1439" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1439" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1439" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1439" s="3"/>
+      <c r="D1439" s="4"/>
+      <c r="E1439" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1439" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1439" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1439" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1440" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1440" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1440" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1440" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1440" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1440" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1440" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1440" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1440" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1441" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1441" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1441" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1441" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1441" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1441" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1441" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1441" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1441" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1442" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1442" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1442" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1442" s="4"/>
+      <c r="D1442" s="4"/>
+      <c r="E1442" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1442" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1442" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1442" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1443" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1443" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1443" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1443" s="3"/>
+      <c r="D1443" s="3"/>
+      <c r="E1443" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1443" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1443" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1443" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1444" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1444" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1444" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1444" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1444" s="3"/>
+      <c r="E1444" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1444" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1444" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1444" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1445" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1445" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1445" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1445" s="3"/>
+      <c r="D1445" s="4"/>
+      <c r="E1445" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1445" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1445" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1445" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1446" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1446" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1446" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1446" s="3"/>
+      <c r="D1446" s="6"/>
+      <c r="E1446" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1446" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1446" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1446" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1447" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1447" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1447" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1447" s="3"/>
+      <c r="D1447" s="6"/>
+      <c r="E1447" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1447" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1447" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1447" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1448" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1448" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1448" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1448" s="3"/>
+      <c r="D1448" s="6"/>
+      <c r="E1448" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1448" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1448" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1448" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1449" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1449" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1449" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1449" s="3"/>
+      <c r="D1449" s="6"/>
+      <c r="E1449" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1449" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1449" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1449" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1450" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1450" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1450" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1450" s="3"/>
+      <c r="D1450" s="6"/>
+      <c r="E1450" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1450" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1450" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1450" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1451" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1451" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1451" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1451" s="3"/>
+      <c r="D1451" s="6"/>
+      <c r="E1451" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1451" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1451" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1451" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1452" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1452" s="2">
+        <v>43996</v>
+      </c>
+      <c r="B1452" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1452" s="3"/>
+      <c r="D1452" s="4"/>
+      <c r="E1452" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1452" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1452" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1452" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.04.14 and EUS hospitalized data
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACEF5759-79BA-427E-B29D-47254BD56798}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44625230-78AE-4A58-B4E6-6CE14278E471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10200" yWindow="3816" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5812" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5892" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1452"/>
+  <dimension ref="A1:J1472"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -36010,6 +36010,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1453" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1453" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1453" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1453" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1453" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1453" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1453" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1453" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1453" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1454" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1454" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1454" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1454" s="3">
+        <v>18</v>
+      </c>
+      <c r="D1454" s="4"/>
+      <c r="E1454" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1454" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1454" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1454" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1455" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1455" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1455" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1455" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1455" s="3"/>
+      <c r="E1455" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1455" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1455" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1455" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1456" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1456" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1456" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1456" s="3"/>
+      <c r="D1456" s="3"/>
+      <c r="E1456" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1456" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1456" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1456" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1457" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1457" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1457" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1457" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1457" s="4"/>
+      <c r="E1457" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1457" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1457" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1457" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1458" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1458" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1458" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1458" s="3"/>
+      <c r="D1458" s="3"/>
+      <c r="E1458" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1458" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1458" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1458" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1459" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1459" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1459" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1459" s="3"/>
+      <c r="D1459" s="4"/>
+      <c r="E1459" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1459" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1459" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1459" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1460" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1460" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1460" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1460" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1460" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1460" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1460" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1460" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1460" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1461" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1461" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1461" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1461" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1461" s="4"/>
+      <c r="E1461" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1461" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1461" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1461" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1462" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1462" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1462" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1462" s="4"/>
+      <c r="D1462" s="4"/>
+      <c r="E1462" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1462" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1462" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1462" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1463" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1463" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1463" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1463" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1463" s="3"/>
+      <c r="E1463" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1463" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1463" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1463" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1464" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1464" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1464" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1464" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1464" s="3"/>
+      <c r="E1464" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1464" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1464" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1464" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1465" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1465" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1465" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1465" s="3"/>
+      <c r="D1465" s="4"/>
+      <c r="E1465" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1465" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1465" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1465" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1466" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1466" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1466" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1466" s="3"/>
+      <c r="D1466" s="6"/>
+      <c r="E1466" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1466" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1466" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1466" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1467" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1467" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1467" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1467" s="3"/>
+      <c r="D1467" s="6"/>
+      <c r="E1467" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1467" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1467" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1467" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1468" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1468" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1468" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1468" s="3"/>
+      <c r="D1468" s="6"/>
+      <c r="E1468" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1468" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1468" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1468" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1469" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1469" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1469" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1469" s="3"/>
+      <c r="D1469" s="6"/>
+      <c r="E1469" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1469" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1469" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1469" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1470" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1470" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1470" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1470" s="3"/>
+      <c r="D1470" s="6"/>
+      <c r="E1470" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1470" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1470" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1470" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1471" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1471" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1471" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1471" s="3"/>
+      <c r="D1471" s="6"/>
+      <c r="E1471" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1471" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1471" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1471" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1472" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1472" s="2">
+        <v>43997</v>
+      </c>
+      <c r="B1472" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1472" s="3"/>
+      <c r="D1472" s="4"/>
+      <c r="E1472" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1472" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1472" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1472" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data (add RENAVE ISCIII data)  and charts 2020.06.15
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44625230-78AE-4A58-B4E6-6CE14278E471}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C6125-CF39-4A1E-9AD9-8267FF669C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7992" yWindow="3096" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5892" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5972" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1472"/>
+  <dimension ref="A1:J1492"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -36470,6 +36470,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1473" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1473" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1473" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1473" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1473" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1473" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1473" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1473" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1473" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1474" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1474" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1474" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1474" s="3">
+        <v>22</v>
+      </c>
+      <c r="D1474" s="4"/>
+      <c r="E1474" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1474" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1474" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1474" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1475" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1475" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1475" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1475" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1475" s="3"/>
+      <c r="E1475" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1475" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1475" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1475" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1476" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1476" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1476" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1476" s="3"/>
+      <c r="D1476" s="3"/>
+      <c r="E1476" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1476" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1476" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1476" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1477" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1477" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1477" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1477" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1477" s="4"/>
+      <c r="E1477" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1477" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1477" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1477" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1478" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1478" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1478" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1478" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1478" s="3"/>
+      <c r="E1478" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1478" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1478" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1478" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1479" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1479" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1479" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1479" s="3"/>
+      <c r="D1479" s="4"/>
+      <c r="E1479" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1479" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1479" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1479" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1480" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1480" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1480" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1480" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1480" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1480" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1480" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1480" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1480" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1481" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1481" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1481" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1481" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1481" s="4"/>
+      <c r="E1481" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1481" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1481" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1481" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1482" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1482" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1482" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1482" s="4"/>
+      <c r="D1482" s="4"/>
+      <c r="E1482" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1482" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1482" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1482" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1483" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1483" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1483" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1483" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1483" s="3"/>
+      <c r="E1483" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1483" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1483" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1483" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1484" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1484" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1484" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1484" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1484" s="3"/>
+      <c r="E1484" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1484" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1484" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1484" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1485" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1485" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1485" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1485" s="3"/>
+      <c r="D1485" s="4"/>
+      <c r="E1485" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1485" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1485" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1485" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1486" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1486" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1486" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1486" s="3"/>
+      <c r="D1486" s="6"/>
+      <c r="E1486" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1486" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1486" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1486" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1487" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1487" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1487" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1487" s="3"/>
+      <c r="D1487" s="6"/>
+      <c r="E1487" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1487" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1487" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1487" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1488" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1488" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1488" s="3"/>
+      <c r="D1488" s="6"/>
+      <c r="E1488" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1488" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1488" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1488" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1489" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1489" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1489" s="3"/>
+      <c r="D1489" s="6"/>
+      <c r="E1489" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1489" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1489" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1489" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1490" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1490" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1490" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1490" s="3"/>
+      <c r="D1490" s="6"/>
+      <c r="E1490" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1490" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1490" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1490" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1491" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1491" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1491" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1491" s="3"/>
+      <c r="D1491" s="6"/>
+      <c r="E1491" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1491" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1491" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1491" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1492" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1492" s="2">
+        <v>43998</v>
+      </c>
+      <c r="B1492" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1492" s="3"/>
+      <c r="D1492" s="4"/>
+      <c r="E1492" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1492" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1492" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1492" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.16
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{712C6125-CF39-4A1E-9AD9-8267FF669C5B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F755FC96-DFAE-4952-BB55-4651F163ACC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7992" yWindow="3096" windowWidth="17280" windowHeight="6612" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8508" yWindow="4140" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5972" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6052" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1492"/>
+  <dimension ref="A1:J1512"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -36932,6 +36932,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1493" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1493" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1493" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1493" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1493" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1493" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1493" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1493" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1493" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1494" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1494" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1494" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1494" s="3">
+        <v>23</v>
+      </c>
+      <c r="D1494" s="4"/>
+      <c r="E1494" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1494" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1494" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1494" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1495" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1495" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1495" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1495" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1495" s="3"/>
+      <c r="E1495" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1495" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1495" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1495" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1496" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1496" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1496" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1496" s="3"/>
+      <c r="D1496" s="3"/>
+      <c r="E1496" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1496" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1496" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1496" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1497" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1497" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1497" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1497" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1497" s="4"/>
+      <c r="E1497" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1497" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1497" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1497" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1498" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1498" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1498" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1498" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1498" s="3"/>
+      <c r="E1498" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1498" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1498" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1498" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1499" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1499" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1499" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1499" s="3"/>
+      <c r="D1499" s="4"/>
+      <c r="E1499" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1499" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1499" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1499" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1500" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1500" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1500" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1500" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1500" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1500" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1500" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1500" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1500" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1501" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1501" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1501" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1501" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1501" s="4"/>
+      <c r="E1501" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1501" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1501" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1501" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1502" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1502" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1502" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1502" s="4"/>
+      <c r="D1502" s="4"/>
+      <c r="E1502" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1502" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1502" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1502" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1503" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1503" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1503" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1503" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1503" s="3"/>
+      <c r="E1503" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1503" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1503" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1503" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1504" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1504" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1504" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1504" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1504" s="3"/>
+      <c r="E1504" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1504" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1504" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1504" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1505" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1505" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1505" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1505" s="3"/>
+      <c r="D1505" s="4"/>
+      <c r="E1505" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1505" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1505" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1505" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1506" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1506" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1506" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1506" s="3"/>
+      <c r="D1506" s="6"/>
+      <c r="E1506" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1506" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1506" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1506" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1507" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1507" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1507" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1507" s="3"/>
+      <c r="D1507" s="6"/>
+      <c r="E1507" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1507" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1507" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1507" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1508" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1508" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1508" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1508" s="3"/>
+      <c r="D1508" s="6"/>
+      <c r="E1508" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1508" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1508" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1508" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1509" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1509" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1509" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1509" s="3"/>
+      <c r="D1509" s="6"/>
+      <c r="E1509" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1509" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1509" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1509" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1510" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1510" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1510" s="3"/>
+      <c r="D1510" s="6"/>
+      <c r="E1510" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1510" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1510" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1510" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1511" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1511" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1511" s="3"/>
+      <c r="D1511" s="6"/>
+      <c r="E1511" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1511" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1511" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1511" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1512" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1512" s="2">
+        <v>43999</v>
+      </c>
+      <c r="B1512" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1512" s="3"/>
+      <c r="D1512" s="4"/>
+      <c r="E1512" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1512" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1512" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1512" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain province data 2020-06-17
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F755FC96-DFAE-4952-BB55-4651F163ACC4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC90BEF4-8F1B-4EC3-B8C2-243DC5027B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8508" yWindow="4140" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9876" yWindow="2868" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6052" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6132" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1512"/>
+  <dimension ref="A1:J1532"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -37394,6 +37394,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1513" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1513" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1513" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1513" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1513" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1513" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1513" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1513" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1513" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1514" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1514" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1514" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1514" s="3">
+        <v>25</v>
+      </c>
+      <c r="D1514" s="4"/>
+      <c r="E1514" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1514" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1514" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1514" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1515" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1515" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1515" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1515" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1515" s="3"/>
+      <c r="E1515" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1515" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1515" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1515" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1516" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1516" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1516" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1516" s="3"/>
+      <c r="D1516" s="3"/>
+      <c r="E1516" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1516" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1516" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1516" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1517" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1517" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1517" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1517" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1517" s="4"/>
+      <c r="E1517" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1517" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1517" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1517" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1518" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1518" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1518" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1518" s="3"/>
+      <c r="E1518" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1518" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1518" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1518" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1519" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1519" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1519" s="3"/>
+      <c r="D1519" s="4"/>
+      <c r="E1519" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1519" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1519" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1519" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1520" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1520" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1520" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1520" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1520" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1520" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1520" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1520" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1520" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1521" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1521" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1521" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1521" s="3"/>
+      <c r="D1521" s="4"/>
+      <c r="E1521" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1521" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1521" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1521" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1522" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1522" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1522" s="4"/>
+      <c r="D1522" s="4"/>
+      <c r="E1522" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1522" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1522" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1522" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1523" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1523" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1523" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1523" s="3"/>
+      <c r="E1523" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1523" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1523" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1523" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1524" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1524" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1524" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1524" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1524" s="3"/>
+      <c r="E1524" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1524" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1524" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1524" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1525" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1525" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1525" s="3"/>
+      <c r="D1525" s="4"/>
+      <c r="E1525" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1525" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1525" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1525" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1526" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1526" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1526" s="3"/>
+      <c r="D1526" s="6"/>
+      <c r="E1526" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1526" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1526" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1526" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1527" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1527" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1527" s="3"/>
+      <c r="D1527" s="6"/>
+      <c r="E1527" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1527" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1527" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1527" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1528" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1528" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1528" s="3"/>
+      <c r="D1528" s="6"/>
+      <c r="E1528" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1528" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1528" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1528" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1529" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1529" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1529" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1529" s="3"/>
+      <c r="D1529" s="6"/>
+      <c r="E1529" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1529" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1529" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1529" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1530" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1530" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1530" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1530" s="3"/>
+      <c r="D1530" s="6"/>
+      <c r="E1530" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1530" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1530" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1530" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1531" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1531" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1531" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1531" s="3"/>
+      <c r="D1531" s="6"/>
+      <c r="E1531" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1531" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1531" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1531" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1532" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1532" s="2">
+        <v>44000</v>
+      </c>
+      <c r="B1532" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1532" s="3"/>
+      <c r="D1532" s="4"/>
+      <c r="E1532" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1532" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1532" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1532" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain province data 2002.06.18
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC90BEF4-8F1B-4EC3-B8C2-243DC5027B2A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F776189-6A1B-451A-B207-B34CC3CD1ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9876" yWindow="2868" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6132" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6212" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1532"/>
+  <dimension ref="A1:J1552"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -37854,6 +37854,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1533" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1533" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1533" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1533" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1533" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1533" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1533" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1533" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1533" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1534" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1534" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1534" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1534" s="3">
+        <v>21</v>
+      </c>
+      <c r="D1534" s="4"/>
+      <c r="E1534" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1534" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1534" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1534" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1535" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1535" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1535" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1535" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1535" s="3"/>
+      <c r="E1535" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1535" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1535" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1535" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1536" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1536" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1536" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1536" s="3"/>
+      <c r="D1536" s="3"/>
+      <c r="E1536" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1536" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1536" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1536" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1537" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1537" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1537" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1537" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1537" s="4"/>
+      <c r="E1537" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1537" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1537" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1537" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1538" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1538" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1538" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1538" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1538" s="3"/>
+      <c r="E1538" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1538" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1538" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1538" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1539" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1539" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1539" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1539" s="3"/>
+      <c r="D1539" s="4"/>
+      <c r="E1539" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1539" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1539" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1539" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1540" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1540" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1540" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1540" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1540" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1540" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1540" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1540" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1540" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1541" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1541" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1541" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1541" s="3"/>
+      <c r="D1541" s="4"/>
+      <c r="E1541" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1541" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1541" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1541" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1542" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1542" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1542" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1542" s="4"/>
+      <c r="D1542" s="4"/>
+      <c r="E1542" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1542" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1542" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1542" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1543" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1543" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1543" s="3"/>
+      <c r="D1543" s="3"/>
+      <c r="E1543" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1543" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1543" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1543" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1544" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1544" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1544" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1544" s="3"/>
+      <c r="E1544" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1544" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1544" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1544" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1545" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1545" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1545" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1545" s="4"/>
+      <c r="E1545" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1545" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1545" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1545" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1546" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1546" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1546" s="3"/>
+      <c r="D1546" s="6"/>
+      <c r="E1546" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1546" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1546" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1546" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1547" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1547" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1547" s="3"/>
+      <c r="D1547" s="6"/>
+      <c r="E1547" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1547" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1547" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1547" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1548" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1548" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1548" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1548" s="3"/>
+      <c r="D1548" s="6"/>
+      <c r="E1548" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1548" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1548" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1548" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1549" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1549" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1549" s="3"/>
+      <c r="D1549" s="6"/>
+      <c r="E1549" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1549" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1549" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1549" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1550" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1550" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1550" s="3"/>
+      <c r="D1550" s="6"/>
+      <c r="E1550" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1550" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1550" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1550" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1551" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1551" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1551" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1551" s="3"/>
+      <c r="D1551" s="6"/>
+      <c r="E1551" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1551" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1551" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1551" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1552" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1552" s="2">
+        <v>44001</v>
+      </c>
+      <c r="B1552" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1552" s="3"/>
+      <c r="D1552" s="4"/>
+      <c r="E1552" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1552" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1552" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1552" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.19. fix euskadi hospitalized data
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F776189-6A1B-451A-B207-B34CC3CD1ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80E30E2-14BC-4CB1-B1FB-BF426E5BC4CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10908" yWindow="3144" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6212" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6292" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1552"/>
+  <dimension ref="A1:J1572"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -38314,6 +38314,464 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1553" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1553" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1553" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1553" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1553" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1553" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1553" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1553" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1553" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1554" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1554" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1554" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1554" s="3">
+        <v>21</v>
+      </c>
+      <c r="D1554" s="4"/>
+      <c r="E1554" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1554" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1554" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1554" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1555" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1555" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1555" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1555" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1555" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1555" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1555" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1555" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1555" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1556" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1556" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1556" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1556" s="3"/>
+      <c r="D1556" s="3"/>
+      <c r="E1556" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1556" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1556" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1556" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1557" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1557" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1557" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1557" s="3"/>
+      <c r="D1557" s="4"/>
+      <c r="E1557" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1557" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1557" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1557" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1558" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1558" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1558" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1558" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1558" s="3"/>
+      <c r="E1558" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1558" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1558" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1558" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1559" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1559" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1559" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1559" s="3"/>
+      <c r="D1559" s="4"/>
+      <c r="E1559" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1559" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1559" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1559" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1560" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1560" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1560" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1560" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1560" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1560" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1560" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1560" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1560" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1561" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1561" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1561" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1561" s="3"/>
+      <c r="D1561" s="4"/>
+      <c r="E1561" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1561" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1561" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1561" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1562" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1562" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1562" s="4"/>
+      <c r="D1562" s="4"/>
+      <c r="E1562" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1562" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1562" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1562" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1563" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1563" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1563" s="3"/>
+      <c r="D1563" s="3"/>
+      <c r="E1563" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1563" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1563" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1563" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1564" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1564" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1564" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1564" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1564" s="3"/>
+      <c r="E1564" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1564" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1564" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1564" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1565" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1565" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1565" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1565" s="3"/>
+      <c r="D1565" s="4"/>
+      <c r="E1565" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1565" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1565" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1565" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1566" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1566" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1566" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1566" s="3"/>
+      <c r="D1566" s="6"/>
+      <c r="E1566" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1566" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1566" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1566" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1567" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1567" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1567" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1567" s="3"/>
+      <c r="D1567" s="6"/>
+      <c r="E1567" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1567" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1567" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1567" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1568" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1568" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1568" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1568" s="3"/>
+      <c r="D1568" s="6"/>
+      <c r="E1568" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1568" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1568" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1568" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1569" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1569" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1569" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1569" s="3"/>
+      <c r="D1569" s="6"/>
+      <c r="E1569" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1569" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1569" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1569" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1570" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1570" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1570" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1570" s="3"/>
+      <c r="D1570" s="6"/>
+      <c r="E1570" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1570" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1570" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1570" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1571" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1571" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1571" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1571" s="3"/>
+      <c r="D1571" s="6"/>
+      <c r="E1571" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1571" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1571" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1571" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1572" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1572" s="2">
+        <v>44002</v>
+      </c>
+      <c r="B1572" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1572" s="3"/>
+      <c r="D1572" s="4"/>
+      <c r="E1572" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1572" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1572" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1572" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.20
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80E30E2-14BC-4CB1-B1FB-BF426E5BC4CB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD57F5E-1124-4662-ACEF-AF4EDE2CF12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10908" yWindow="3144" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10176" yWindow="2448" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6292" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6372" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1572"/>
+  <dimension ref="A1:J1592"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -38772,6 +38772,464 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1573" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1573" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1573" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1573" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1573" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1573" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1573" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1573" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1573" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1574" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1574" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1574" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1574" s="3">
+        <v>16</v>
+      </c>
+      <c r="D1574" s="4"/>
+      <c r="E1574" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1574" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1574" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1574" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1575" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1575" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1575" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1575" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1575" s="3"/>
+      <c r="E1575" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1575" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1575" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1575" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1576" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1576" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1576" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1576" s="3"/>
+      <c r="D1576" s="3"/>
+      <c r="E1576" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1576" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1576" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1576" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1577" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1577" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1577" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1577" s="3"/>
+      <c r="D1577" s="4"/>
+      <c r="E1577" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1577" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1577" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1577" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1578" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1578" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1578" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1578" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1578" s="3"/>
+      <c r="E1578" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1578" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1578" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1578" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1579" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1579" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1579" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1579" s="3"/>
+      <c r="D1579" s="4"/>
+      <c r="E1579" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1579" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1579" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1579" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1580" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1580" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1580" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1580" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1580" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1580" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1580" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1580" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1580" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1581" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1581" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1581" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1581" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1581" s="4"/>
+      <c r="E1581" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1581" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1581" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1581" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1582" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1582" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1582" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1582" s="4"/>
+      <c r="D1582" s="4"/>
+      <c r="E1582" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1582" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1582" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1582" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1583" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1583" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1583" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1583" s="3"/>
+      <c r="D1583" s="3"/>
+      <c r="E1583" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1583" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1583" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1583" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1584" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1584" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1584" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1584" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1584" s="3"/>
+      <c r="E1584" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1584" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1584" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1584" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1585" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1585" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1585" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1585" s="3"/>
+      <c r="D1585" s="4"/>
+      <c r="E1585" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1585" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1585" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1585" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1586" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1586" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1586" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1586" s="3"/>
+      <c r="D1586" s="6"/>
+      <c r="E1586" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1586" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1586" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1586" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1587" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1587" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1587" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1587" s="3"/>
+      <c r="D1587" s="6"/>
+      <c r="E1587" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1587" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1587" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1587" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1588" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1588" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1588" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1588" s="3"/>
+      <c r="D1588" s="6"/>
+      <c r="E1588" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1588" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1588" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1588" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1589" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1589" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1589" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1589" s="3"/>
+      <c r="D1589" s="6"/>
+      <c r="E1589" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1589" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1589" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1589" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1590" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1590" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1590" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1590" s="3"/>
+      <c r="D1590" s="6"/>
+      <c r="E1590" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1590" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1590" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1590" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1591" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1591" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1591" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1591" s="3"/>
+      <c r="D1591" s="6"/>
+      <c r="E1591" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1591" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1591" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1591" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1592" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1592" s="2">
+        <v>44003</v>
+      </c>
+      <c r="B1592" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1592" s="3"/>
+      <c r="D1592" s="4"/>
+      <c r="E1592" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1592" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1592" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1592" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.21
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD57F5E-1124-4662-ACEF-AF4EDE2CF12F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9893D5CD-C4B8-49F1-B7D2-D07214B43F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10176" yWindow="2448" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10704" yWindow="3816" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6372" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6452" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1592"/>
+  <dimension ref="A1:J1612"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -39230,6 +39230,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1593" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1593" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1593" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1593" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1593" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1593" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1593" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1593" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1593" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1594" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1594" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1594" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1594" s="3">
+        <v>23</v>
+      </c>
+      <c r="D1594" s="4"/>
+      <c r="E1594" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1594" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1594" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1594" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1595" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1595" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1595" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1595" s="3"/>
+      <c r="E1595" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1595" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1595" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1595" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1596" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1596" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1596" s="3"/>
+      <c r="D1596" s="3"/>
+      <c r="E1596" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1596" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1596" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1596" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1597" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1597" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1597" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1597" s="4"/>
+      <c r="E1597" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1597" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1597" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1597" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1598" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1598" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1598" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1598" s="3"/>
+      <c r="E1598" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1598" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1598" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1598" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1599" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1599" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1599" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1599" s="3"/>
+      <c r="D1599" s="4"/>
+      <c r="E1599" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1599" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1599" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1599" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1600" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1600" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1600" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1600" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1600" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1600" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1600" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1600" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1600" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1601" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1601" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1601" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1601" s="3"/>
+      <c r="D1601" s="4"/>
+      <c r="E1601" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1601" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1601" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1601" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1602" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1602" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1602" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1602" s="4"/>
+      <c r="D1602" s="4"/>
+      <c r="E1602" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1602" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1602" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1602" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1603" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1603" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1603" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1603" s="3"/>
+      <c r="D1603" s="3"/>
+      <c r="E1603" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1603" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1603" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1603" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1604" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1604" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1604" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1604" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1604" s="3"/>
+      <c r="E1604" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1604" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1604" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1604" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1605" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1605" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1605" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1605" s="3"/>
+      <c r="D1605" s="4"/>
+      <c r="E1605" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1605" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1605" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1605" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1606" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1606" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1606" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1606" s="3"/>
+      <c r="D1606" s="6"/>
+      <c r="E1606" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1606" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1606" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1606" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1607" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1607" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1607" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1607" s="3"/>
+      <c r="D1607" s="6"/>
+      <c r="E1607" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1607" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1607" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1607" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1608" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1608" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1608" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1608" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1608" s="6"/>
+      <c r="E1608" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1608" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1608" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1608" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1609" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1609" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1609" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1609" s="3"/>
+      <c r="D1609" s="6"/>
+      <c r="E1609" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1609" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1609" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1609" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1610" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1610" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1610" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1610" s="3"/>
+      <c r="D1610" s="6"/>
+      <c r="E1610" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1610" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1610" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1610" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1611" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1611" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1611" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1611" s="3"/>
+      <c r="D1611" s="6"/>
+      <c r="E1611" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1611" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1611" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1611" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1612" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1612" s="2">
+        <v>44004</v>
+      </c>
+      <c r="B1612" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1612" s="3"/>
+      <c r="D1612" s="4"/>
+      <c r="E1612" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1612" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1612" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1612" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.22
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9893D5CD-C4B8-49F1-B7D2-D07214B43F07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5CD2CB-36EF-4F9A-B38F-1E516A2A0BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10704" yWindow="3816" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3600" yWindow="3552" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6452" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6532" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1612"/>
+  <dimension ref="A1:J1632"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -39690,6 +39690,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1613" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1613" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1613" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1613" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1613" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1613" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1613" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1613" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1613" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1614" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1614" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1614" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1614" s="3">
+        <v>21</v>
+      </c>
+      <c r="D1614" s="4"/>
+      <c r="E1614" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1614" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1614" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1614" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1615" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1615" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1615" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1615" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1615" s="3"/>
+      <c r="E1615" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1615" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1615" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1615" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1616" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1616" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1616" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1616" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1616" s="3"/>
+      <c r="E1616" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1616" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1616" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1616" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1617" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1617" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1617" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1617" s="3"/>
+      <c r="D1617" s="4"/>
+      <c r="E1617" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1617" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1617" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1617" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1618" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1618" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1618" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1618" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1618" s="3"/>
+      <c r="E1618" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1618" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1618" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1618" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1619" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1619" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1619" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1619" s="3"/>
+      <c r="D1619" s="4"/>
+      <c r="E1619" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1619" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1619" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1619" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1620" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1620" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1620" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1620" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1620" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1620" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1620" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1620" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1620" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1621" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1621" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1621" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1621" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1621" s="4"/>
+      <c r="E1621" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1621" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1621" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1621" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1622" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1622" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1622" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1622" s="4"/>
+      <c r="D1622" s="4"/>
+      <c r="E1622" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1622" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1622" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1622" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1623" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1623" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1623" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1623" s="3"/>
+      <c r="D1623" s="3"/>
+      <c r="E1623" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1623" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1623" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1623" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1624" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1624" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1624" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1624" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1624" s="3"/>
+      <c r="E1624" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1624" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1624" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1624" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1625" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1625" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1625" s="3"/>
+      <c r="D1625" s="4"/>
+      <c r="E1625" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1625" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1625" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1625" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1626" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1626" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1626" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1626" s="3"/>
+      <c r="D1626" s="6"/>
+      <c r="E1626" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1626" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1626" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1626" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1627" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1627" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1627" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1627" s="3"/>
+      <c r="D1627" s="6"/>
+      <c r="E1627" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1627" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1627" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1627" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1628" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1628" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1628" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1628" s="3"/>
+      <c r="D1628" s="6"/>
+      <c r="E1628" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1628" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1628" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1628" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1629" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1629" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1629" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1629" s="3"/>
+      <c r="D1629" s="6"/>
+      <c r="E1629" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1629" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1629" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1629" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1630" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1630" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1630" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1630" s="3"/>
+      <c r="D1630" s="6"/>
+      <c r="E1630" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1630" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1630" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1630" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1631" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1631" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1631" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1631" s="3"/>
+      <c r="D1631" s="6"/>
+      <c r="E1631" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1631" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1631" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1631" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1632" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1632" s="2">
+        <v>44005</v>
+      </c>
+      <c r="B1632" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1632" s="3"/>
+      <c r="D1632" s="4"/>
+      <c r="E1632" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1632" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1632" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1632" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update SPain provinces data and charts 2020.06.23
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E5CD2CB-36EF-4F9A-B38F-1E516A2A0BAC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5B8181-3612-4D89-9D01-6EB846F0D23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3600" yWindow="3552" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9420" yWindow="2652" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6532" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6612" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1632"/>
+  <dimension ref="A1:J1652"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -40150,6 +40150,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1633" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1633" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1633" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1633" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1633" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1633" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1633" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1633" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1633" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1634" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1634" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1634" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1634" s="3">
+        <v>26</v>
+      </c>
+      <c r="D1634" s="4"/>
+      <c r="E1634" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1634" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1634" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1634" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1635" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1635" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1635" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1635" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1635" s="3"/>
+      <c r="E1635" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1635" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1635" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1635" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1636" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1636" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1636" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1636" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1636" s="3"/>
+      <c r="E1636" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1636" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1636" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1636" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1637" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1637" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1637" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1637" s="3"/>
+      <c r="D1637" s="4"/>
+      <c r="E1637" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1637" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1637" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1637" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1638" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1638" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1638" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1638" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1638" s="3"/>
+      <c r="E1638" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1638" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1638" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1638" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1639" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1639" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1639" s="3"/>
+      <c r="D1639" s="4"/>
+      <c r="E1639" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1639" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1639" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1639" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1640" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1640" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1640" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1640" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1640" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1640" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1640" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1640" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1641" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1641" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1641" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1641" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1641" s="4"/>
+      <c r="E1641" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1641" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1641" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1641" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1642" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1642" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1642" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1642" s="4"/>
+      <c r="D1642" s="4"/>
+      <c r="E1642" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1642" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1642" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1642" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1643" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1643" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1643" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1643" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1643" s="3"/>
+      <c r="E1643" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1643" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1643" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1643" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1644" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1644" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1644" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1644" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1644" s="3"/>
+      <c r="E1644" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1644" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1644" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1644" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1645" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1645" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1645" s="3"/>
+      <c r="D1645" s="4"/>
+      <c r="E1645" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1645" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1645" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1645" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1646" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1646" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1646" s="3"/>
+      <c r="D1646" s="6"/>
+      <c r="E1646" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1646" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1646" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1646" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1647" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1647" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1647" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1647" s="3"/>
+      <c r="D1647" s="6"/>
+      <c r="E1647" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1647" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1647" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1647" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1648" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1648" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1648" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1648" s="3"/>
+      <c r="D1648" s="6"/>
+      <c r="E1648" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1648" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1648" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1648" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1649" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1649" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1649" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1649" s="3"/>
+      <c r="D1649" s="6"/>
+      <c r="E1649" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1649" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1649" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1649" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1650" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1650" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1650" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1650" s="3"/>
+      <c r="D1650" s="6"/>
+      <c r="E1650" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1650" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1650" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1650" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1651" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1651" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1651" s="3"/>
+      <c r="D1651" s="6"/>
+      <c r="E1651" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1651" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1651" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1651" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1652" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1652" s="2">
+        <v>44006</v>
+      </c>
+      <c r="B1652" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1652" s="3"/>
+      <c r="D1652" s="4"/>
+      <c r="E1652" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1652" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1652" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1652" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts + euskadi hospitalized 2020.06.24
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF5B8181-3612-4D89-9D01-6EB846F0D23D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7EB33A-E3F2-48AA-AEAA-04C4364BEB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9420" yWindow="2652" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="2640" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6612" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1652"/>
+  <dimension ref="A1:J1672"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -40612,6 +40612,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1653" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1653" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1653" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1653" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1653" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1653" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1653" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1653" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1653" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1654" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1654" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1654" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1654" s="3">
+        <v>25</v>
+      </c>
+      <c r="D1654" s="4"/>
+      <c r="E1654" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1654" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1654" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1654" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1655" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1655" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1655" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1655" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1655" s="3"/>
+      <c r="E1655" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1655" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1655" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1655" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1656" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1656" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1656" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1656" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1656" s="3"/>
+      <c r="E1656" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1656" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1656" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1656" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1657" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1657" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1657" s="3"/>
+      <c r="D1657" s="4"/>
+      <c r="E1657" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1657" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1657" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1657" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1658" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1658" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1658" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1658" s="3"/>
+      <c r="E1658" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1658" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1658" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1658" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1659" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1659" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1659" s="3"/>
+      <c r="D1659" s="4"/>
+      <c r="E1659" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1659" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1659" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1659" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1660" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1660" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1660" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1660" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1660" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1660" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1660" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1660" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1660" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1661" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1661" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1661" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1661" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1661" s="4"/>
+      <c r="E1661" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1661" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1661" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1661" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1662" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1662" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1662" s="4"/>
+      <c r="D1662" s="4"/>
+      <c r="E1662" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1662" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1662" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1662" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1663" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1663" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1663" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1663" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1663" s="3"/>
+      <c r="E1663" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1663" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1663" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1663" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1664" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1664" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1664" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1664" s="3"/>
+      <c r="E1664" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1664" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1664" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1664" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1665" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1665" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1665" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1665" s="3"/>
+      <c r="D1665" s="4"/>
+      <c r="E1665" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1665" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1665" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1665" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1666" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1666" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1666" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1666" s="3"/>
+      <c r="D1666" s="6"/>
+      <c r="E1666" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1666" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1666" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1666" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1667" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1667" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1667" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1667" s="3"/>
+      <c r="D1667" s="6"/>
+      <c r="E1667" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1667" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1667" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1667" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1668" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1668" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1668" s="3"/>
+      <c r="D1668" s="6"/>
+      <c r="E1668" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1668" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1668" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1668" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1669" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1669" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1669" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1669" s="3"/>
+      <c r="D1669" s="6"/>
+      <c r="E1669" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1669" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1669" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1669" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1670" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1670" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1670" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1670" s="3"/>
+      <c r="D1670" s="6"/>
+      <c r="E1670" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1670" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1670" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1670" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1671" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1671" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1671" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1671" s="3"/>
+      <c r="D1671" s="6"/>
+      <c r="E1671" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1671" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1671" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1671" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1672" s="2">
+        <v>44007</v>
+      </c>
+      <c r="B1672" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1672" s="3"/>
+      <c r="D1672" s="4"/>
+      <c r="E1672" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1672" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1672" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1672" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data 2020.06.25
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB7EB33A-E3F2-48AA-AEAA-04C4364BEB0A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D45D373-1B2C-41A6-85BA-87F49B65F94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2640" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8076" yWindow="2664" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6692" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6772" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1672"/>
+  <dimension ref="A1:J1692"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -41074,6 +41074,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1673" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1673" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1673" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1673" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1673" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1673" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1673" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1673" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1673" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1674" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1674" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1674" s="3">
+        <v>26</v>
+      </c>
+      <c r="D1674" s="4"/>
+      <c r="E1674" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1674" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1674" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1674" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1675" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1675" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1675" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1675" s="3"/>
+      <c r="E1675" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1675" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1675" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1675" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1676" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1676" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1676" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1676" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1676" s="3"/>
+      <c r="E1676" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1676" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1676" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1676" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1677" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1677" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1677" s="3"/>
+      <c r="D1677" s="4"/>
+      <c r="E1677" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1677" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1677" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1677" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1678" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1678" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1678" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1678" s="3"/>
+      <c r="E1678" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1678" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1678" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1678" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1679" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1679" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1679" s="3"/>
+      <c r="D1679" s="4"/>
+      <c r="E1679" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1679" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1679" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1679" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1680" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1680" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1680" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1680" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1680" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1680" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1680" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1680" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1681" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1681" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1681" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1681" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1681" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1681" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1681" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1681" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1682" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1682" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1682" s="4"/>
+      <c r="D1682" s="4"/>
+      <c r="E1682" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1682" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1682" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1682" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1683" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1683" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1683" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1683" s="3"/>
+      <c r="D1683" s="3"/>
+      <c r="E1683" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1683" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1683" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1683" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1684" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1684" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1684" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1684" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1684" s="3"/>
+      <c r="E1684" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1684" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1684" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1684" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1685" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1685" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1685" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1685" s="3"/>
+      <c r="D1685" s="4"/>
+      <c r="E1685" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1685" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1685" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1685" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1686" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1686" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1686" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1686" s="3"/>
+      <c r="D1686" s="6"/>
+      <c r="E1686" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1686" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1686" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1686" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1687" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1687" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1687" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1687" s="3"/>
+      <c r="D1687" s="6"/>
+      <c r="E1687" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1687" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1687" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1687" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1688" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1688" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1688" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1688" s="3"/>
+      <c r="D1688" s="6"/>
+      <c r="E1688" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1688" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1688" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1688" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1689" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1689" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1689" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1689" s="3"/>
+      <c r="D1689" s="6"/>
+      <c r="E1689" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1689" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1689" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1689" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1690" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1690" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1690" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1690" s="3"/>
+      <c r="D1690" s="6"/>
+      <c r="E1690" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1690" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1690" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1690" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1691" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1691" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1691" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1691" s="3"/>
+      <c r="D1691" s="6"/>
+      <c r="E1691" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1691" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1691" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1691" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1692" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1692" s="2">
+        <v>44008</v>
+      </c>
+      <c r="B1692" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1692" s="3"/>
+      <c r="D1692" s="4"/>
+      <c r="E1692" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1692" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1692" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1692" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data and charts 2020.06.27
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D45D373-1B2C-41A6-85BA-87F49B65F94D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459C82D2-AD1F-4873-89C3-BA46784E1D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8076" yWindow="2664" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7248" yWindow="2196" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6772" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6932" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1692"/>
+  <dimension ref="A1:J1732"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -41536,6 +41536,926 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1693" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1693" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1693" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1693" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1693" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1693" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1693" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1693" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1693" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1694" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1694" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1694" s="3">
+        <v>30</v>
+      </c>
+      <c r="D1694" s="4"/>
+      <c r="E1694" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1694" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1694" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1694" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1695" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1695" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1695" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1695" s="3"/>
+      <c r="E1695" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1695" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1695" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1695" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1696" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1696" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1696" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1696" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1696" s="3"/>
+      <c r="E1696" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1696" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1696" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1696" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1697" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1697" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1697" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1697" s="3"/>
+      <c r="D1697" s="4"/>
+      <c r="E1697" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1697" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1697" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1697" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1698" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1698" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1698" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1698" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1698" s="3"/>
+      <c r="E1698" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1698" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1698" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1698" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1699" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1699" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1699" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1699" s="3"/>
+      <c r="D1699" s="4"/>
+      <c r="E1699" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1699" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1699" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1699" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1700" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1700" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1700" s="3">
+        <v>9</v>
+      </c>
+      <c r="D1700" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1700" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1700" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1700" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1700" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1701" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1701" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1701" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1701" s="4"/>
+      <c r="E1701" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1701" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1701" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1701" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1702" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1702" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1702" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1702" s="4"/>
+      <c r="D1702" s="4"/>
+      <c r="E1702" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1702" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1702" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1702" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1703" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1703" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1703" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1703" s="3"/>
+      <c r="D1703" s="3"/>
+      <c r="E1703" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1703" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1703" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1703" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1704" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1704" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1704" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1704" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1704" s="3"/>
+      <c r="E1704" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1704" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1704" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1704" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1705" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1705" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1705" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1705" s="3"/>
+      <c r="D1705" s="4"/>
+      <c r="E1705" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1705" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1705" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1705" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1706" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1706" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1706" s="3"/>
+      <c r="D1706" s="6"/>
+      <c r="E1706" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1706" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1706" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1706" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1707" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1707" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1707" s="3"/>
+      <c r="D1707" s="6"/>
+      <c r="E1707" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1707" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1707" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1707" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1708" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1708" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1708" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1708" s="3"/>
+      <c r="D1708" s="6"/>
+      <c r="E1708" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1708" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1708" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1708" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1709" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1709" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1709" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1709" s="3"/>
+      <c r="D1709" s="6"/>
+      <c r="E1709" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1709" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1709" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1709" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1710" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1710" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1710" s="3"/>
+      <c r="D1710" s="6"/>
+      <c r="E1710" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1710" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1710" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1710" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1711" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1711" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1711" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1711" s="3"/>
+      <c r="D1711" s="6"/>
+      <c r="E1711" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1711" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1711" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1711" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1712" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1712" s="2">
+        <v>44009</v>
+      </c>
+      <c r="B1712" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1712" s="3"/>
+      <c r="D1712" s="4"/>
+      <c r="E1712" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1712" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1712" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1712" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1713" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1713" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1713" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1713" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1713" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1713" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1713" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1713" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1714" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1714" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1714" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1714" s="3">
+        <v>22</v>
+      </c>
+      <c r="D1714" s="4"/>
+      <c r="E1714" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1714" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1714" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1714" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1715" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1715" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1715" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1715" s="3"/>
+      <c r="D1715" s="3"/>
+      <c r="E1715" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1715" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1715" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1715" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1716" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1716" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1716" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1716" s="3"/>
+      <c r="E1716" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1716" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1716" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1716" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1717" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1717" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1717" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1717" s="3"/>
+      <c r="D1717" s="4"/>
+      <c r="E1717" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1717" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1717" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1717" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1718" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1718" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1718" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1718" s="3"/>
+      <c r="E1718" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1718" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1718" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1718" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1719" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1719" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1719" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1719" s="3"/>
+      <c r="D1719" s="4"/>
+      <c r="E1719" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1719" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1719" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1719" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1720" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1720" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1720" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1720" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1720" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1720" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1720" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1720" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1720" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1721" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1721" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1721" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1721" s="4"/>
+      <c r="E1721" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1721" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1721" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1721" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1722" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1722" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1722" s="4"/>
+      <c r="D1722" s="4"/>
+      <c r="E1722" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1722" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1722" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1722" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1723" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1723" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1723" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1723" s="3"/>
+      <c r="D1723" s="3"/>
+      <c r="E1723" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1723" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1723" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1723" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1724" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1724" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1724" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1724" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1724" s="3"/>
+      <c r="E1724" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1724" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1724" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1724" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1725" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1725" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1725" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1725" s="3"/>
+      <c r="D1725" s="4"/>
+      <c r="E1725" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1725" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1725" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1725" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1726" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1726" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1726" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1726" s="3"/>
+      <c r="D1726" s="6"/>
+      <c r="E1726" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1726" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1726" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1726" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1727" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1727" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1727" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1727" s="3"/>
+      <c r="D1727" s="6"/>
+      <c r="E1727" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1727" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1727" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1727" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1728" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1728" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1728" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1728" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1728" s="6"/>
+      <c r="E1728" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1728" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1728" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1728" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1729" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1729" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1729" s="3"/>
+      <c r="D1729" s="6"/>
+      <c r="E1729" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1729" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1729" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1729" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1730" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1730" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1730" s="3"/>
+      <c r="D1730" s="6"/>
+      <c r="E1730" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1730" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1730" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1730" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1731" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1731" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1731" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1731" s="3"/>
+      <c r="D1731" s="6"/>
+      <c r="E1731" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1731" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1731" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1731" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1732" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1732" s="2">
+        <v>44010</v>
+      </c>
+      <c r="B1732" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1732" s="3"/>
+      <c r="D1732" s="4"/>
+      <c r="E1732" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1732" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1732" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1732" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data and charts 2020.06.29
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{459C82D2-AD1F-4873-89C3-BA46784E1D0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A86ED05-C5D5-4D77-BA04-CC4A83E657B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7248" yWindow="2196" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9924" yWindow="2040" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6932" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1732"/>
+  <dimension ref="A1:J1752"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -42456,6 +42456,466 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1733" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1733" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1733" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1733" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1733" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1733" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1733" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1733" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1733" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1734" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1734" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1734" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1734" s="3">
+        <v>26</v>
+      </c>
+      <c r="D1734" s="4"/>
+      <c r="E1734" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1734" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1734" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1734" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1735" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1735" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1735" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1735" s="3"/>
+      <c r="D1735" s="3"/>
+      <c r="E1735" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1735" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1735" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1735" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1736" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1736" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1736" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1736" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1736" s="3"/>
+      <c r="E1736" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1736" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1736" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1736" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1737" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1737" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1737" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1737" s="3"/>
+      <c r="D1737" s="4"/>
+      <c r="E1737" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1737" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1737" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1737" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1738" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1738" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1738" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1738" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1738" s="3"/>
+      <c r="E1738" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1738" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1738" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1738" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1739" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1739" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1739" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1739" s="3"/>
+      <c r="D1739" s="4"/>
+      <c r="E1739" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1739" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1739" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1739" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1740" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1740" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1740" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1740" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1740" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1740" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1740" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1740" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1740" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1741" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1741" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1741" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1741" s="4"/>
+      <c r="E1741" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1741" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1741" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1741" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1742" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1742" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1742" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1742" s="4"/>
+      <c r="D1742" s="4"/>
+      <c r="E1742" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1742" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1742" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1742" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1743" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1743" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1743" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1743" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1743" s="3"/>
+      <c r="E1743" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1743" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1743" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1743" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1744" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1744" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1744" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1744" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1744" s="3"/>
+      <c r="E1744" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1744" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1744" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1744" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1745" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1745" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1745" s="3"/>
+      <c r="D1745" s="4"/>
+      <c r="E1745" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1745" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1745" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1745" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1746" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1746" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1746" s="3"/>
+      <c r="D1746" s="6"/>
+      <c r="E1746" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1746" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1746" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1746" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1747" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1747" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1747" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1747" s="3"/>
+      <c r="D1747" s="6"/>
+      <c r="E1747" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1747" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1747" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1747" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1748" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1748" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1748" s="3"/>
+      <c r="D1748" s="6"/>
+      <c r="E1748" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1748" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1748" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1748" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1749" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1749" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1749" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1749" s="3"/>
+      <c r="D1749" s="6"/>
+      <c r="E1749" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1749" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1749" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1749" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1750" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1750" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1750" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1750" s="3"/>
+      <c r="D1750" s="6"/>
+      <c r="E1750" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1750" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1750" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1750" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1751" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1751" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1751" s="3"/>
+      <c r="D1751" s="6"/>
+      <c r="E1751" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1751" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1751" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1751" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1752" s="2">
+        <v>44012</v>
+      </c>
+      <c r="B1752" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1752" s="3"/>
+      <c r="D1752" s="4"/>
+      <c r="E1752" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1752" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1752" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1752" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data and charts 2020.06.30
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A86ED05-C5D5-4D77-BA04-CC4A83E657B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12E801D-0631-4F59-A635-D97C28C20837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9924" yWindow="2040" windowWidth="17292" windowHeight="6600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10248" yWindow="2172" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7012" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1752"/>
+  <dimension ref="A1:J1772"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -42916,6 +42916,470 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1753" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1753" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1753" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1753" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1753" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1753" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1753" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1753" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1753" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1754" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1754" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1754" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1754" s="3">
+        <v>27</v>
+      </c>
+      <c r="D1754" s="4"/>
+      <c r="E1754" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1754" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1754" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1754" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1755" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1755" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1755" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1755" s="3"/>
+      <c r="D1755" s="3"/>
+      <c r="E1755" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1755" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1755" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1755" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1756" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1756" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1756" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1756" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1756" s="3"/>
+      <c r="E1756" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1756" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1756" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1756" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1757" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1757" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1757" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1757" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1757" s="4"/>
+      <c r="E1757" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1757" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1757" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1757" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1758" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1758" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1758" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1758" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1758" s="3"/>
+      <c r="E1758" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1758" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1758" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1758" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1759" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1759" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1759" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1759" s="3"/>
+      <c r="D1759" s="4"/>
+      <c r="E1759" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1759" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1759" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1759" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1760" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1760" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1760" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1760" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1760" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1760" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1760" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1760" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1760" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1761" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1761" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1761" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1761" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1761" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1761" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1761" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1761" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1761" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1762" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1762" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1762" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1762" s="4"/>
+      <c r="D1762" s="4"/>
+      <c r="E1762" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1762" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1762" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1762" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1763" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1763" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1763" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1763" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1763" s="3"/>
+      <c r="E1763" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1763" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1763" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1763" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1764" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1764" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1764" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1764" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1764" s="3"/>
+      <c r="E1764" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1764" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1764" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1764" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1765" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1765" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1765" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1765" s="3"/>
+      <c r="D1765" s="4"/>
+      <c r="E1765" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1765" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1765" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1765" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1766" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1766" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1766" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1766" s="3"/>
+      <c r="D1766" s="6"/>
+      <c r="E1766" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1766" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1766" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1766" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1767" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1767" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1767" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1767" s="3"/>
+      <c r="D1767" s="6"/>
+      <c r="E1767" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1767" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1767" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1767" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1768" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1768" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1768" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1768" s="3"/>
+      <c r="D1768" s="6"/>
+      <c r="E1768" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1768" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1768" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1768" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1769" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1769" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1769" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1769" s="3"/>
+      <c r="D1769" s="6"/>
+      <c r="E1769" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1769" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1769" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1769" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1770" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1770" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1770" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1770" s="3"/>
+      <c r="D1770" s="6"/>
+      <c r="E1770" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1770" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1770" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1770" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1771" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1771" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1771" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1771" s="3"/>
+      <c r="D1771" s="6"/>
+      <c r="E1771" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1771" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1771" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1771" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1772" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1772" s="2">
+        <v>44013</v>
+      </c>
+      <c r="B1772" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1772" s="3"/>
+      <c r="D1772" s="4"/>
+      <c r="E1772" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1772" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1772" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1772" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data 2020.07.01
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12E801D-0631-4F59-A635-D97C28C20837}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CA7DC0-44EA-4506-8B31-B3EB71042E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10248" yWindow="2172" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9744" yWindow="2448" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7092" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7172" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1772"/>
+  <dimension ref="A1:J1792"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -43380,6 +43380,470 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1773" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1773" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1773" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1773" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1773" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1773" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1773" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1773" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1773" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1774" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1774" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1774" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1774" s="3">
+        <v>20</v>
+      </c>
+      <c r="D1774" s="4"/>
+      <c r="E1774" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1774" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1774" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1774" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1775" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1775" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1775" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1775" s="3"/>
+      <c r="D1775" s="3"/>
+      <c r="E1775" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1775" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1775" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1775" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1776" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1776" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1776" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1776" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1776" s="3"/>
+      <c r="E1776" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1776" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1776" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1776" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1777" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1777" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1777" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1777" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1777" s="4"/>
+      <c r="E1777" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1777" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1777" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1777" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1778" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1778" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1778" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1778" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1778" s="3"/>
+      <c r="E1778" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1778" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1778" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1778" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1779" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1779" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1779" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1779" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1779" s="4"/>
+      <c r="E1779" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1779" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1779" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1779" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1780" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1780" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1780" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1780" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1780" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1780" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1780" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1780" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1780" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1781" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1781" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1781" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1781" s="3">
+        <v>6</v>
+      </c>
+      <c r="D1781" s="4"/>
+      <c r="E1781" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1781" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1781" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1781" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1782" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1782" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1782" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1782" s="4"/>
+      <c r="D1782" s="4"/>
+      <c r="E1782" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1782" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1782" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1782" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1783" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1783" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1783" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1783" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1783" s="3"/>
+      <c r="E1783" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1783" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1783" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1783" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1784" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1784" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1784" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1784" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1784" s="3"/>
+      <c r="E1784" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1784" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1784" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1784" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1785" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1785" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1785" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1785" s="3"/>
+      <c r="D1785" s="4"/>
+      <c r="E1785" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1785" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1785" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1785" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1786" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1786" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1786" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1786" s="3"/>
+      <c r="D1786" s="6"/>
+      <c r="E1786" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1786" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1786" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1786" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1787" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1787" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1787" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1787" s="3"/>
+      <c r="D1787" s="6"/>
+      <c r="E1787" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1787" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1787" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1787" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1788" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1788" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1788" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1788" s="3"/>
+      <c r="D1788" s="6"/>
+      <c r="E1788" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1788" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1788" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1788" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1789" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1789" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1789" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1789" s="3"/>
+      <c r="D1789" s="6"/>
+      <c r="E1789" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1789" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1789" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1789" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1790" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1790" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1790" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1790" s="3"/>
+      <c r="D1790" s="6"/>
+      <c r="E1790" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1790" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1790" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1790" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1791" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1791" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1791" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1791" s="3"/>
+      <c r="D1791" s="6"/>
+      <c r="E1791" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1791" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1791" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1791" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1792" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1792" s="2">
+        <v>44014</v>
+      </c>
+      <c r="B1792" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1792" s="3"/>
+      <c r="D1792" s="4"/>
+      <c r="E1792" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1792" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1792" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1792" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data and charts 2020.07.03
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49CA7DC0-44EA-4506-8B31-B3EB71042E3F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6A9966-286B-479C-9F35-918E94642826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9744" yWindow="2448" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4068" yWindow="5292" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7172" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7252" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1792"/>
+  <dimension ref="A1:J1812"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -43844,6 +43844,472 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1793" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1793" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1793" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1793" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1793" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1793" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1793" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1793" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1793" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1794" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1794" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1794" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1794" s="3">
+        <v>20</v>
+      </c>
+      <c r="D1794" s="4"/>
+      <c r="E1794" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1794" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1794" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1794" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1795" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1795" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1795" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1795" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1795" s="3"/>
+      <c r="E1795" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1795" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1795" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1795" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1796" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1796" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1796" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1796" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1796" s="3"/>
+      <c r="E1796" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1796" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1796" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1796" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1797" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1797" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1797" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1797" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1797" s="4"/>
+      <c r="E1797" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1797" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1797" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1797" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1798" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1798" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1798" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1798" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1798" s="3"/>
+      <c r="E1798" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1798" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1798" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1798" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1799" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1799" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1799" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1799" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1799" s="4"/>
+      <c r="E1799" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1799" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1799" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1799" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1800" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1800" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1800" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1800" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1800" s="3">
+        <v>3</v>
+      </c>
+      <c r="E1800" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1800" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1800" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1800" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1801" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1801" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1801" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1801" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1801" s="4"/>
+      <c r="E1801" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1801" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1801" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1801" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1802" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1802" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1802" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1802" s="4"/>
+      <c r="D1802" s="4"/>
+      <c r="E1802" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1802" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1802" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1802" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1803" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1803" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1803" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1803" s="3"/>
+      <c r="D1803" s="3"/>
+      <c r="E1803" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1803" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1803" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1803" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1804" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1804" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1804" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1804" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1804" s="3"/>
+      <c r="E1804" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1804" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1804" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1804" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1805" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1805" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1805" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1805" s="3"/>
+      <c r="D1805" s="4"/>
+      <c r="E1805" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1805" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1805" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1805" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1806" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1806" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1806" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1806" s="3"/>
+      <c r="D1806" s="6"/>
+      <c r="E1806" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1806" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1806" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1806" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1807" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1807" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1807" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1807" s="3"/>
+      <c r="D1807" s="6"/>
+      <c r="E1807" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1807" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1807" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1807" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1808" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1808" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1808" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1808" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1808" s="6"/>
+      <c r="E1808" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1808" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1808" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1808" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1809" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1809" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1809" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1809" s="3"/>
+      <c r="D1809" s="6"/>
+      <c r="E1809" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1809" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1809" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1809" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1810" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1810" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1810" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1810" s="3"/>
+      <c r="D1810" s="6"/>
+      <c r="E1810" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1810" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1810" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1810" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1811" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1811" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1811" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1811" s="3"/>
+      <c r="D1811" s="6"/>
+      <c r="E1811" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1811" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1811" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1811" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1812" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1812" s="2">
+        <v>44015</v>
+      </c>
+      <c r="B1812" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1812" s="3"/>
+      <c r="D1812" s="4"/>
+      <c r="E1812" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1812" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1812" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1812" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts and Euskadi hospitalized 2020.07.06
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC6A9966-286B-479C-9F35-918E94642826}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B5FB99-6490-46B9-B669-C16BEAB12920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4068" yWindow="5292" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9720" yWindow="3084" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7252" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7332" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1812"/>
+  <dimension ref="A1:J1832"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -44310,6 +44310,474 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1813" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1813" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1813" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1813" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1813" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1813" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1813" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1813" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1813" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1814" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1814" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1814" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1814" s="3">
+        <v>18</v>
+      </c>
+      <c r="D1814" s="4"/>
+      <c r="E1814" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1814" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1814" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1814" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1815" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1815" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1815" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1815" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1815" s="3"/>
+      <c r="E1815" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1815" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1815" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1815" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1816" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1816" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1816" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1816" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1816" s="3"/>
+      <c r="E1816" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1816" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1816" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1816" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1817" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1817" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1817" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1817" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1817" s="4"/>
+      <c r="E1817" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1817" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1817" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1817" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1818" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1818" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1818" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1818" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1818" s="3"/>
+      <c r="E1818" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1818" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1818" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1818" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1819" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1819" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1819" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1819" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1819" s="4"/>
+      <c r="E1819" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1819" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1819" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1819" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1820" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1820" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1820" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1820" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1820" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1820" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1820" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1820" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1820" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1821" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1821" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1821" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1821" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1821" s="4"/>
+      <c r="E1821" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1821" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1821" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1821" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1822" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1822" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1822" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1822" s="4"/>
+      <c r="D1822" s="4"/>
+      <c r="E1822" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1822" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1822" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1822" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1823" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1823" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1823" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1823" s="3"/>
+      <c r="D1823" s="3"/>
+      <c r="E1823" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1823" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1823" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1823" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1824" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1824" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1824" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1824" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1824" s="3"/>
+      <c r="E1824" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1824" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1824" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1824" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1825" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1825" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1825" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1825" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1825" s="4"/>
+      <c r="E1825" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1825" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1825" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1825" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1826" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1826" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1826" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1826" s="3"/>
+      <c r="D1826" s="6"/>
+      <c r="E1826" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1826" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1826" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1826" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1827" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1827" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1827" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1827" s="3"/>
+      <c r="D1827" s="6"/>
+      <c r="E1827" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1827" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1827" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1827" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1828" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1828" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1828" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1828" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1828" s="6"/>
+      <c r="E1828" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1828" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1828" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1828" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1829" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1829" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1829" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1829" s="3"/>
+      <c r="D1829" s="6"/>
+      <c r="E1829" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1829" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1829" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1829" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1830" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1830" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1830" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1830" s="3"/>
+      <c r="D1830" s="6"/>
+      <c r="E1830" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1830" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1830" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1830" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1831" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1831" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1831" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1831" s="3"/>
+      <c r="D1831" s="6"/>
+      <c r="E1831" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1831" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1831" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1831" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1832" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1832" s="2">
+        <v>44018</v>
+      </c>
+      <c r="B1832" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1832" s="3"/>
+      <c r="D1832" s="4"/>
+      <c r="E1832" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1832" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1832" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1832" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data and charts and Euskadi hospitalized data-charts 2020.07.07
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33B5FB99-6490-46B9-B669-C16BEAB12920}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{827D64A6-A961-4C27-8915-C4FCDC2E45F3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9720" yWindow="3084" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9648" yWindow="2508" windowWidth="17280" windowHeight="6540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7332" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7412" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1832"/>
+  <dimension ref="A1:J1852"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -44778,6 +44778,470 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1833" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1833" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1833" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1833" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1833" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1833" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1833" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1833" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1833" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1834" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1834" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1834" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1834" s="3">
+        <v>19</v>
+      </c>
+      <c r="D1834" s="4"/>
+      <c r="E1834" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1834" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1834" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1834" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1835" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1835" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1835" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1835" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1835" s="3"/>
+      <c r="E1835" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1835" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1835" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1835" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1836" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1836" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1836" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1836" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1836" s="3"/>
+      <c r="E1836" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1836" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1836" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1836" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1837" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1837" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1837" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1837" s="4"/>
+      <c r="E1837" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1837" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1837" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1837" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1838" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1838" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1838" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1838" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1838" s="3"/>
+      <c r="E1838" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1838" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1838" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1838" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1839" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1839" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1839" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1839" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1839" s="4"/>
+      <c r="E1839" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1839" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1839" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1839" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1840" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1840" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1840" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1840" s="3">
+        <v>7</v>
+      </c>
+      <c r="D1840" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1840" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1840" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1840" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1840" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1841" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1841" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1841" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1841" s="3"/>
+      <c r="D1841" s="4"/>
+      <c r="E1841" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1841" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1841" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1841" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1842" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1842" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1842" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1842" s="4"/>
+      <c r="D1842" s="4"/>
+      <c r="E1842" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1842" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1842" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1842" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1843" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1843" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1843" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1843" s="3"/>
+      <c r="D1843" s="3"/>
+      <c r="E1843" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1843" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1843" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1843" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1844" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1844" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1844" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1844" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1844" s="3"/>
+      <c r="E1844" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1844" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1844" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1844" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1845" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1845" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1845" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1845" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1845" s="4"/>
+      <c r="E1845" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1845" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1845" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1845" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1846" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1846" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1846" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1846" s="3"/>
+      <c r="D1846" s="6"/>
+      <c r="E1846" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1846" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1846" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1846" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1847" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1847" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1847" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1847" s="3"/>
+      <c r="D1847" s="6"/>
+      <c r="E1847" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1847" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1847" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1847" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1848" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1848" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1848" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1848" s="3"/>
+      <c r="D1848" s="6"/>
+      <c r="E1848" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1848" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1848" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1848" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1849" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1849" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1849" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1849" s="3"/>
+      <c r="D1849" s="6"/>
+      <c r="E1849" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1849" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1849" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1849" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1850" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1850" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1850" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1850" s="3"/>
+      <c r="D1850" s="6"/>
+      <c r="E1850" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1850" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1850" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1850" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1851" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1851" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1851" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1851" s="3"/>
+      <c r="D1851" s="6"/>
+      <c r="E1851" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1851" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1851" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1851" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1852" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1852" s="2">
+        <v>44019</v>
+      </c>
+      <c r="B1852" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1852" s="3"/>
+      <c r="D1852" s="4"/>
+      <c r="E1852" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1852" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1852" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1852" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-chartas and euskadi hospitalized 2020.07.11
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBDDBDDC-1A56-4331-8213-2B5AA00F8B7B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F58A5A4-6C90-49B4-AB7D-32F96996C5B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9924" yWindow="3552" windowWidth="22560" windowHeight="7308" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9936" yWindow="3564" windowWidth="22560" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7492" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7652" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1872"/>
+  <dimension ref="A1:J1912"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -45704,6 +45704,928 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1873" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1873" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1873" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1873" s="3">
+        <v>4</v>
+      </c>
+      <c r="D1873" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1873" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1873" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1873" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1873" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1874" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1874" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1874" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1874" s="3">
+        <v>5</v>
+      </c>
+      <c r="D1874" s="4"/>
+      <c r="E1874" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1874" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1874" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1874" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1875" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1875" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1875" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1875" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1875" s="3"/>
+      <c r="E1875" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1875" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1875" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1875" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1876" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1876" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1876" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1876" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1876" s="3"/>
+      <c r="E1876" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1876" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1876" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1876" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1877" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1877" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1877" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1877" s="3"/>
+      <c r="D1877" s="4"/>
+      <c r="E1877" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1877" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1877" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1877" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1878" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1878" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1878" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1878" s="3"/>
+      <c r="D1878" s="3"/>
+      <c r="E1878" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1878" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1878" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1878" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1879" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1879" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1879" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1879" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1879" s="4"/>
+      <c r="E1879" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1879" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1879" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1879" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1880" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1880" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1880" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1880" s="3">
+        <v>8</v>
+      </c>
+      <c r="D1880" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1880" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1880" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1880" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1880" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1881" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1881" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1881" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1881" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1881" s="4"/>
+      <c r="E1881" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1881" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1881" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1881" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1882" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1882" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1882" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1882" s="4"/>
+      <c r="D1882" s="4"/>
+      <c r="E1882" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1882" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1882" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1882" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1883" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1883" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1883" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1883" s="3"/>
+      <c r="D1883" s="3"/>
+      <c r="E1883" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1883" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1883" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1883" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1884" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1884" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1884" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1884" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1884" s="3"/>
+      <c r="E1884" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1884" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1884" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1884" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1885" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1885" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1885" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1885" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1885" s="4"/>
+      <c r="E1885" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1885" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1885" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1885" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1886" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1886" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1886" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1886" s="3"/>
+      <c r="D1886" s="6"/>
+      <c r="E1886" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1886" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1886" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1886" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1887" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1887" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1887" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1887" s="3"/>
+      <c r="D1887" s="6"/>
+      <c r="E1887" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1887" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1887" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1887" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1888" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1888" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1888" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1888" s="3"/>
+      <c r="D1888" s="6"/>
+      <c r="E1888" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1888" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1888" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1888" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1889" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1889" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1889" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1889" s="3"/>
+      <c r="D1889" s="6"/>
+      <c r="E1889" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1889" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1889" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1889" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1890" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1890" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1890" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1890" s="3"/>
+      <c r="D1890" s="6"/>
+      <c r="E1890" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1890" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1890" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1890" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1891" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1891" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1891" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1891" s="3"/>
+      <c r="D1891" s="6"/>
+      <c r="E1891" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1891" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1891" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1891" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1892" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1892" s="2">
+        <v>44022</v>
+      </c>
+      <c r="B1892" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1892" s="3"/>
+      <c r="D1892" s="4"/>
+      <c r="E1892" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1892" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1892" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1892" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1893" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1893" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1893" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1893" s="3">
+        <v>10</v>
+      </c>
+      <c r="D1893" s="3"/>
+      <c r="E1893" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1893" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1893" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1893" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1894" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1894" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1894" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1894" s="3">
+        <v>15</v>
+      </c>
+      <c r="D1894" s="4"/>
+      <c r="E1894" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1894" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1894" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1894" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1895" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1895" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1895" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1895" s="3"/>
+      <c r="D1895" s="3"/>
+      <c r="E1895" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1895" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1895" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1895" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1896" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1896" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1896" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1896" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1896" s="3"/>
+      <c r="E1896" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1896" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1896" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1896" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1897" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1897" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1897" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1897" s="3"/>
+      <c r="D1897" s="4"/>
+      <c r="E1897" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1897" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1897" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1897" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1898" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1898" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1898" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1898" s="3"/>
+      <c r="D1898" s="3"/>
+      <c r="E1898" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1898" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1898" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1898" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1899" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1899" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1899" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1899" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1899" s="4"/>
+      <c r="E1899" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1899" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1899" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1899" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1900" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1900" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1900" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1900" s="3">
+        <v>12</v>
+      </c>
+      <c r="D1900" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1900" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1900" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1900" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1900" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1901" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1901" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1901" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1901" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1901" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1901" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1901" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1901" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1901" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1902" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1902" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1902" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1902" s="4"/>
+      <c r="D1902" s="4"/>
+      <c r="E1902" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1902" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1902" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1902" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1903" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1903" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1903" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1903" s="3"/>
+      <c r="D1903" s="3"/>
+      <c r="E1903" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1903" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1903" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1903" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1904" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1904" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1904" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1904" s="3"/>
+      <c r="D1904" s="3"/>
+      <c r="E1904" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1904" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1904" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1904" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1905" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1905" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1905" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1905" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1905" s="4"/>
+      <c r="E1905" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1905" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1905" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1905" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1906" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1906" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1906" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1906" s="3"/>
+      <c r="D1906" s="6"/>
+      <c r="E1906" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1906" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1906" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1906" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1907" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1907" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1907" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1907" s="3"/>
+      <c r="D1907" s="6"/>
+      <c r="E1907" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1907" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1907" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1907" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1908" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1908" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1908" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1908" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1908" s="6"/>
+      <c r="E1908" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1908" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1908" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1908" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1909" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1909" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1909" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1909" s="3"/>
+      <c r="D1909" s="6"/>
+      <c r="E1909" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1909" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1909" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1909" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1910" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1910" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1910" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1910" s="3"/>
+      <c r="D1910" s="6"/>
+      <c r="E1910" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1910" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1910" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1910" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1911" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1911" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1911" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1911" s="3"/>
+      <c r="D1911" s="6"/>
+      <c r="E1911" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1911" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1911" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1911" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1912" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1912" s="2">
+        <v>44025</v>
+      </c>
+      <c r="B1912" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1912" s="3"/>
+      <c r="D1912" s="4"/>
+      <c r="E1912" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1912" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1912" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1912" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-chartas and eus hosp 2020.07.13
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F58A5A4-6C90-49B4-AB7D-32F96996C5B6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A91934-AFAF-402F-A85A-4E578877629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9936" yWindow="3564" windowWidth="22560" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10392" yWindow="2124" windowWidth="22560" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7652" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7732" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -550,7 +550,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1912"/>
+  <dimension ref="A1:J1932"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -46626,6 +46626,468 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1913" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1913" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1913" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1913" s="3">
+        <v>15</v>
+      </c>
+      <c r="D1913" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1913" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1913" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1913" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1913" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1914" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1914" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1914" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1914" s="3">
+        <v>19</v>
+      </c>
+      <c r="D1914" s="4"/>
+      <c r="E1914" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1914" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1914" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1914" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1915" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1915" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1915" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1915" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1915" s="3"/>
+      <c r="E1915" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1915" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1915" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1915" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1916" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1916" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1916" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1916" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1916" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1916" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1916" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1916" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1916" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1917" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1917" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1917" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1917" s="3"/>
+      <c r="D1917" s="4"/>
+      <c r="E1917" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1917" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1917" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1917" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1918" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1918" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1918" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1918" s="3"/>
+      <c r="D1918" s="3"/>
+      <c r="E1918" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1918" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1918" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1918" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1919" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1919" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1919" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1919" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1919" s="4"/>
+      <c r="E1919" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1919" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1919" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1919" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1920" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1920" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1920" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1920" s="3">
+        <v>15</v>
+      </c>
+      <c r="D1920" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1920" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1920" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1920" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1920" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1921" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1921" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1921" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1921" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1921" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1921" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1921" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1921" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1921" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1922" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1922" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1922" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1922" s="4"/>
+      <c r="D1922" s="4"/>
+      <c r="E1922" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1922" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1922" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1922" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1923" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1923" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1923" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1923" s="3"/>
+      <c r="D1923" s="3"/>
+      <c r="E1923" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1923" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1923" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1923" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1924" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1924" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1924" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1924" s="3"/>
+      <c r="D1924" s="3"/>
+      <c r="E1924" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1924" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1924" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1924" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1925" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1925" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1925" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1925" s="3"/>
+      <c r="D1925" s="4"/>
+      <c r="E1925" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1925" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1925" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1925" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1926" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1926" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1926" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1926" s="3"/>
+      <c r="D1926" s="6"/>
+      <c r="E1926" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1926" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1926" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1926" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1927" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1927" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1927" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1927" s="3"/>
+      <c r="D1927" s="6"/>
+      <c r="E1927" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1927" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1927" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1927" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1928" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1928" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1928" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1928" s="3"/>
+      <c r="D1928" s="6"/>
+      <c r="E1928" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1928" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1928" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1928" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1929" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1929" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1929" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1929" s="3"/>
+      <c r="D1929" s="6"/>
+      <c r="E1929" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1929" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1929" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1929" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1930" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1930" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1930" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1930" s="3"/>
+      <c r="D1930" s="6"/>
+      <c r="E1930" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1930" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1930" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1930" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1931" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1931" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1931" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1931" s="3"/>
+      <c r="D1931" s="6"/>
+      <c r="E1931" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1931" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1931" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1931" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1932" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1932" s="2">
+        <v>44026</v>
+      </c>
+      <c r="B1932" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1932" s="3"/>
+      <c r="D1932" s="4"/>
+      <c r="E1932" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1932" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1932" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1932" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts and Euskadi hospitalized 2020.07.15
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmoyano\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90A91934-AFAF-402F-A85A-4E578877629D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10392" yWindow="2124" windowWidth="22560" windowHeight="6360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="9276"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$197</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7732" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7812" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -156,7 +155,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -549,8 +548,8 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J1932"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J1952"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -47088,6 +47087,474 @@
         <v>38</v>
       </c>
     </row>
+    <row r="1933" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1933" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1933" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C1933" s="3">
+        <v>16</v>
+      </c>
+      <c r="D1933" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1933" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1933" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1933" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1933" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1934" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1934" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1934" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1934" s="3">
+        <v>26</v>
+      </c>
+      <c r="D1934" s="4"/>
+      <c r="E1934" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1934" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1934" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1934" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1935" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1935" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1935" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1935" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1935" s="3"/>
+      <c r="E1935" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1935" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1935" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1935" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1936" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1936" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1936" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1936" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1936" s="3">
+        <v>1</v>
+      </c>
+      <c r="E1936" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1936" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1936" s="3">
+        <v>50297</v>
+      </c>
+      <c r="H1936" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1937" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1937" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1937" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1937" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1937" s="4"/>
+      <c r="E1937" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1937" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1937" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1937" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1938" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1938" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1938" s="3">
+        <v>2</v>
+      </c>
+      <c r="D1938" s="3"/>
+      <c r="E1938" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1938" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1938" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1938" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1939" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1939" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1939" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1939" s="4"/>
+      <c r="E1939" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1939" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1939" s="4">
+        <v>44013</v>
+      </c>
+      <c r="H1939" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1940" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1940" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1940" s="3">
+        <v>16</v>
+      </c>
+      <c r="D1940" s="3">
+        <v>2</v>
+      </c>
+      <c r="E1940" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1940" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1940" s="3">
+        <v>22048</v>
+      </c>
+      <c r="H1940" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1941" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1941" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1941" s="3">
+        <v>3</v>
+      </c>
+      <c r="D1941" s="4">
+        <v>1</v>
+      </c>
+      <c r="E1941" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1941" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1941" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1941" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1942" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1942" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1942" s="4"/>
+      <c r="D1942" s="4"/>
+      <c r="E1942" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1942" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1942" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1942" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1943" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1943" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1943" s="3"/>
+      <c r="D1943" s="3"/>
+      <c r="E1943" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1943" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1943" s="3">
+        <v>50067</v>
+      </c>
+      <c r="H1943" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1944" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1944" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C1944" s="3"/>
+      <c r="D1944" s="3"/>
+      <c r="E1944" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1944" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1944" s="3">
+        <v>44216</v>
+      </c>
+      <c r="H1944" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1945" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1945" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1945" s="3"/>
+      <c r="D1945" s="4"/>
+      <c r="E1945" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1945" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1945" s="4">
+        <v>50095</v>
+      </c>
+      <c r="H1945" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1946" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1946" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1946" s="3"/>
+      <c r="D1946" s="6"/>
+      <c r="E1946" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1946" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1946" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1946" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1947" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1947" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1947" s="3"/>
+      <c r="D1947" s="6"/>
+      <c r="E1947" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1947" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1947" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1947" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1948" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1948" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1948" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1948" s="3"/>
+      <c r="D1948" s="6"/>
+      <c r="E1948" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1948" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1948" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1948" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1949" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1949" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1949" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1949" s="3">
+        <v>1</v>
+      </c>
+      <c r="D1949" s="6"/>
+      <c r="E1949" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1949" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1949" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1949" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1950" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1950" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1950" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1950" s="3"/>
+      <c r="D1950" s="6"/>
+      <c r="E1950" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1950" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1950" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1950" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1951" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1951" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1951" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1951" s="3"/>
+      <c r="D1951" s="6"/>
+      <c r="E1951" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F1951" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1951" s="4">
+        <v>22125</v>
+      </c>
+      <c r="H1951" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="1952" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1952" s="2">
+        <v>44027</v>
+      </c>
+      <c r="B1952" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1952" s="3"/>
+      <c r="D1952" s="4"/>
+      <c r="E1952" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="F1952" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="G1952" s="4">
+        <v>50297</v>
+      </c>
+      <c r="H1952" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.07.27
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clozanof\Downloads\CORONAVIRUS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Downloads\COVID\AOD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A48201C-9622-405E-A71D-F7CAA9F2D2F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685"/>
+    <workbookView xWindow="315" yWindow="390" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8452" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8532" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -545,11 +546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2112"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2086" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D2109" sqref="D2109"/>
+    <sheetView tabSelected="1" topLeftCell="A2120" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2132" sqref="B2132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -51299,6 +51300,472 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2113" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2113" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2113" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2113" s="1">
+        <v>90</v>
+      </c>
+      <c r="D2113" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2113" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2113" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2114" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2114" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2114" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2114" s="1">
+        <v>84</v>
+      </c>
+      <c r="D2114" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2114" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2114" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2115" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2115" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2115" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2115" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2115" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2115" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2116" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2116" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2116" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2116" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2116" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2116" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2116" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2117" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2117" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2117" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2117" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2117" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2117" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2117" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2118" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2118" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2118" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2118" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2118" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2118" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2118" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2119" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2119" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2119" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2119" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2119" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2119" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2119" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2119" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2120" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2120" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2120" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2120" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2120" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2120" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2120" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2120" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2120" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2121" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2121" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2121" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2121" s="1">
+        <v>15</v>
+      </c>
+      <c r="D2121" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2121" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2121" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2121" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2121" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2122" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2122" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2122" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2122" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2122" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2122" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2122" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2123" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2123" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2123" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2123" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2123" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2123" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2123" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2124" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2124" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2124" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2124" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2124" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2124" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2124" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2125" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2125" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2125" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2125" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2125" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2125" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2125" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2126" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2126" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2126" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2126" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2126" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2126" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2126" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2126" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2126" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2127" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2127" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2127" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2127" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2127" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2127" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2127" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2128" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2128" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2128" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2128" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2128" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2128" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2128" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2128" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2129" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2129" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2129" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2129" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2129" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2129" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2129" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2129" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2130" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2130" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2130" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2130" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2130" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2130" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2130" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2131" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2131" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2131" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2131" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2131" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2131" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2131" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2132" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2132" s="2">
+        <v>44040</v>
+      </c>
+      <c r="B2132" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2132" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2132" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2132" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2132" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts and Euskadi municipalities 2020.07.29
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia\Desktop\coronavirus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1DA93B2-6FD9-4BF6-9DED-3145E6F3EACA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985F6187-5768-4D6F-B4BE-F39BBDEEE62E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10476" yWindow="1524" windowWidth="13860" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10164" yWindow="2484" windowWidth="13860" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8612" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8692" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,7 +547,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2152"/>
+  <dimension ref="A1:J2172"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
@@ -52227,6 +52227,475 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2153" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2153" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2153" s="1">
+        <v>92</v>
+      </c>
+      <c r="D2153" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2153" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2153" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2153" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2153" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2154" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2154" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2154" s="1">
+        <v>94</v>
+      </c>
+      <c r="D2154" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2154" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2154" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2154" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2154" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2155" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2155" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2155" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2155" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2155" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2155" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2155" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2155" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2156" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2156" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2156" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2156" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2156" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2156" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2157" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2157" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2157" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2157" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2157" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2157" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2157" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2158" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2158" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2158" s="1">
+        <v>26</v>
+      </c>
+      <c r="E2158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2158" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2158" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2158" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2159" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2159" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2159" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2159" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2159" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2159" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2159" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2160" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2160" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2160" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2160" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2160" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2160" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2160" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2160" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2161" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2161" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2161" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2161" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2161" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2161" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2162" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2162" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2162" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2162" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2162" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2162" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2163" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2163" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2163" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2163" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2163" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2163" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2163" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2164" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2164" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2164" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2164" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2164" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2165" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2165" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2165" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2165" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2165" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2165" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2165" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2166" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2166" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2166" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2166" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2166" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2166" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2166" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2166" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2167" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2167" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2167" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2167" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2168" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2168" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2168" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2168" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2168" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2169" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2169" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2169" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2169" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2169" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2169" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2170" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2170" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2170" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2170" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2170" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2170" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2171" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2171" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2171" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2171" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2171" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2171" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2172" s="2">
+        <v>44042</v>
+      </c>
+      <c r="B2172" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2172" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2172" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2172" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2172" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts. Atomatizes Aragon hospitalized and UCI, and Catalunya deaths 2020.08.02
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Downloads\COVID\AOD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{86DCF9D8-F262-44AD-BB65-4DC300CE7917}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8772" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8932" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -150,7 +149,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -546,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2192"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2232"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2177" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="H2172" sqref="H2172:H2192"/>
+    <sheetView tabSelected="1" topLeftCell="A2208" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2214" sqref="A2214:A2232"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -53164,6 +53163,950 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2193" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2193" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2193" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2193" s="1">
+        <v>110</v>
+      </c>
+      <c r="D2193" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2193" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2193" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2193" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2193" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2194" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2194" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2194" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2194" s="1">
+        <v>104</v>
+      </c>
+      <c r="D2194" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2194" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2194" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2194" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2194" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2195" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2195" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2195" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2195" s="1">
+        <v>29</v>
+      </c>
+      <c r="D2195" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2195" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2195" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2195" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2195" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2196" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2196" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2196" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2196" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2196" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2196" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2196" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2196" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2196" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2197" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2197" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2197" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2197" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2197" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2197" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2197" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2197" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2198" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2198" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2198" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2198" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2198" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2198" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2199" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2199" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2199" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2199" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2199" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2199" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2199" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2199" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2200" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2200" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2200" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2200" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2200" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2200" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2200" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2200" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2200" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2201" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2201" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2201" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2201" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2201" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2201" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2201" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2201" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2202" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2202" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2202" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2202" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2202" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2202" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2202" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2203" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2203" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2203" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2203" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2203" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2203" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2203" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2203" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2204" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2204" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2204" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2204" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2204" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2204" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2204" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2205" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2205" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2205" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2205" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2205" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2205" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2205" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2205" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2206" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2206" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2206" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2206" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2206" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2206" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2206" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2206" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2206" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2207" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2207" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2207" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2207" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2207" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2207" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2207" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2208" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2208" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2208" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2208" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2208" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2208" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2208" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2208" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2209" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2209" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2209" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2209" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2209" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2209" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2209" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2209" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2209" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2210" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2210" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2210" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2210" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2210" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2210" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2210" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2210" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2211" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2211" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2211" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2211" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2211" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2211" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2211" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2212" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2212" s="2">
+        <v>44044</v>
+      </c>
+      <c r="B2212" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2212" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2212" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2212" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2212" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2213" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2213" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2213" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2213" s="1">
+        <v>137</v>
+      </c>
+      <c r="D2213" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2213" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2213" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2213" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2213" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2214" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2214" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2214" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2214" s="1">
+        <v>135</v>
+      </c>
+      <c r="D2214" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2214" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2214" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2214" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2214" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2215" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2215" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2215" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2215" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2215" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2215" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2215" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2215" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2215" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2216" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2216" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2216" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2216" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2216" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2216" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2216" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2216" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2216" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2217" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2217" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2217" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2217" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2217" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2217" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2217" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2217" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2218" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2218" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2218" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2218" s="1">
+        <v>39</v>
+      </c>
+      <c r="E2218" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2218" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2218" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2218" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2219" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2219" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2219" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2219" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2219" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2219" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2219" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2219" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2220" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2220" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2220" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2220" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2220" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2220" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2220" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2220" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2220" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2221" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2221" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2221" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2221" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2221" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2221" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2221" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2221" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2221" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2222" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2222" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2222" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2222" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2222" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2222" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2222" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2223" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2223" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2223" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2223" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2223" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2223" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2223" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2223" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2224" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2224" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2224" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2224" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2224" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2224" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2224" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2224" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2225" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2225" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2225" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2225" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2225" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2225" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2225" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2225" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2226" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2226" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2226" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2226" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2226" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2226" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2226" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2226" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2226" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2227" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2227" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2227" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2227" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2227" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2227" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2227" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2228" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2228" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2228" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2228" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2228" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2228" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2228" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2228" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2229" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2229" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2229" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2229" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2229" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2229" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2229" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2229" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2229" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2230" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2230" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2230" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2230" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2230" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2230" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2230" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2230" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2231" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2231" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2231" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2231" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2231" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2231" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2231" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2231" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2232" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2232" s="2">
+        <v>44046</v>
+      </c>
+      <c r="B2232" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2232" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2232" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2232" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2232" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts and Euskadi 2020.08.03
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8932" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9012" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -546,10 +546,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2232"/>
+  <dimension ref="A1:J2252"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2208" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2214" sqref="A2214:A2232"/>
+    <sheetView tabSelected="1" topLeftCell="A2228" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2234" sqref="A2234:A2252"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54107,6 +54107,484 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2233" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2233" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2233" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2233" s="1">
+        <v>133</v>
+      </c>
+      <c r="D2233" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2233" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2233" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2233" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2233" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2234" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2234" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2234" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2234" s="1">
+        <v>141</v>
+      </c>
+      <c r="D2234" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2234" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2234" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2234" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2234" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2235" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2235" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2235" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2235" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2235" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2235" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2235" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2235" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2235" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2236" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2236" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2236" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2236" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2236" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2236" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2236" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2236" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2236" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2237" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2237" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2237" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2237" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2237" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2237" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2237" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2237" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2238" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2238" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2238" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2238" s="1">
+        <v>39</v>
+      </c>
+      <c r="E2238" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2238" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2238" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2238" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2239" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2239" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2239" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2239" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2239" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2239" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2239" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2239" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2240" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2240" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2240" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2240" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2240" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2240" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2240" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2240" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2240" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2241" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2241" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2241" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2241" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2241" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2241" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2241" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2241" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2242" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2242" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2242" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2242" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2242" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2242" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2243" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2243" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2243" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2243" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2243" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2243" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2243" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2243" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2244" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2244" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2244" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2244" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2244" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2244" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2244" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2244" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2245" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2245" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2245" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2245" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2245" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2245" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2245" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2245" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2246" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2246" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2246" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2246" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2246" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2246" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2246" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2246" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2246" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2247" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2247" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2247" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2247" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2247" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2247" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2247" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2248" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2248" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2248" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2248" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2248" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2248" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2248" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2248" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2249" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2249" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2249" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2249" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2249" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2249" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2249" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2249" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2249" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2250" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2250" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2250" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2250" s="1">
+        <v>20</v>
+      </c>
+      <c r="E2250" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2250" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2250" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2250" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2251" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2251" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2251" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2251" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2251" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2251" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2251" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2251" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2252" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2252" s="2">
+        <v>44047</v>
+      </c>
+      <c r="B2252" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2252" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2252" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2252" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2252" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2252" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.08.04
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Downloads\COVID\AOD\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E47B193-6D00-4EE3-A1DD-5572A18A9F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9012" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9092" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -545,11 +546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2252"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2272"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2228" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2234" sqref="A2234:A2252"/>
+    <sheetView tabSelected="1" topLeftCell="A2257" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2272" sqref="A2272"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -54585,6 +54586,478 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2253" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2253" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2253" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2253" s="1">
+        <v>131</v>
+      </c>
+      <c r="D2253" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2253" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2253" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2253" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2253" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2254" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2254" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2254" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2254" s="1">
+        <v>141</v>
+      </c>
+      <c r="D2254" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2254" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2254" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2254" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2254" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2255" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2255" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2255" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2255" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2255" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2255" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2255" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2255" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2255" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2256" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2256" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2256" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2256" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2256" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2256" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2256" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2256" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2256" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2257" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2257" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2257" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2257" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2257" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2257" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2257" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2257" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2258" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2258" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2258" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2258" s="1">
+        <v>37</v>
+      </c>
+      <c r="E2258" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2258" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2258" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2258" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2259" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2259" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2259" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2259" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2259" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2259" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2259" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2259" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2260" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2260" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2260" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2260" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2260" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2260" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2260" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2260" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2260" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2261" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2261" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2261" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2261" s="1">
+        <v>26</v>
+      </c>
+      <c r="D2261" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2261" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2261" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2261" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2261" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2262" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2262" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2262" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2262" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2262" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2262" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2262" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2263" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2263" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2263" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2263" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2263" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2263" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2263" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2263" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2264" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2264" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2264" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2264" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2264" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2264" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2264" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2265" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2265" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2265" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2265" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2265" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2265" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2265" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2265" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2266" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2266" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2266" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2266" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2266" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2266" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2266" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2266" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2266" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2267" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2267" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2267" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2267" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2267" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2267" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2267" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2268" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2268" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2268" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2268" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2268" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2268" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2268" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2268" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2269" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2269" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2269" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2269" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2269" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2269" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2269" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2269" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2269" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2270" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2270" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2270" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2270" s="1">
+        <v>26</v>
+      </c>
+      <c r="E2270" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2270" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2270" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2270" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2271" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2271" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2271" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2271" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2271" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2271" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2271" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2272" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2272" s="2">
+        <v>44048</v>
+      </c>
+      <c r="B2272" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2272" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2272" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2272" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2272" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2272" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain province data-charts 2020.08.05
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pc\Downloads\COVID\AOD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E47B193-6D00-4EE3-A1DD-5572A18A9F57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEE4D4F-A1CB-452A-83EA-857AF03BC748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="600" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9092" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9172" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2272"/>
+  <dimension ref="A1:J2292"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2257" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2272" sqref="A2272"/>
+    <sheetView tabSelected="1" topLeftCell="A2265" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2274" sqref="A2274:A2292"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55058,6 +55058,484 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2273" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2273" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2273" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2273" s="1">
+        <v>136</v>
+      </c>
+      <c r="D2273" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2273" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2273" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2273" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2273" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2274" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2274" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2274" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2274" s="1">
+        <v>147</v>
+      </c>
+      <c r="D2274" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2274" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2274" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2274" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2274" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2275" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2275" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2275" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2275" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2275" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2275" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2275" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2275" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2275" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2276" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2276" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2276" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2276" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2276" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2276" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2276" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2276" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2276" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2277" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2277" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2277" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2277" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2277" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2277" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2277" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2277" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2278" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2278" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2278" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2278" s="1">
+        <v>38</v>
+      </c>
+      <c r="E2278" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2278" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2278" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2278" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2279" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2279" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2279" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2279" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2279" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2279" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2279" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2279" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2280" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2280" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2280" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2280" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2280" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2280" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2280" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2280" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2280" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2281" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2281" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2281" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2281" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2281" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2281" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2281" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2281" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2281" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2282" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2282" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2282" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2282" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2282" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2282" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2282" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2283" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2283" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2283" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2283" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2283" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2283" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2283" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2283" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2284" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2284" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2284" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2284" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2284" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2284" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2284" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2284" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2285" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2285" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2285" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2285" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2285" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2285" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2285" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2285" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2286" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2286" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2286" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2286" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2286" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2286" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2286" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2286" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2286" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2287" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2287" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2287" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2287" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2287" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2287" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2287" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2288" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2288" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2288" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2288" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2288" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2288" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2288" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2288" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2289" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2289" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2289" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2289" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2289" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2289" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2289" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2289" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2289" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2290" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2290" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2290" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2290" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2290" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2290" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2290" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2290" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2291" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2291" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2291" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2291" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2291" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2291" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2291" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2291" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2292" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2292" s="2">
+        <v>44049</v>
+      </c>
+      <c r="B2292" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2292" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2292" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2292" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2292" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2292" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain IT FR data-charts
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CEE4D4F-A1CB-452A-83EA-857AF03BC748}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F734A1-54F6-44D4-9EC0-19F86069B164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="600" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9172" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9252" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2292"/>
+  <dimension ref="A1:J2312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2265" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2274" sqref="A2274:A2292"/>
+    <sheetView tabSelected="1" topLeftCell="A2285" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2294" sqref="A2294:A2312"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -55536,6 +55536,484 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2293" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2293" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2293" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2293" s="1">
+        <v>136</v>
+      </c>
+      <c r="D2293" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2293" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2293" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2293" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2293" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2294" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2294" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2294" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2294" s="1">
+        <v>138</v>
+      </c>
+      <c r="D2294" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2294" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2294" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2294" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2294" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2295" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2295" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2295" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2295" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2295" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2295" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2295" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2295" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2295" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2296" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2296" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2296" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2296" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2296" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2296" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2296" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2296" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2296" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2297" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2297" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2297" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2297" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2297" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2297" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2297" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2297" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2297" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2298" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2298" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2298" s="1">
+        <v>36</v>
+      </c>
+      <c r="E2298" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2298" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2298" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2298" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2299" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2299" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2299" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2299" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2299" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2299" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2299" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2300" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2300" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2300" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2300" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2300" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2300" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2300" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2300" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2301" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2301" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2301" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2301" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2301" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2301" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2301" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2301" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2302" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2302" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2302" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2302" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2302" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2302" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2303" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2303" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2303" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2303" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2303" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2303" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2303" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2304" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2304" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2304" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2304" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2304" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2304" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2304" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2305" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2305" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2305" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2305" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2305" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2305" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2305" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2305" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2306" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2306" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2306" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2306" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2306" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2306" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2306" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2306" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2306" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2307" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2307" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2307" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2307" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2307" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2307" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2307" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2308" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2308" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2308" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2308" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2308" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2308" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2308" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2308" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2309" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2309" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2309" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2309" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2309" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2309" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2309" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2309" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2309" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2310" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2310" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2310" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2310" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2310" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2310" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2310" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2310" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2311" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2311" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2311" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2311" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2311" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2311" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2311" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2312" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2312" s="2">
+        <v>44050</v>
+      </c>
+      <c r="B2312" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2312" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2312" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2312" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2312" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.08.07
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2F734A1-54F6-44D4-9EC0-19F86069B164}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D2B4C5-A93E-4AB9-A5D9-B1C9FAB068B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9252" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9332" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2312"/>
+  <dimension ref="A1:J2332"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2285" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2294" sqref="A2294:A2312"/>
+    <sheetView tabSelected="1" topLeftCell="A2317" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2314" sqref="A2314:A2332"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56014,6 +56014,481 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2313" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2313" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2313" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2313" s="1">
+        <v>133</v>
+      </c>
+      <c r="D2313" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2313" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2313" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2313" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2313" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2314" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2314" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2314" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2314" s="1">
+        <v>147</v>
+      </c>
+      <c r="D2314" s="1">
+        <v>14</v>
+      </c>
+      <c r="E2314" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2314" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2314" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2314" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2315" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2315" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2315" s="1">
+        <v>33</v>
+      </c>
+      <c r="D2315" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2315" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2315" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2315" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2315" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2316" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2316" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2316" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2316" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2316" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2316" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2316" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2316" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2316" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2317" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2317" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2317" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2317" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2317" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2317" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2317" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2317" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2318" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2318" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2318" s="1">
+        <v>34</v>
+      </c>
+      <c r="E2318" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2318" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2318" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2318" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2319" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2319" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2319" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2319" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2319" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2319" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2319" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2319" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2320" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2320" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2320" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2320" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2320" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2320" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2320" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2320" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2320" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2321" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2321" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2321" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2321" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2321" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2321" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2321" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2321" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2321" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2322" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2322" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2322" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2322" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2322" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2322" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2322" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2323" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2323" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2323" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2323" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2323" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2323" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2323" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2323" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2324" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2324" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2324" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2324" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2324" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2324" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2324" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2324" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2325" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2325" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2325" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2325" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2325" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2325" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2325" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2325" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2326" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2326" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2326" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2326" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2326" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2326" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2326" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2326" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2326" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2327" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2327" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2327" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2327" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2327" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2327" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2327" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2328" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2328" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2328" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2328" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2328" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2328" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2328" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2328" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2329" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2329" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2329" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2329" s="1">
+        <v>13</v>
+      </c>
+      <c r="D2329" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2329" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2329" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2329" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2329" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2330" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2330" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2330" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2330" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2330" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2330" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2330" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2330" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2331" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2331" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2331" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2331" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2331" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2331" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2331" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2332" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2332" s="2">
+        <v>44051</v>
+      </c>
+      <c r="B2332" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2332" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2332" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2332" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2332" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.08.09. Move cases to PCR+ in CyL. Fixed source URL
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0D2B4C5-A93E-4AB9-A5D9-B1C9FAB068B3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7983C532-98DA-4B12-8551-FFF0777C5672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9332" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9412" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2332"/>
+  <dimension ref="A1:J2352"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2317" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2314" sqref="A2314:A2332"/>
+    <sheetView tabSelected="1" topLeftCell="A2325" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2334" sqref="A2334:A2352"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56489,6 +56489,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2333" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2333" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2333" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2333" s="1">
+        <v>132</v>
+      </c>
+      <c r="D2333" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2333" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2333" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2333" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2333" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2334" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2334" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2334" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2334" s="1">
+        <v>161</v>
+      </c>
+      <c r="D2334" s="1">
+        <v>14</v>
+      </c>
+      <c r="E2334" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2334" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2334" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2334" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2335" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2335" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2335" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2335" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2335" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2335" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2335" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2335" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2335" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2336" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2336" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2336" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2336" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2336" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2336" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2336" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2336" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2336" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2337" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2337" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2337" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2337" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2337" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2337" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2337" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2337" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2337" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2338" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2338" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2338" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2338" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2338" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2338" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2338" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2338" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2338" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2339" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2339" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2339" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2339" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2339" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2339" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2339" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2339" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2340" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2340" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2340" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2340" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2340" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2340" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2340" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2340" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2340" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2341" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2341" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2341" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2341" s="1">
+        <v>29</v>
+      </c>
+      <c r="D2341" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2341" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2341" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2341" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2341" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2342" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2342" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2342" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2342" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2342" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2342" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2342" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2343" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2343" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2343" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2343" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2343" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2343" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2343" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2343" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2344" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2344" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2344" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2344" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2344" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2344" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2344" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2344" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2345" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2345" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2345" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2345" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2345" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2345" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2345" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2345" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2346" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2346" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2346" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2346" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2346" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2346" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2346" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2346" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2346" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2347" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2347" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2347" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2347" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2347" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2347" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2347" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2348" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2348" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2348" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2348" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2348" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2348" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2348" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2348" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2349" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2349" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2349" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2349" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2349" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2349" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2349" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2349" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2349" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2350" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2350" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2350" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2350" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2350" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2350" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2350" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2350" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2351" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2351" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2351" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2351" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2351" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2351" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2351" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2351" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2352" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2352" s="2">
+        <v>44052</v>
+      </c>
+      <c r="B2352" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2352" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2352" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2352" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2352" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.08.09 second part: Madrid, Aragón
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7983C532-98DA-4B12-8551-FFF0777C5672}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95491C32-4C09-43FD-B308-6C7A0A0DC395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9412" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9492" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2352"/>
+  <dimension ref="A1:J2372"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2325" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2334" sqref="A2334:A2352"/>
+    <sheetView tabSelected="1" topLeftCell="A2357" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2354" sqref="A2354:A2372"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -56970,6 +56970,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2353" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2353" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2353" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2353" s="1">
+        <v>148</v>
+      </c>
+      <c r="D2353" s="1">
+        <v>16</v>
+      </c>
+      <c r="E2353" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2353" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2353" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2353" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2354" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2354" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2354" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2354" s="1">
+        <v>156</v>
+      </c>
+      <c r="D2354" s="1">
+        <v>14</v>
+      </c>
+      <c r="E2354" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2354" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2354" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2354" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2355" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2355" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2355" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2355" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2355" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2355" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2355" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2355" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2355" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2356" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2356" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2356" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2356" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2356" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2356" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2356" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2356" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2356" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2357" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2357" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2357" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2357" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2357" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2357" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2357" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2357" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2357" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2358" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2358" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2358" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2358" s="1">
+        <v>38</v>
+      </c>
+      <c r="D2358" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2358" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2358" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2358" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2358" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2359" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2359" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2359" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2359" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2359" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2359" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2359" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2359" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2360" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2360" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2360" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2360" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2360" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2360" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2360" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2360" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2360" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2361" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2361" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2361" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2361" s="1">
+        <v>30</v>
+      </c>
+      <c r="D2361" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2361" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2361" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2361" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2361" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2362" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2362" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2362" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2362" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2362" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2362" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2362" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2363" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2363" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2363" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2363" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2363" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2363" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2363" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2363" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2364" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2364" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2364" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2364" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2364" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2364" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2364" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2364" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2365" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2365" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2365" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2365" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2365" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2365" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2365" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2365" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2366" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2366" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2366" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2366" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2366" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2366" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2366" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2366" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2366" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2367" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2367" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2367" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2367" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2367" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2367" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2367" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2368" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2368" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2368" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2368" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2368" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2368" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2368" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2368" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2369" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2369" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2369" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2369" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2369" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2369" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2369" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2369" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2369" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2370" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2370" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2370" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2370" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2370" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2370" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2370" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2370" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2371" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2371" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2371" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2371" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2371" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2371" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2371" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2371" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2372" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2372" s="2">
+        <v>44053</v>
+      </c>
+      <c r="B2372" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2372" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2372" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2372" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2372" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces. new formula for average daile deaths
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{95491C32-4C09-43FD-B308-6C7A0A0DC395}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CE4C94-E2AF-4DF6-BFE2-8737B48815BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9492" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9572" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2372"/>
+  <dimension ref="A1:J2392"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2357" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2354" sqref="A2354:A2372"/>
+    <sheetView tabSelected="1" topLeftCell="A2383" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2374" sqref="A2374:A2392"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57451,6 +57451,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2373" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2373" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2373" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2373" s="1">
+        <v>153</v>
+      </c>
+      <c r="D2373" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2373" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2373" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2373" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2373" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2374" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2374" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2374" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2374" s="1">
+        <v>161</v>
+      </c>
+      <c r="D2374" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2374" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2374" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2374" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2374" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2375" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2375" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2375" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2375" s="1">
+        <v>36</v>
+      </c>
+      <c r="D2375" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2375" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2375" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2375" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2375" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2376" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2376" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2376" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2376" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2376" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2376" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2376" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2376" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2376" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2377" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2377" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2377" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2377" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2377" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2377" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2377" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2377" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2377" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2378" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2378" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2378" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2378" s="1">
+        <v>36</v>
+      </c>
+      <c r="D2378" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2378" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2378" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2378" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2378" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2379" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2379" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2379" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2379" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2379" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2379" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2379" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2379" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2380" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2380" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2380" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2380" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2380" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2380" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2380" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2380" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2380" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2381" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2381" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2381" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2381" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2381" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2381" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2381" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2381" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2381" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2382" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2382" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2382" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2382" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2382" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2382" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2382" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2383" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2383" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2383" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2383" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2383" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2383" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2383" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2383" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2384" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2384" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2384" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2384" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2384" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2384" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2384" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2384" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2385" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2385" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2385" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2385" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2385" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2385" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2385" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2385" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2386" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2386" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2386" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2386" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2386" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2386" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2386" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2386" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2386" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2387" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2387" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2387" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2387" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2387" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2387" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2387" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2388" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2388" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2388" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2388" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2388" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2388" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2388" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2388" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2389" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2389" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2389" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2389" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2389" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2389" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2389" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2389" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2389" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2390" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2390" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2390" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2390" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2390" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2390" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2390" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2390" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2391" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2391" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2391" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2391" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2391" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2391" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2391" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2391" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2392" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2392" s="2">
+        <v>44054</v>
+      </c>
+      <c r="B2392" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2392" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2392" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2392" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2392" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts. Add PCR+ to Baleares 2020.08.11
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8CE4C94-E2AF-4DF6-BFE2-8737B48815BD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9572" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9652" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -150,7 +149,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -546,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2392"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2412"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2383" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2374" sqref="A2374:A2392"/>
+    <sheetView tabSelected="1" topLeftCell="A2384" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2394" sqref="A2394:A2412"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -57932,6 +57931,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2393" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2393" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2393" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2393" s="1">
+        <v>157</v>
+      </c>
+      <c r="D2393" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2393" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2393" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2393" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2393" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2394" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2394" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2394" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2394" s="1">
+        <v>155</v>
+      </c>
+      <c r="D2394" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2394" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2394" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2394" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2394" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2395" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2395" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2395" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2395" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2395" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2395" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2395" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2395" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2395" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2396" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2396" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2396" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2396" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2396" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2396" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2396" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2396" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2396" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2397" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2397" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2397" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2397" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2397" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2397" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2397" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2397" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2397" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2398" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2398" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2398" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2398" s="1">
+        <v>38</v>
+      </c>
+      <c r="D2398" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2398" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2398" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2398" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2398" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2399" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2399" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2399" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2399" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2399" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2399" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2399" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2399" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2400" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2400" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2400" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2400" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2400" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2400" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2400" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2400" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2400" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2401" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2401" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2401" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2401" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2401" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2401" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2401" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2401" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2401" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2402" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2402" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2402" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2402" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2402" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2402" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2402" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2403" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2403" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2403" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2403" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2403" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2403" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2403" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2403" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2404" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2404" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2404" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2404" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2404" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2404" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2404" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2404" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2405" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2405" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2405" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2405" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2405" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2405" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2405" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2405" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2406" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2406" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2406" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2406" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2406" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2406" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2406" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2406" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2406" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2407" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2407" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2407" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2407" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2407" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2407" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2407" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2408" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2408" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2408" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2408" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2408" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2408" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2408" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2408" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2409" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2409" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2409" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2409" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2409" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2409" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2409" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2409" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2409" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2410" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2410" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2410" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2410" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2410" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2410" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2410" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2410" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2411" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2411" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2411" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2411" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2411" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2411" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2411" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2411" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2412" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2412" s="2">
+        <v>44055</v>
+      </c>
+      <c r="B2412" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2412" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2412" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2412" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2412" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces II 2020.08.12
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58A0AFF-A21B-4FEF-920A-AB132C33311A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9652" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9732" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -545,11 +546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2412"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2432"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2384" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2394" sqref="A2394:A2412"/>
+    <sheetView tabSelected="1" topLeftCell="A2399" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2414" sqref="A2414:A2432"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58412,6 +58413,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2413" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2413" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2413" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2413" s="1">
+        <v>155</v>
+      </c>
+      <c r="D2413" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2413" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2413" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2413" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2413" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2414" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2414" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2414" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2414" s="1">
+        <v>156</v>
+      </c>
+      <c r="D2414" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2414" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2414" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2414" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2414" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2415" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2415" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2415" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2415" s="1">
+        <v>41</v>
+      </c>
+      <c r="D2415" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2415" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2415" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2415" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2415" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2416" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2416" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2416" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2416" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2416" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2416" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2416" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2416" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2416" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2417" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2417" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2417" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2417" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2417" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2417" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2417" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2417" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2417" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2418" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2418" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2418" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2418" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2418" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2418" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2418" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2418" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2418" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2419" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2419" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2419" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2419" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2419" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2419" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2419" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2419" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2420" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2420" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2420" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2420" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2420" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2420" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2420" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2420" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2420" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2421" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2421" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2421" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2421" s="1">
+        <v>29</v>
+      </c>
+      <c r="D2421" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2421" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2421" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2421" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2421" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2422" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2422" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2422" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2422" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2422" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2422" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2422" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2423" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2423" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2423" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2423" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2423" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2423" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2423" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2423" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2424" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2424" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2424" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2424" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2424" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2424" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2424" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2424" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2425" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2425" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2425" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2425" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2425" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2425" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2425" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2425" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2426" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2426" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2426" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2426" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2426" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2426" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2426" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2426" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2426" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2427" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2427" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2427" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2427" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2427" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2427" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2427" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2428" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2428" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2428" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2428" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2428" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2428" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2428" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2428" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2429" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2429" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2429" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2429" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2429" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2429" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2429" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2429" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2429" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2430" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2430" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2430" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2430" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2430" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2430" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2430" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2430" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2431" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2431" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2431" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2431" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2431" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2431" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2431" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2431" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2432" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2432" s="2">
+        <v>44056</v>
+      </c>
+      <c r="B2432" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2432" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2432" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2432" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2432" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.08.14
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E58A0AFF-A21B-4FEF-920A-AB132C33311A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F66550-79E0-4D7E-A0E3-C6D600A72157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9732" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9892" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2432"/>
+  <dimension ref="A1:J2472"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2399" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2414" sqref="A2414:A2432"/>
+    <sheetView tabSelected="1" topLeftCell="A2445" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2454" sqref="A2454:A2472"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -58894,6 +58894,962 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2433" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2433" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2433" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2433" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2433" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2433" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2433" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2433" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2433" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2434" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2434" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2434" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2434" s="1">
+        <v>158</v>
+      </c>
+      <c r="D2434" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2434" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2434" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2434" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2434" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2435" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2435" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2435" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2435" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2435" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2435" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2435" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2435" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2435" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2436" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2436" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2436" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2436" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2436" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2436" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2436" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2436" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2436" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2437" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2437" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2437" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2437" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2437" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2437" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2437" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2437" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2437" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2438" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2438" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2438" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2438" s="1">
+        <v>42</v>
+      </c>
+      <c r="D2438" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2438" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2438" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2438" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2438" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2439" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2439" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2439" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2439" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2439" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2439" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2439" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2439" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2440" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2440" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2440" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2440" s="1">
+        <v>30</v>
+      </c>
+      <c r="D2440" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2440" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2440" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2440" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2440" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2441" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2441" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2441" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2441" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2441" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2441" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2441" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2441" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2441" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2442" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2442" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2442" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2442" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2442" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2442" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2442" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2443" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2443" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2443" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2443" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2443" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2443" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2443" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2443" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2444" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2444" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2444" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2444" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2444" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2444" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2444" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2444" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2445" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2445" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2445" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2445" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2445" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2445" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2445" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2445" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2446" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2446" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2446" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2446" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2446" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2446" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2446" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2446" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2446" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2447" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2447" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2447" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2447" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2447" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2447" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2447" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2448" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2448" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2448" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2448" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2448" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2448" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2448" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2448" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2449" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2449" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2449" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2449" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2449" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2449" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2449" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2449" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2449" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2450" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2450" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2450" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2450" s="1">
+        <v>26</v>
+      </c>
+      <c r="E2450" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2450" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2450" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2450" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2451" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2451" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2451" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2451" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2451" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2451" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2451" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2452" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2452" s="2">
+        <v>44057</v>
+      </c>
+      <c r="B2452" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2452" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2452" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2452" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2452" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2453" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2453" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2453" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2453" s="1">
+        <v>143</v>
+      </c>
+      <c r="D2453" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2453" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2453" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2453" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2453" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2454" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2454" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2454" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2454" s="1">
+        <v>158</v>
+      </c>
+      <c r="D2454" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2454" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2454" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2454" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2454" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2455" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2455" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2455" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2455" s="1">
+        <v>36</v>
+      </c>
+      <c r="D2455" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2455" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2455" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2455" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2455" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2456" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2456" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2456" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2456" s="1">
+        <v>13</v>
+      </c>
+      <c r="D2456" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2456" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2456" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2456" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2456" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2457" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2457" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2457" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2457" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2457" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2457" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2457" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2457" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2457" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2458" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2458" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2458" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2458" s="1">
+        <v>38</v>
+      </c>
+      <c r="D2458" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2458" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2458" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2458" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2458" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2459" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2459" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2459" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2459" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2459" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2459" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2459" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2459" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2460" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2460" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2460" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2460" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2460" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2460" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2460" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2460" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2460" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2461" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2461" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2461" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2461" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2461" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2461" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2461" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2461" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2461" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2462" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2462" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2462" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2462" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2462" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2462" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2462" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2463" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2463" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2463" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2463" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2463" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2463" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2463" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2463" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2464" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2464" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2464" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2464" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2464" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2464" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2464" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2464" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2465" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2465" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2465" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2465" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2465" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2465" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2465" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2465" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2466" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2466" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2466" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2466" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2466" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2466" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2466" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2466" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2466" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2467" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2467" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2467" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2467" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2467" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2467" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2467" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2468" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2468" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2468" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2468" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2468" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2468" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2468" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2468" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2469" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2469" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2469" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2469" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2469" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2469" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2469" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2469" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2469" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2470" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2470" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2470" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2470" s="1">
+        <v>28</v>
+      </c>
+      <c r="E2470" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2470" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2470" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2470" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2471" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2471" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2471" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2471" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2471" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2471" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2471" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2472" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2472" s="2">
+        <v>44058</v>
+      </c>
+      <c r="B2472" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2472" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2472" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2472" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2472" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts. Add hospitalized Andalucia data 2020.08.15
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3F66550-79E0-4D7E-A0E3-C6D600A72157}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7FF1CF-C910-43D6-B697-588748077EF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9892" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9972" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2472"/>
+  <dimension ref="A1:J2492"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2445" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2454" sqref="A2454:A2472"/>
+    <sheetView tabSelected="1" topLeftCell="A2477" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C2490" sqref="C2490"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -59850,6 +59850,484 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2473" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2473" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2473" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2473" s="1">
+        <v>145</v>
+      </c>
+      <c r="D2473" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2473" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2473" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2473" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2473" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2474" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2474" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2474" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2474" s="1">
+        <v>162</v>
+      </c>
+      <c r="D2474" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2474" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2474" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2474" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2474" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2475" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2475" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2475" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2475" s="1">
+        <v>41</v>
+      </c>
+      <c r="D2475" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2475" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2475" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2475" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2475" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2476" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2476" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2476" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2476" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2476" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2476" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2476" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2476" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2476" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2477" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2477" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2477" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2477" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2477" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2477" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2477" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2477" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2477" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2478" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2478" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2478" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2478" s="1">
+        <v>38</v>
+      </c>
+      <c r="D2478" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2478" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2478" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2478" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2478" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2479" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2479" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2479" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2479" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2479" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2479" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2479" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2479" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2480" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2480" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2480" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2480" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2480" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2480" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2480" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2480" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2480" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2481" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2481" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2481" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2481" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2481" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2481" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2481" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2481" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2481" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2482" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2482" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2482" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2482" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2482" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2482" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2482" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2483" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2483" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2483" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2483" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2483" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2483" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2483" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2483" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2484" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2484" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2484" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2484" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2484" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2484" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2484" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2484" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2485" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2485" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2485" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2485" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2485" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2485" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2485" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2485" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2486" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2486" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2486" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2486" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2486" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2486" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2486" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2486" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2486" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2487" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2487" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2487" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2487" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2487" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2487" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2487" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2488" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2488" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2488" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2488" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2488" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2488" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2488" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2488" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2489" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2489" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2489" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2489" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2489" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2489" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2489" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2489" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2489" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2490" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2490" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2490" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2490" s="1">
+        <v>27</v>
+      </c>
+      <c r="E2490" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2490" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2490" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2490" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2491" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2491" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2491" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2491" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2491" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2491" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2491" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2492" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2492" s="2">
+        <v>44059</v>
+      </c>
+      <c r="B2492" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2492" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2492" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2492" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2492" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.08.17
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clozanof\Downloads\CORONAVIRUS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA7FF1CF-C910-43D6-B697-588748077EF4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9972" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10052" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -150,7 +149,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -546,11 +545,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2492"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2512"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2477" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C2490" sqref="C2490"/>
+    <sheetView tabSelected="1" topLeftCell="A2491" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B2520" sqref="B2520"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60328,6 +60327,484 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2493" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2493" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2493" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2493" s="1">
+        <v>156</v>
+      </c>
+      <c r="D2493" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2493" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2493" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2493" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2493" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2494" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2494" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2494" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2494" s="1">
+        <v>161</v>
+      </c>
+      <c r="D2494" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2494" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2494" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2494" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2494" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2495" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2495" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2495" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2495" s="1">
+        <v>41</v>
+      </c>
+      <c r="D2495" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2495" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2495" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2495" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2495" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2496" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2496" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2496" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2496" s="1">
+        <v>15</v>
+      </c>
+      <c r="D2496" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2496" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2496" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2496" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2496" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2497" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2497" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2497" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2497" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2497" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2497" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2497" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2497" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2497" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2498" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2498" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2498" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2498" s="1">
+        <v>40</v>
+      </c>
+      <c r="D2498" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2498" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2498" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2498" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2498" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2499" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2499" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2499" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2499" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2499" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2499" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2499" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2499" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2500" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2500" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2500" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2500" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2500" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2500" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2500" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2500" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2500" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2501" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2501" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2501" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2501" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2501" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2501" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2501" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2501" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2501" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2502" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2502" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2502" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2502" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2502" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2502" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2502" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2503" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2503" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2503" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2503" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2503" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2503" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2503" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2503" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2504" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2504" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2504" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2504" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2504" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2504" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2504" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2504" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2505" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2505" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2505" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2505" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2505" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2505" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2505" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2506" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2506" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2506" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2506" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2506" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2506" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2506" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2506" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2506" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2507" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2507" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2507" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2507" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2507" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2507" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2507" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2508" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2508" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2508" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2508" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2508" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2508" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2508" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2508" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2509" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2509" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2509" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2509" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2509" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2509" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2509" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2509" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2509" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2510" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2510" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2510" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2510" s="1">
+        <v>26</v>
+      </c>
+      <c r="E2510" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2510" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2510" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2510" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2511" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2511" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2511" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2511" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2511" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2511" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2511" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2511" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2512" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2512" s="2">
+        <v>44060</v>
+      </c>
+      <c r="B2512" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2512" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2512" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2512" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2512" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update data-charts Spain provnes II 2020.08.17
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clozanof\Downloads\CORONAVIRUS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F463592C-65FA-42DE-8986-02E5284124F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10052" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10132" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -149,7 +150,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -545,11 +546,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2512"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2532"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2491" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B2520" sqref="B2520"/>
+    <sheetView tabSelected="1" topLeftCell="A2505" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2514" sqref="A2514:A2532"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -60805,6 +60806,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2513" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2513" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2513" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2513" s="1">
+        <v>153</v>
+      </c>
+      <c r="D2513" s="1">
+        <v>17</v>
+      </c>
+      <c r="E2513" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2513" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2513" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2513" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2514" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2514" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2514" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2514" s="1">
+        <v>161</v>
+      </c>
+      <c r="D2514" s="1">
+        <v>24</v>
+      </c>
+      <c r="E2514" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2514" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2514" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2514" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2515" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2515" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2515" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2515" s="1">
+        <v>42</v>
+      </c>
+      <c r="D2515" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2515" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2515" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2515" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2515" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2516" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2516" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2516" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2516" s="1">
+        <v>15</v>
+      </c>
+      <c r="D2516" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2516" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2516" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2516" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2516" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2517" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2517" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2517" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2517" s="1">
+        <v>18</v>
+      </c>
+      <c r="D2517" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2517" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2517" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2517" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2517" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2518" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2518" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2518" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2518" s="1">
+        <v>44</v>
+      </c>
+      <c r="D2518" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2518" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2518" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2518" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2518" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2519" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2519" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2519" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2519" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2519" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2519" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2519" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2519" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2520" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2520" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2520" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2520" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2520" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2520" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2520" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2520" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2520" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2521" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2521" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2521" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2521" s="1">
+        <v>30</v>
+      </c>
+      <c r="D2521" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2521" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2521" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2521" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2521" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2522" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2522" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2522" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2522" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2522" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2522" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2522" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2523" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2523" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2523" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2523" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2523" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2523" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2523" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2523" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2524" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2524" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2524" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2524" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2524" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2524" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2524" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2524" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2525" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2525" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2525" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2525" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2525" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2525" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2525" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2525" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2526" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2526" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2526" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2526" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2526" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2526" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2526" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2526" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2526" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2527" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2527" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2527" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2527" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2527" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2527" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2527" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2528" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2528" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2528" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2528" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2528" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2528" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2528" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2528" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2529" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2529" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2529" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2529" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2529" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2529" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2529" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2529" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2529" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2530" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2530" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2530" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2530" s="1">
+        <v>28</v>
+      </c>
+      <c r="E2530" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2530" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2530" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2530" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2531" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2531" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2531" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2531" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2531" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2531" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2531" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2531" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2532" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2532" s="2">
+        <v>44061</v>
+      </c>
+      <c r="B2532" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2532" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2532" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2532" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2532" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces and Euskadi data-charts. Create agregated data by CCAA and Spain
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F463592C-65FA-42DE-8986-02E5284124F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F48332-DF7E-41C8-9A21-ADE6B531B163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10132" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10212" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2532"/>
+  <dimension ref="A1:J2552"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2505" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2514" sqref="A2514:A2532"/>
+    <sheetView tabSelected="1" topLeftCell="A2528" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2534" sqref="A2534:A2552"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61287,6 +61287,484 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2533" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2533" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2533" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2533" s="1">
+        <v>141</v>
+      </c>
+      <c r="D2533" s="1">
+        <v>18</v>
+      </c>
+      <c r="E2533" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2533" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2533" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2533" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2534" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2534" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2534" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2534" s="1">
+        <v>158</v>
+      </c>
+      <c r="D2534" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2534" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2534" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2534" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2534" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2535" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2535" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2535" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2535" s="1">
+        <v>49</v>
+      </c>
+      <c r="D2535" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2535" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2535" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2535" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2535" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2536" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2536" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2536" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2536" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2536" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2536" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2536" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2536" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2536" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2537" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2537" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2537" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2537" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2537" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2537" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2537" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2537" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2537" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2538" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2538" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2538" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2538" s="1">
+        <v>38</v>
+      </c>
+      <c r="D2538" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2538" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2538" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2538" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2538" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2539" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2539" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2539" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2539" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2539" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2539" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2539" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2539" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2540" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2540" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2540" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2540" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2540" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2540" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2540" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2540" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2540" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2541" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2541" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2541" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2541" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2541" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2541" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2541" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2541" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2541" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2542" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2542" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2542" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2542" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2542" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2542" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2542" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2543" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2543" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2543" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2543" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2543" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2543" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2543" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2543" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2544" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2544" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2544" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2544" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2544" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2544" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2544" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2544" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2545" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2545" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2545" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2545" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2545" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2545" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2545" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2545" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2546" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2546" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2546" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2546" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2546" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2546" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2546" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2546" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2546" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2547" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2547" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2547" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2547" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2547" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2547" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2547" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2548" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2548" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2548" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2548" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2548" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2548" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2548" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2548" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2549" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2549" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2549" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2549" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2549" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2549" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2549" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2549" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2549" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2550" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2550" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2550" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2550" s="1">
+        <v>26</v>
+      </c>
+      <c r="E2550" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2550" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2550" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2550" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2551" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2551" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2551" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2551" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2551" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2551" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2551" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2552" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2552" s="2">
+        <v>44062</v>
+      </c>
+      <c r="B2552" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2552" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2552" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2552" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2552" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix death average and NA in aggregated CCAA. update Spain data-charts 2020.08.19
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68F48332-DF7E-41C8-9A21-ADE6B531B163}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512AA00-78E0-44E3-991D-773D229DD738}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10212" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10292" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2552"/>
+  <dimension ref="A1:J2572"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2528" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2534" sqref="A2534:A2552"/>
+    <sheetView tabSelected="1" topLeftCell="A2545" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2554" sqref="A2554:A2572"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -61765,6 +61765,490 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2553" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2553" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2553" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2553" s="1">
+        <v>133</v>
+      </c>
+      <c r="D2553" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2553" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2553" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2553" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2553" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2554" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2554" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2554" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2554" s="1">
+        <v>163</v>
+      </c>
+      <c r="D2554" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2554" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2554" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2554" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2554" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2555" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2555" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2555" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2555" s="1">
+        <v>47</v>
+      </c>
+      <c r="D2555" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2555" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2555" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2555" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2555" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2556" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2556" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2556" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2556" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2556" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2556" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2556" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2556" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2556" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2557" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2557" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2557" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2557" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2557" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2557" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2557" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2557" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2558" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2558" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2558" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2558" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2558" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2558" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2558" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2558" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2558" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2559" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2559" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2559" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2559" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2559" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2559" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2559" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2559" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2560" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2560" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2560" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2560" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2560" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2560" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2560" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2560" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2560" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2561" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2561" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2561" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2561" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2561" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2561" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2561" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2561" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2562" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2562" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2562" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2562" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2562" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2562" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2563" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2563" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2563" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2563" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2563" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2563" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2563" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2564" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2564" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2564" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2564" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2564" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2564" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2564" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2564" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2565" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2565" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2565" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2565" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2565" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2565" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2565" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2565" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2566" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2566" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2566" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2566" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2566" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2566" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2566" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2566" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2566" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2567" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2567" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2567" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2567" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2567" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2567" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2568" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2568" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2568" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2568" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2568" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2568" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2568" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2569" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2569" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2569" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2569" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2569" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2569" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2569" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2569" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2569" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2570" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2570" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2570" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2570" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2570" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2570" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2570" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2570" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2571" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2571" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2571" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2571" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2571" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2571" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2571" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2571" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2572" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2572" s="2">
+        <v>44063</v>
+      </c>
+      <c r="B2572" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2572" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2572" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2572" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2572" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2572" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts- Pending fixes aggregate Spain and Spain CCAA
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1512AA00-78E0-44E3-991D-773D229DD738}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2852F3-B896-4ED1-9D3F-514DD3BCBE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10292" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10372" uniqueCount="39">
   <si>
     <t>fecha</t>
   </si>
@@ -547,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2572"/>
+  <dimension ref="A1:J2592"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2545" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2554" sqref="A2554:A2572"/>
+    <sheetView tabSelected="1" topLeftCell="A2565" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2574" sqref="A2574:A2592"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62249,6 +62249,487 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2573" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2573" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2573" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2573" s="1">
+        <v>134</v>
+      </c>
+      <c r="D2573" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2573" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2573" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2573" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2573" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2574" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2574" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2574" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2574" s="1">
+        <v>174</v>
+      </c>
+      <c r="D2574" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2574" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2574" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2574" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2574" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2575" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2575" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2575" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2575" s="1">
+        <v>50</v>
+      </c>
+      <c r="D2575" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2575" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2575" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2575" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2575" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2576" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2576" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2576" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2576" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2576" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2576" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2576" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2576" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2576" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2577" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2577" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2577" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2577" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2577" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2577" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2577" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2577" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2577" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2578" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2578" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2578" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2578" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2578" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2578" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2578" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2578" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2578" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2579" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2579" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2579" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2579" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2579" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2579" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2579" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2579" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2580" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2580" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2580" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2580" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2580" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2580" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2580" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2580" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2581" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2581" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2581" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2581" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2581" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2581" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2581" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2581" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2581" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2582" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2582" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2582" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2582" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2582" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2582" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2582" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2583" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2583" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2583" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2583" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2583" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2583" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2583" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2583" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2584" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2584" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2584" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2584" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2584" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2584" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2584" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2584" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2585" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2585" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2585" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2585" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2585" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2585" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2585" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2585" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2586" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2586" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2586" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2586" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2586" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2586" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2586" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2586" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2587" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2587" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2587" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E2587" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2587" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2587" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2587" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2588" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2588" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2588" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2588" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2588" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2588" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2588" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2588" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2589" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2589" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2589" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2589" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2589" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2589" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2589" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2589" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2589" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2590" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2590" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2590" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2590" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2590" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2590" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2590" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2590" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2591" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2591" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2591" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2591" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2591" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2591" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2591" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2591" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2592" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2592" s="2">
+        <v>44064</v>
+      </c>
+      <c r="B2592" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2592" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2592" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2592" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2592" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2592" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain and EUS data-charts 2020.08.23
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E2852F3-B896-4ED1-9D3F-514DD3BCBE43}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F2A13E-C9F7-498B-A7EA-C06D52126A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$197</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10372" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10548" uniqueCount="43">
   <si>
     <t>fecha</t>
   </si>
@@ -145,6 +145,18 @@
   </si>
   <si>
     <t>Fuente Aragón Hoy</t>
+  </si>
+  <si>
+    <t>C.S. Fraga - Bajo Cinca</t>
+  </si>
+  <si>
+    <t>Hospital de Jaca</t>
+  </si>
+  <si>
+    <t>Jaca</t>
+  </si>
+  <si>
+    <t>Transparencia Aragón</t>
   </si>
 </sst>
 </file>
@@ -547,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2592"/>
+  <dimension ref="A1:J2636"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2565" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A2574" sqref="A2574:A2592"/>
+    <sheetView tabSelected="1" topLeftCell="A2621" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B2635" sqref="B2635"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -62730,6 +62742,1051 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2593" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2593" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2593" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2593" s="1">
+        <v>119</v>
+      </c>
+      <c r="D2593" s="1">
+        <v>19</v>
+      </c>
+      <c r="E2593" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2593" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2593" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2593" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2594" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2594" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2594" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2594" s="1">
+        <v>151</v>
+      </c>
+      <c r="D2594" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2594" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2594" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2594" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2594" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2595" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2595" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2595" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2595" s="1">
+        <v>38</v>
+      </c>
+      <c r="D2595" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2595" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2595" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2595" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2595" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2596" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2596" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2596" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2596" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2596" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2596" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2596" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2596" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2596" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2597" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2597" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2597" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2597" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2597" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2597" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2597" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2597" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2598" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2598" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2598" s="1">
+        <v>26</v>
+      </c>
+      <c r="D2598" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2598" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2598" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2598" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2598" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2599" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2599" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2599" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2599" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2599" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2599" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2599" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2599" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2599" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2600" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2600" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2600" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2600" s="1">
+        <v>26</v>
+      </c>
+      <c r="D2600" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2600" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2600" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2600" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2600" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2601" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2601" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2601" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2601" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2601" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2601" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2601" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2601" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2601" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2602" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2602" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2602" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2602" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2602" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2602" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2602" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2603" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2603" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2603" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2603" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2603" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2603" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2603" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2603" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2603" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2604" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2604" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2604" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2604" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2604" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2604" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2604" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2604" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2604" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2605" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2605" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2605" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2605" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2605" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2605" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2605" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2606" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2606" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2606" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2606" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2606" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2606" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2606" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2606" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2607" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2607" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2607" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2607" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2607" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2607" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2607" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2607" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2608" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2608" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2608" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2608" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2608" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2608" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2608" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2608" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2609" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2609" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2609" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2609" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2609" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2609" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2609" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2609" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2609" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2610" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2610" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2610" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2610" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2610" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2610" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2610" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2610" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2611" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2611" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2611" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2611" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2611" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2611" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2611" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2612" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2612" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2612" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2612" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2612" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2612" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2612" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2612" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2613" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2613" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2613" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2613" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2613" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2613" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2613" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2614" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2614" s="2">
+        <v>44065</v>
+      </c>
+      <c r="B2614" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2614" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2614" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2614" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2614" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2615" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2615" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2615" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2615" s="1">
+        <v>122</v>
+      </c>
+      <c r="D2615" s="1">
+        <v>20</v>
+      </c>
+      <c r="E2615" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2615" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2615" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2615" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2616" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2616" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2616" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2616" s="1">
+        <v>151</v>
+      </c>
+      <c r="D2616" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2616" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2616" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2616" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2616" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2617" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2617" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2617" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2617" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2617" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2617" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2617" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2617" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2617" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2618" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2618" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2618" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2618" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2618" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2618" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2618" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2618" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2618" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2619" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2619" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2619" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2619" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2619" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2619" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2619" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2619" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2619" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2620" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2620" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2620" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2620" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2620" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2620" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2620" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2620" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2620" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2621" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2621" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2621" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2621" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2621" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2621" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2621" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2621" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2622" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2622" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2622" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2622" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2622" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2622" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2622" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2622" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2622" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2623" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2623" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2623" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2623" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2623" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2623" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2623" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2623" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2623" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2624" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2624" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2624" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2624" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2624" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2624" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2624" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2625" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2625" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2625" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2625" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2625" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2625" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2625" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2625" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2626" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2626" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2626" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2626" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2626" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2626" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2626" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2626" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2627" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2627" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2627" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="E2627" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2627" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2627" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2627" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2628" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2628" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2628" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2628" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2628" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2628" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2628" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2628" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2629" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2629" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2629" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2629" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2629" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2629" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2629" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2629" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2630" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2630" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2630" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2630" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2630" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2630" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2630" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2630" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2631" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2631" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2631" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2631" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2631" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2631" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2631" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2631" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2631" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2632" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2632" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2632" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2632" s="1">
+        <v>28</v>
+      </c>
+      <c r="E2632" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2632" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2632" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2632" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2633" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2633" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2633" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2633" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2633" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2633" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2633" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2634" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2634" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2634" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2634" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2634" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2634" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2634" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2634" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2635" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2635" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2635" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2635" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2635" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2635" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2635" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2636" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2636" s="2">
+        <v>44066</v>
+      </c>
+      <c r="B2636" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2636" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2636" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2636" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2636" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
fix cantabria source. update Spain provinces data-charts 2020.08.23
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24F2A13E-C9F7-498B-A7EA-C06D52126A5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965390B2-4666-4451-BFEF-95F0937AA2CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10548" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10636" uniqueCount="43">
   <si>
     <t>fecha</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2636"/>
+  <dimension ref="A1:J2658"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2621" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B2635" sqref="B2635"/>
+      <selection activeCell="A2638" sqref="A2638:A2658"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -63787,6 +63787,530 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2637" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2637" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2637" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2637" s="1">
+        <v>141</v>
+      </c>
+      <c r="D2637" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2637" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2637" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2637" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2637" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2638" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2638" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2638" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2638" s="1">
+        <v>170</v>
+      </c>
+      <c r="D2638" s="1">
+        <v>24</v>
+      </c>
+      <c r="E2638" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2638" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2638" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2638" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2639" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2639" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2639" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2639" s="1">
+        <v>47</v>
+      </c>
+      <c r="D2639" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2639" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2639" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2639" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2639" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2640" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2640" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2640" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2640" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2640" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2640" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2640" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2640" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2640" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2641" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2641" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2641" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2641" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2641" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2641" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2641" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2641" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2641" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2642" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2642" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2642" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2642" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2642" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2642" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2642" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2642" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2642" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2643" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2643" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2643" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2643" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2643" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2643" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2643" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2643" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2644" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2644" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2644" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2644" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2644" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2644" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2644" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2644" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2644" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2645" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2645" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2645" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2645" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2645" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2645" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2645" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2645" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2645" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2646" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2646" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2646" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2646" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2646" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2646" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2646" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2647" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2647" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2647" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2647" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2647" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2647" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2647" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2647" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2648" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2648" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2648" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2648" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2648" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2648" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2648" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2648" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2649" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2649" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2649" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2649" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2649" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2649" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2649" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2649" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2650" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2650" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2650" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2650" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2650" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2650" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2650" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2650" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2651" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2651" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2651" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2651" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2651" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2651" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2651" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2651" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2652" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2652" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2652" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2652" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2652" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2652" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2652" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2652" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2653" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2653" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2653" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2653" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2653" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2653" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2653" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2653" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2653" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2654" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2654" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2654" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2654" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2654" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2654" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2654" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2654" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2655" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2655" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2655" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2655" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2655" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2655" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2655" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2655" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2656" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2656" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2656" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2656" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2656" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2656" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2656" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2656" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2657" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2657" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2657" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2657" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2657" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2657" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2657" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2658" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2658" s="2">
+        <v>44067</v>
+      </c>
+      <c r="B2658" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2658" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2658" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2658" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2658" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.08.24 II
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965390B2-4666-4451-BFEF-95F0937AA2CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7CC04-5E1C-4AC6-BCE0-97435F9C0A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10636" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10724" uniqueCount="43">
   <si>
     <t>fecha</t>
   </si>
@@ -559,10 +559,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2658"/>
+  <dimension ref="A1:J2680"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2621" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2638" sqref="A2638:A2658"/>
+    <sheetView tabSelected="1" topLeftCell="A2649" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2660" sqref="A2660:A2680"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64311,6 +64311,530 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2659" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2659" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2659" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2659" s="1">
+        <v>134</v>
+      </c>
+      <c r="D2659" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2659" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2659" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2659" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2659" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2660" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2660" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2660" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2660" s="1">
+        <v>167</v>
+      </c>
+      <c r="D2660" s="1">
+        <v>24</v>
+      </c>
+      <c r="E2660" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2660" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2660" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2660" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2661" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2661" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2661" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2661" s="1">
+        <v>49</v>
+      </c>
+      <c r="D2661" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2661" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2661" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2661" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2661" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2662" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2662" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2662" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2662" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2662" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2662" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2662" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2662" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2662" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2663" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2663" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2663" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2663" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2663" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2663" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2663" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2663" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2663" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2664" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2664" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2664" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2664" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2664" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2664" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2664" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2664" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2664" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2665" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2665" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2665" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2665" s="1">
+        <v>13</v>
+      </c>
+      <c r="E2665" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2665" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2665" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2665" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2666" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2666" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2666" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2666" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2666" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2666" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2666" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2666" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2666" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2667" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2667" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2667" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2667" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2667" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2667" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2667" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2667" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2667" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2668" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2668" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2668" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2668" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2668" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2668" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2668" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2669" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2669" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2669" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2669" s="1">
+        <v>11</v>
+      </c>
+      <c r="E2669" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2669" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2669" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2669" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2670" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2670" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2670" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2670" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2670" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2670" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2670" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2670" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2671" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2671" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2671" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2671" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2671" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2671" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2671" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2671" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2672" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2672" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2672" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2672" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2672" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2672" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2672" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2672" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2673" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2673" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2673" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2673" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2673" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2673" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2673" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2673" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2674" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2674" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2674" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2674" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2674" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2674" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2674" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2674" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2675" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2675" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2675" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2675" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2675" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2675" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2675" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2675" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2675" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2676" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2676" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2676" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2676" s="1">
+        <v>26</v>
+      </c>
+      <c r="E2676" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2676" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2676" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2676" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2677" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2677" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2677" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2677" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2677" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2677" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2677" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2677" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2678" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2678" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2678" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2678" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2678" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2678" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2678" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2678" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2679" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2679" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2679" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2679" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2679" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2679" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2679" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2680" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2680" s="2">
+        <v>44068</v>
+      </c>
+      <c r="B2680" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2680" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2680" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2680" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2680" s="4" t="s">
+        <v>42</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain, IT, FR, EUS data-charts 2020.08.25
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59D7CC04-5E1C-4AC6-BCE0-97435F9C0A27}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -18,7 +17,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Hoja1!$A$1:$H$197</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10724" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10809" uniqueCount="43">
   <si>
     <t>fecha</t>
   </si>
@@ -162,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -558,11 +557,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2680"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2702"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2649" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2660" sqref="A2660:A2680"/>
+    <sheetView tabSelected="1" topLeftCell="A2668" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2682" sqref="A2682:A2702"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -64835,6 +64834,521 @@
         <v>42</v>
       </c>
     </row>
+    <row r="2681" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2681" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2681" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2681" s="1">
+        <v>135</v>
+      </c>
+      <c r="D2681" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2681" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2681" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2681" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2681" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2682" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2682" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2682" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2682" s="1">
+        <v>162</v>
+      </c>
+      <c r="D2682" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2682" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2682" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2682" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2682" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2683" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2683" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2683" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2683" s="1">
+        <v>45</v>
+      </c>
+      <c r="D2683" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2683" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2683" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2683" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2683" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2684" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2684" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2684" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2684" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2684" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2684" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2684" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2684" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2684" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2685" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2685" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2685" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2685" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2685" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2685" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2685" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2685" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2685" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2686" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2686" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2686" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2686" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2686" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2686" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2686" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2686" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2686" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2687" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2687" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2687" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2687" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2687" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2687" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2687" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2687" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2688" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2688" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2688" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2688" s="1">
+        <v>29</v>
+      </c>
+      <c r="D2688" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2688" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2688" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2688" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2688" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2689" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2689" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2689" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2689" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2689" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2689" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2689" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2689" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2689" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2690" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2690" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2690" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2690" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2690" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2690" s="1">
+        <v>22125</v>
+      </c>
+    </row>
+    <row r="2691" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2691" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2691" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2691" s="1">
+        <v>10</v>
+      </c>
+      <c r="E2691" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2691" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2691" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2691" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2692" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2692" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2692" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2692" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2692" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2692" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2692" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2692" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2693" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2693" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2693" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2693" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2693" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2693" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2693" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2693" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2694" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2694" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2694" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2694" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2694" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2694" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2694" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2694" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2695" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2695" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2695" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2695" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2695" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2695" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2695" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2695" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2696" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2696" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2696" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2696" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2696" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2696" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2696" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2696" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2697" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2697" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2697" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2697" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2697" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2697" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2697" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2697" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2697" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2698" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2698" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2698" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2698" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2698" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2698" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2698" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2698" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2699" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2699" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2699" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2699" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2699" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2699" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2699" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2699" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2700" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2700" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2700" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2700" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2700" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2700" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2700" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2700" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2701" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2701" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2701" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2701" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2701" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2701" s="1">
+        <v>22125</v>
+      </c>
+    </row>
+    <row r="2702" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2702" s="2">
+        <v>44069</v>
+      </c>
+      <c r="B2702" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2702" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2702" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2702" s="1">
+        <v>22125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020-08-27
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3636128D-3ED7-4947-9C9A-FD0D6EF4C3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10809" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10897" uniqueCount="43">
   <si>
     <t>fecha</t>
   </si>
@@ -161,7 +162,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -557,11 +558,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2702"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J2724"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2668" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2682" sqref="A2682:A2702"/>
+    <sheetView tabSelected="1" topLeftCell="A2708" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H2711" sqref="H2711:H2712"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65349,6 +65350,527 @@
         <v>22125</v>
       </c>
     </row>
+    <row r="2703" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2703" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2703" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2703" s="1">
+        <v>128</v>
+      </c>
+      <c r="D2703" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2703" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2703" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2703" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2703" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2704" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2704" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2704" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2704" s="1">
+        <v>164</v>
+      </c>
+      <c r="D2704" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2704" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2704" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2704" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2704" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2705" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2705" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2705" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2705" s="1">
+        <v>43</v>
+      </c>
+      <c r="D2705" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2705" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2705" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2705" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2705" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2706" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2706" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2706" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2706" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2706" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2706" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2706" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2706" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2707" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2707" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2707" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2707" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2707" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2707" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2707" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2707" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2707" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2708" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2708" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2708" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2708" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2708" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2708" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2708" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2708" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2708" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2709" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2709" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2709" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2709" s="1">
+        <v>15</v>
+      </c>
+      <c r="E2709" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2709" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2709" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2709" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2710" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2710" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2710" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2710" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2710" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2710" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2710" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2710" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2710" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2711" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2711" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2711" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2711" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2711" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2711" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2711" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2711" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2711" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2712" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2712" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2712" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2712" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2712" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2712" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2712" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2713" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2713" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2713" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2713" s="1">
+        <v>9</v>
+      </c>
+      <c r="E2713" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2713" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2713" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2713" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2714" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2714" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2714" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2714" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2714" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2714" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2714" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2714" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2715" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2715" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2715" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2715" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2715" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2715" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2715" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2715" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2716" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2716" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2716" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2716" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2716" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2716" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2716" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2716" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2717" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2717" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2717" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2717" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2717" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2717" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2717" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2717" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2718" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2718" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2718" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2718" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2718" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2718" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2718" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2718" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2719" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2719" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2719" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2719" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2719" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2719" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2719" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2719" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2719" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2720" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2720" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2720" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2720" s="1">
+        <v>29</v>
+      </c>
+      <c r="E2720" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2720" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2720" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2720" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2721" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2721" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2721" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2721" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2721" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2721" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2721" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2721" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2722" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2722" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2722" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2722" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2722" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2722" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2722" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2722" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2723" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2723" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2723" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2723" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2723" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2723" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2723" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2724" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2724" s="2">
+        <v>44070</v>
+      </c>
+      <c r="B2724" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2724" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2724" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2724" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2724" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020-08-28 II
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3636128D-3ED7-4947-9C9A-FD0D6EF4C3D9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10897" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10982" uniqueCount="43">
   <si>
     <t>fecha</t>
   </si>
@@ -162,7 +161,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
@@ -558,11 +557,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2724"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2746"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2708" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2711" sqref="H2711:H2712"/>
+    <sheetView tabSelected="1" topLeftCell="A2715" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2726" sqref="A2726:A2746"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -65871,6 +65870,518 @@
         <v>38</v>
       </c>
     </row>
+    <row r="2725" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2725" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2725" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2725" s="1">
+        <v>131</v>
+      </c>
+      <c r="D2725" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2725" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2725" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2725" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2725" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2726" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2726" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2726" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2726" s="1">
+        <v>170</v>
+      </c>
+      <c r="D2726" s="1">
+        <v>20</v>
+      </c>
+      <c r="E2726" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2726" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2726" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2726" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2727" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2727" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2727" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2727" s="1">
+        <v>43</v>
+      </c>
+      <c r="D2727" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2727" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2727" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2727" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2727" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2728" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2728" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2728" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2728" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2728" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2728" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2728" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2728" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2729" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2729" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2729" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2729" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2729" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2729" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2729" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2729" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2729" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2730" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2730" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2730" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2730" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2730" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2730" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2730" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2730" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2730" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2731" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2731" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2731" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2731" s="1">
+        <v>12</v>
+      </c>
+      <c r="E2731" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2731" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2731" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2731" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2732" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2732" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2732" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2732" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2732" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2732" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2732" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2732" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2732" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2733" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2733" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2733" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2733" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2733" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2733" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2733" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2733" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2733" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2734" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2734" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2734" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E2734" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2734" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2734" s="1">
+        <v>22125</v>
+      </c>
+    </row>
+    <row r="2735" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2735" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2735" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2735" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2735" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2735" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2735" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2735" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2736" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2736" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2736" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2736" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2736" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2736" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2736" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2736" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2737" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2737" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2737" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2737" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2737" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2737" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2737" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2737" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2738" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2738" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2738" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2738" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2738" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2738" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2738" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2738" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2739" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2739" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2739" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2739" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2739" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2739" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2739" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2739" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2740" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2740" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2740" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2740" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2740" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2740" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2740" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2740" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2741" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2741" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2741" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2741" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2741" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2741" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2741" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2741" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2741" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2742" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2742" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2742" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2742" s="1">
+        <v>30</v>
+      </c>
+      <c r="E2742" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2742" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2742" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2742" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2743" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2743" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2743" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2743" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2743" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2743" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2743" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2743" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2744" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2744" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2744" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2744" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2744" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2744" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2744" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2744" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2745" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2745" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2745" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E2745" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2745" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2745" s="1">
+        <v>22125</v>
+      </c>
+    </row>
+    <row r="2746" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2746" s="2">
+        <v>44071</v>
+      </c>
+      <c r="B2746" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2746" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2746" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2746" s="1">
+        <v>22125</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain proivinces data-charts 2020.08.30
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="315" yWindow="0" windowWidth="20175" windowHeight="10920"/>
+    <workbookView xWindow="315" yWindow="0" windowWidth="14745" windowHeight="7095"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10982" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11246" uniqueCount="46">
   <si>
     <t>fecha</t>
   </si>
@@ -156,6 +156,15 @@
   </si>
   <si>
     <t>Transparencia Aragón</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200828 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200829 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200830 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -558,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2746"/>
+  <dimension ref="A1:J2812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2715" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2726" sqref="A2726:A2746"/>
+    <sheetView tabSelected="1" topLeftCell="A2781" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2792" sqref="A2792:A2812"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -66382,6 +66391,1722 @@
         <v>22125</v>
       </c>
     </row>
+    <row r="2747" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2747" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2747" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2747" s="1">
+        <v>121</v>
+      </c>
+      <c r="D2747" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2747" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2747" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2747" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2747" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2748" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2748" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2748" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2748" s="1">
+        <v>165</v>
+      </c>
+      <c r="D2748" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2748" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2748" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2748" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2748" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2749" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2749" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2749" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2749" s="1">
+        <v>47</v>
+      </c>
+      <c r="D2749" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2749" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2749" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2749" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2749" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2750" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2750" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2750" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2750" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2750" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2750" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2750" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2750" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2750" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2751" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2751" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2751" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2751" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2751" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2751" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2751" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2751" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2751" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2752" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2752" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2752" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2752" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2752" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2752" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2752" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2752" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2752" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2753" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2753" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2753" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2753" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2753" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2753" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2753" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2753" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2753" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2754" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2754" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2754" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2754" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2754" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2754" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2754" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2754" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2754" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2755" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2755" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2755" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2755" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2755" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2755" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2755" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2755" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2755" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2756" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2756" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2756" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2756" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2756" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2756" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2756" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2756" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2756" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2757" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2757" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2757" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2757" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2757" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2757" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2757" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2757" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2757" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2758" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2758" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2758" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2758" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2758" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2758" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2758" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2758" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2758" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2759" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2759" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2759" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2759" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2759" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2759" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2759" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2759" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2759" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2760" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2760" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2760" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2760" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2760" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2760" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2760" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2760" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2760" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2761" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2761" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2761" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2761" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2761" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2761" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2761" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2761" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2761" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2762" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2762" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2762" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2762" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2762" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2762" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2762" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2762" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2762" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2763" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2763" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2763" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2763" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2763" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2763" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2763" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2763" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2763" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2764" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2764" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2764" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2764" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2764" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2764" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2764" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2764" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2764" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2765" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2765" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2765" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2765" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2765" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2765" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2765" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2765" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2765" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2766" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2766" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2766" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2766" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2766" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2766" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2766" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2766" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2766" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2767" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2767" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2767" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2767" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2767" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2767" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2767" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2767" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2767" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2768" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2768" s="2">
+        <v>44072</v>
+      </c>
+      <c r="B2768" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2768" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2768" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2768" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2768" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2768" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2768" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2769" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2769" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2769" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2769" s="1">
+        <v>126</v>
+      </c>
+      <c r="D2769" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2769" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2769" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2769" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2769" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2770" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2770" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2770" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2770" s="1">
+        <v>166</v>
+      </c>
+      <c r="D2770" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2770" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2770" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2770" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2770" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2771" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2771" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2771" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2771" s="1">
+        <v>49</v>
+      </c>
+      <c r="D2771" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2771" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2771" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2771" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2771" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2772" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2772" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2772" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2772" s="1">
+        <v>9</v>
+      </c>
+      <c r="D2772" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2772" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2772" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2772" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2772" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2773" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2773" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2773" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2773" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2773" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2773" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2773" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2773" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2773" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2774" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2774" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2774" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2774" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2774" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2774" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2774" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2774" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2774" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2775" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2775" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2775" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2775" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2775" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2775" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2775" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2775" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2775" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2776" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2776" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2776" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2776" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2776" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2776" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2776" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2776" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2776" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2777" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2777" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2777" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2777" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2777" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2777" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2777" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2777" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2777" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2778" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2778" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2778" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2778" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2778" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2778" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2778" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2778" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2778" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2779" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2779" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2779" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2779" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2779" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2779" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2779" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2779" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2779" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2780" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2780" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2780" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2780" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2780" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2780" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2780" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2780" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2780" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2781" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2781" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2781" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2781" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2781" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2781" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2781" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2781" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2781" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2782" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2782" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2782" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2782" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2782" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2782" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2782" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2782" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2782" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2783" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2783" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2783" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2783" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2783" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2783" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2783" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2783" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2783" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2784" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2784" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2784" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2784" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2784" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2784" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2784" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2784" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2784" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2785" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2785" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2785" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2785" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2785" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2785" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2785" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2785" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2785" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2786" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2786" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2786" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2786" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2786" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2786" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2786" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2786" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2786" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2787" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2787" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2787" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2787" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2787" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2787" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2787" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2787" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2787" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2788" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2788" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2788" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2788" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2788" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2788" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2788" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2788" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2788" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2789" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2789" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2789" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2789" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2789" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2789" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2789" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2789" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2789" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2790" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2790" s="2">
+        <v>44073</v>
+      </c>
+      <c r="B2790" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2790" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2790" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2790" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2790" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2790" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2790" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2791" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2791" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2791" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2791" s="1">
+        <v>125</v>
+      </c>
+      <c r="D2791" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2791" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2791" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2791" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2791" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2792" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2792" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2792" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2792" s="1">
+        <v>174</v>
+      </c>
+      <c r="D2792" s="1">
+        <v>24</v>
+      </c>
+      <c r="E2792" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2792" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2792" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2792" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2793" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2793" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2793" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2793" s="1">
+        <v>51</v>
+      </c>
+      <c r="D2793" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2793" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2793" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2793" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2793" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2794" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2794" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2794" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2794" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2794" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2794" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2794" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2794" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2794" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2795" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2795" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2795" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2795" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2795" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2795" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2795" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2795" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2795" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2796" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2796" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2796" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2796" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2796" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2796" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2796" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2796" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2796" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2797" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2797" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2797" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2797" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2797" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2797" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2797" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2797" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2797" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2798" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2798" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2798" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2798" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2798" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2798" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2798" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2798" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2798" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2799" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2799" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2799" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2799" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2799" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2799" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2799" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2799" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2799" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2800" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2800" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2800" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2800" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2800" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2800" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2800" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2800" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2800" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2801" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2801" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2801" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2801" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2801" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2801" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2801" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2801" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2801" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2802" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2802" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2802" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2802" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2802" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2802" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2802" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2802" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2802" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2803" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2803" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2803" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2803" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2803" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2803" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2803" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2803" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2803" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2804" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2804" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2804" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2804" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2804" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2804" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2804" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2804" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2804" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2805" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2805" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2805" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2805" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2805" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2805" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2805" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2805" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2805" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2806" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2806" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2806" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2806" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2806" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2806" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2806" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2806" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2806" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2807" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2807" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2807" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2807" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2807" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2807" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2807" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2807" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2807" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2808" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2808" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2808" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2808" s="1">
+        <v>26</v>
+      </c>
+      <c r="D2808" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2808" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2808" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2808" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2808" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2809" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2809" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2809" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2809" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2809" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2809" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2809" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2809" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2809" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2810" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2810" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2810" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2810" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2810" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2810" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2810" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2810" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2810" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2811" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2811" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2811" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2811" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2811" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2811" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2811" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2811" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2811" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2812" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2812" s="2">
+        <v>44074</v>
+      </c>
+      <c r="B2812" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2812" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2812" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2812" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2812" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2812" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2812" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
add non consolidated data in CAT and MAD charts. Update Spain provinves data-charts 2020.08.31
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11246" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11334" uniqueCount="47">
   <si>
     <t>fecha</t>
   </si>
@@ -165,6 +165,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200830 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200831 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -567,10 +570,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2812"/>
+  <dimension ref="A1:J2834"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2781" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2792" sqref="A2792:A2812"/>
+    <sheetView tabSelected="1" topLeftCell="A2803" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2814" sqref="A2814:A2834"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68107,6 +68110,578 @@
         <v>45</v>
       </c>
     </row>
+    <row r="2813" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2813" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2813" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2813" s="1">
+        <v>114</v>
+      </c>
+      <c r="D2813" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2813" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2813" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2813" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2813" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2814" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2814" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2814" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2814" s="1">
+        <v>173</v>
+      </c>
+      <c r="D2814" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2814" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2814" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2814" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2814" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2815" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2815" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2815" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2815" s="1">
+        <v>49</v>
+      </c>
+      <c r="D2815" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2815" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2815" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2815" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2815" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2816" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2816" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2816" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2816" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2816" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2816" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2816" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2816" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2816" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2817" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2817" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2817" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2817" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2817" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2817" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2817" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2817" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2817" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2818" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2818" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2818" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2818" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2818" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2818" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2818" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2818" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2818" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2819" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2819" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2819" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2819" s="1">
+        <v>15</v>
+      </c>
+      <c r="D2819" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2819" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2819" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2819" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2819" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2820" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2820" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2820" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2820" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2820" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2820" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2820" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2820" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2820" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2821" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2821" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2821" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2821" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2821" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2821" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2821" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2821" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2821" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2822" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2822" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2822" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2822" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2822" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2822" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2822" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2822" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2822" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2823" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2823" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2823" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2823" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2823" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2823" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2823" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2823" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2823" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2824" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2824" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2824" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2824" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2824" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2824" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2824" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2824" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2824" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2825" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2825" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2825" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2825" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2825" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2825" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2825" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2825" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2825" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2826" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2826" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2826" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2826" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2826" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2826" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2826" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2826" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2826" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2827" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2827" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2827" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2827" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2827" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2827" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2827" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2827" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2827" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2828" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2828" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2828" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2828" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2828" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2828" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2828" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2828" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2828" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2829" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2829" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2829" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2829" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2829" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2829" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2829" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2829" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2829" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2830" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2830" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2830" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2830" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2830" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2830" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2830" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2830" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2830" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2831" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2831" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2831" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2831" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2831" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2831" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2831" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2831" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2831" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2832" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2832" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2832" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2832" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2832" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2832" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2832" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2832" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2832" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2833" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2833" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2833" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2833" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2833" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2833" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2833" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2833" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2833" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2834" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2834" s="2">
+        <v>44075</v>
+      </c>
+      <c r="B2834" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2834" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2834" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2834" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2834" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2834" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2834" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.09.02. Fix date hospitalized Andalucía
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11334" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11510" uniqueCount="49">
   <si>
     <t>fecha</t>
   </si>
@@ -168,6 +168,12 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200831 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200901 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200902 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -570,10 +576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2834"/>
+  <dimension ref="A1:J2878"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2803" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2814" sqref="A2814:A2834"/>
+    <sheetView tabSelected="1" topLeftCell="A2847" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2858" sqref="A2858:A2878"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -68682,6 +68688,1150 @@
         <v>46</v>
       </c>
     </row>
+    <row r="2835" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2835" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2835" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2835" s="1">
+        <v>108</v>
+      </c>
+      <c r="D2835" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2835" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2835" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2835" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2835" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2836" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2836" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2836" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2836" s="1">
+        <v>160</v>
+      </c>
+      <c r="D2836" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2836" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2836" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2836" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2836" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2837" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2837" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2837" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2837" s="1">
+        <v>40</v>
+      </c>
+      <c r="D2837" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2837" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2837" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2837" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2837" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2838" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2838" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2838" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2838" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2838" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2838" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2838" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2838" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2838" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2839" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2839" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2839" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2839" s="1">
+        <v>25</v>
+      </c>
+      <c r="D2839" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2839" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2839" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2839" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2839" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2840" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2840" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2840" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2840" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2840" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2840" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2840" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2840" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2840" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2841" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2841" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2841" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2841" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2841" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2841" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2841" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2841" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2841" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2842" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2842" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2842" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2842" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2842" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2842" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2842" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2842" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2842" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2843" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2843" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2843" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2843" s="1">
+        <v>39</v>
+      </c>
+      <c r="D2843" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2843" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2843" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2843" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2843" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2844" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2844" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2844" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2844" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2844" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2844" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2844" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2844" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2844" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2845" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2845" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2845" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2845" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2845" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2845" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2845" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2845" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2845" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2846" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2846" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2846" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2846" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2846" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2846" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2846" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2846" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2846" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2847" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2847" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2847" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2847" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2847" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2847" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2847" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2847" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2847" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2848" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2848" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2848" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2848" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2848" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2848" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2848" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2848" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2848" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2849" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2849" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2849" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2849" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2849" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2849" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2849" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2849" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2849" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2850" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2850" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2850" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2850" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2850" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2850" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2850" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2850" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2850" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2851" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2851" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2851" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2851" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2851" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2851" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2851" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2851" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2851" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2852" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2852" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2852" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2852" s="1">
+        <v>30</v>
+      </c>
+      <c r="D2852" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2852" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2852" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2852" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2852" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2853" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2853" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2853" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2853" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2853" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2853" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2853" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2853" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2853" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2854" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2854" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2854" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2854" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2854" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2854" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2854" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2854" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2854" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2855" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2855" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2855" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2855" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2855" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2855" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2855" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2855" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2855" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2856" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2856" s="2">
+        <v>44076</v>
+      </c>
+      <c r="B2856" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2856" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2856" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2856" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2856" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2856" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2856" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2857" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2857" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2857" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2857" s="1">
+        <v>101</v>
+      </c>
+      <c r="D2857" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2857" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2857" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2857" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2857" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2858" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2858" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2858" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2858" s="1">
+        <v>154</v>
+      </c>
+      <c r="D2858" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2858" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2858" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2858" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2858" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2859" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2859" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2859" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2859" s="1">
+        <v>41</v>
+      </c>
+      <c r="D2859" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2859" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2859" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2859" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2859" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2860" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2860" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2860" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2860" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2860" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2860" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2860" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2860" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2860" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2861" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2861" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2861" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2861" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2861" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2861" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2861" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2861" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2861" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2862" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2862" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2862" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2862" s="1">
+        <v>22</v>
+      </c>
+      <c r="D2862" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2862" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2862" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2862" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2862" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2863" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2863" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2863" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2863" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2863" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2863" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2863" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2863" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2863" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2864" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2864" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2864" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2864" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2864" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2864" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2864" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2864" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2864" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2865" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2865" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2865" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2865" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2865" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2865" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2865" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2865" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2865" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2866" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2866" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2866" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2866" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2866" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2866" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2866" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2866" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2866" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2867" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2867" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2867" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2867" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2867" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2867" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2867" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2867" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2867" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2868" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2868" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2868" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2868" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2868" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2868" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2868" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2868" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2868" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2869" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2869" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2869" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2869" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2869" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2869" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2869" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2869" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2869" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2870" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2870" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2870" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2870" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2870" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2870" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2870" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2870" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2870" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2871" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2871" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2871" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2871" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2871" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2871" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2871" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2871" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2871" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2872" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2872" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2872" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2872" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2872" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2872" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2872" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2872" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2872" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2873" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2873" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2873" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2873" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2873" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2873" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2873" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2873" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2873" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2874" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2874" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2874" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2874" s="1">
+        <v>32</v>
+      </c>
+      <c r="D2874" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2874" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2874" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2874" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2874" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2875" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2875" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2875" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2875" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2875" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2875" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2875" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2875" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2875" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2876" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2876" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2876" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2876" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2876" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2876" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2876" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2876" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2876" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2877" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2877" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2877" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2877" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2877" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2877" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2877" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2877" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2878" s="2">
+        <v>44077</v>
+      </c>
+      <c r="B2878" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2878" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2878" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2878" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2878" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2878" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2878" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts. fix cases 7 and 4 days. 2020-09-03
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11510" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11598" uniqueCount="50">
   <si>
     <t>fecha</t>
   </si>
@@ -174,6 +174,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200902 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200903 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -576,10 +579,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2878"/>
+  <dimension ref="A1:J2900"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2847" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2858" sqref="A2858:A2878"/>
+    <sheetView tabSelected="1" topLeftCell="A2869" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2880" sqref="A2880:A2900"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -69832,6 +69835,578 @@
         <v>48</v>
       </c>
     </row>
+    <row r="2879" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2879" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2879" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2879" s="1">
+        <v>100</v>
+      </c>
+      <c r="D2879" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2879" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2879" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2879" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2879" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2880" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2880" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2880" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2880" s="1">
+        <v>155</v>
+      </c>
+      <c r="D2880" s="1">
+        <v>21</v>
+      </c>
+      <c r="E2880" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2880" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2880" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2880" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2881" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2881" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2881" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2881" s="1">
+        <v>34</v>
+      </c>
+      <c r="D2881" s="1">
+        <v>5</v>
+      </c>
+      <c r="E2881" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2881" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2881" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2881" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2882" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2882" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2882" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2882" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2882" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2882" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2882" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2882" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2882" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2883" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2883" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2883" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2883" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2883" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2883" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2883" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2883" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2883" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2884" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2884" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2884" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2884" s="1">
+        <v>20</v>
+      </c>
+      <c r="D2884" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2884" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2884" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2884" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2884" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2885" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2885" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2885" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2885" s="1">
+        <v>17</v>
+      </c>
+      <c r="D2885" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2885" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2885" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2885" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2885" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2886" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2886" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2886" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2886" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2886" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2886" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2886" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2886" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2886" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2887" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2887" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2887" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2887" s="1">
+        <v>31</v>
+      </c>
+      <c r="D2887" s="1">
+        <v>8</v>
+      </c>
+      <c r="E2887" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2887" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2887" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2887" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2888" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2888" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2888" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2888" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2888" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2888" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2888" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2888" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2888" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2889" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2889" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2889" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2889" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2889" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2889" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2889" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2889" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2889" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2890" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2890" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2890" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2890" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2890" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2890" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2890" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2890" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2890" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2891" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2891" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2891" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2891" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2891" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2891" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2891" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2891" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2891" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2892" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2892" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2892" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2892" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2892" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2892" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2892" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2892" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2892" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2893" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2893" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2893" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2893" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2893" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2893" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2893" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2893" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2893" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2894" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2894" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2894" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2894" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2894" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2894" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2894" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2894" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2894" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2895" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2895" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2895" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2895" s="1">
+        <v>5</v>
+      </c>
+      <c r="D2895" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2895" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2895" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2895" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2895" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2896" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2896" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2896" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2896" s="1">
+        <v>36</v>
+      </c>
+      <c r="D2896" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2896" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2896" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2896" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2896" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2897" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2897" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2897" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2897" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2897" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2897" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2897" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2897" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2897" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2898" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2898" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2898" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2898" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2898" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2898" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2898" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2898" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2898" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2899" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2899" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2899" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2899" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2899" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2899" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2899" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2899" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2899" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2900" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2900" s="2">
+        <v>44078</v>
+      </c>
+      <c r="B2900" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2900" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2900" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2900" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2900" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2900" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2900" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts. Fix daily deaths calculatoin. 2020-09-06
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AB63CE6-0899-4AE4-A3DB-797A6345E787}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539E3BF8-3C75-4B27-BD17-B72E60AF51A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="348" yWindow="348" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="696" yWindow="696" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11686" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11862" uniqueCount="53">
   <si>
     <t>fecha</t>
   </si>
@@ -181,6 +181,12 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200904 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200905 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200906 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -583,10 +589,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2922"/>
+  <dimension ref="A1:J2966"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2902" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2902" sqref="A2902:A2922"/>
+    <sheetView tabSelected="1" topLeftCell="A2946" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2946" sqref="A2946:A2966"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -70983,6 +70989,1150 @@
         <v>50</v>
       </c>
     </row>
+    <row r="2923" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2923" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2923" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2923" s="1">
+        <v>99</v>
+      </c>
+      <c r="D2923" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2923" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2923" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2923" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2923" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2924" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2924" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2924" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2924" s="1">
+        <v>144</v>
+      </c>
+      <c r="D2924" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2924" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2924" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2924" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2924" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2925" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2925" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2925" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2925" s="1">
+        <v>42</v>
+      </c>
+      <c r="D2925" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2925" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2925" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2925" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2925" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2926" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2926" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2926" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2926" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2926" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2926" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2926" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2926" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2926" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2927" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2927" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2927" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2927" s="1">
+        <v>18</v>
+      </c>
+      <c r="D2927" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2927" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2927" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2927" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2927" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2928" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2928" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2928" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2928" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2928" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2928" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2928" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2928" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2928" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2929" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2929" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2929" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2929" s="1">
+        <v>19</v>
+      </c>
+      <c r="D2929" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2929" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2929" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2929" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2929" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2930" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2930" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2930" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2930" s="1">
+        <v>13</v>
+      </c>
+      <c r="D2930" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2930" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2930" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2930" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2930" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2931" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2931" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2931" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2931" s="1">
+        <v>27</v>
+      </c>
+      <c r="D2931" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2931" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2931" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2931" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2931" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2932" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2932" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2932" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2932" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2932" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2932" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2932" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2932" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2932" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2933" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2933" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2933" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2933" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2933" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2933" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2933" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2933" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2933" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2934" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2934" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2934" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2934" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2934" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2934" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2934" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2934" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2934" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2935" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2935" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2935" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2935" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2935" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2935" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2935" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2935" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2935" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2936" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2936" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2936" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2936" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2936" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2936" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2936" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2936" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2936" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2937" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2937" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2937" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2937" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2937" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2937" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2937" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2937" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2937" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2938" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2938" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2938" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2938" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2938" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2938" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2938" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2938" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2938" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2939" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2939" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2939" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2939" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2939" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2939" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2939" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2939" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2939" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2940" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2940" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2940" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2940" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2940" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2940" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2940" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2940" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2940" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2941" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2941" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2941" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2941" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2941" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2941" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2941" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2941" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2941" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2942" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2942" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2942" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2942" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2942" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2942" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2942" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2942" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2942" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2943" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2943" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2943" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2943" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2943" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2943" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2943" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2943" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2943" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2944" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2944" s="2">
+        <v>44080</v>
+      </c>
+      <c r="B2944" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2944" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2944" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2944" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2944" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2944" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2944" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="2945" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2945" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2945" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2945" s="1">
+        <v>109</v>
+      </c>
+      <c r="D2945" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2945" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2945" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2945" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2945" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2946" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2946" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2946" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2946" s="1">
+        <v>158</v>
+      </c>
+      <c r="D2946" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2946" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2946" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2946" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2946" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2947" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2947" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2947" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2947" s="1">
+        <v>46</v>
+      </c>
+      <c r="D2947" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2947" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2947" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2947" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2947" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2948" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2948" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2948" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2948" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2948" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2948" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2948" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2948" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2948" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2949" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2949" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2949" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2949" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2949" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2949" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2949" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2949" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2949" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2950" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2950" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2950" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2950" s="1">
+        <v>15</v>
+      </c>
+      <c r="D2950" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2950" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2950" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2950" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2950" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2951" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2951" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2951" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2951" s="1">
+        <v>23</v>
+      </c>
+      <c r="D2951" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2951" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2951" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2951" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2951" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2952" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2952" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2952" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2952" s="1">
+        <v>13</v>
+      </c>
+      <c r="D2952" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2952" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2952" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2952" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2952" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2953" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2953" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2953" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2953" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2953" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2953" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2953" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2953" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2953" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2954" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2954" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2954" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2954" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2954" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2954" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2954" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2954" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2954" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2955" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2955" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2955" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2955" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2955" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2955" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2955" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2955" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2955" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2956" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2956" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2956" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2956" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2956" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2956" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2956" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2956" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2956" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2957" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2957" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2957" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2957" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2957" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2957" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2957" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2957" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2957" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2958" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2958" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2958" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2958" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2958" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2958" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2958" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2958" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2958" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2959" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2959" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2959" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2959" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2959" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2959" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2959" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2959" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2959" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2960" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2960" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2960" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2960" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2960" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2960" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2960" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2960" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2960" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2961" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2961" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2961" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2961" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2961" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2961" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2961" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2961" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2961" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2962" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2962" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2962" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2962" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2962" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2962" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2962" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2962" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2962" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2963" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2963" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2963" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2963" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2963" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2963" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2963" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2963" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2963" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2964" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2964" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2964" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2964" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2964" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2964" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2964" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2964" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2964" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2965" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2965" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2965" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2965" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2965" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2965" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2965" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2965" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2965" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2966" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2966" s="2">
+        <v>44081</v>
+      </c>
+      <c r="B2966" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2966" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2966" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2966" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2966" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2966" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2966" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-chart 2020.09.08
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{539E3BF8-3C75-4B27-BD17-B72E60AF51A6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1398011-D655-47C6-9FCA-D901A693960A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="696" yWindow="696" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1044" yWindow="1044" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11862" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11950" uniqueCount="54">
   <si>
     <t>fecha</t>
   </si>
@@ -187,6 +187,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200906 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200907 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -589,10 +592,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2966"/>
+  <dimension ref="A1:J2988"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2946" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2946" sqref="A2946:A2966"/>
+    <sheetView tabSelected="1" topLeftCell="A2968" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2968" sqref="A2968:A2988"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72133,6 +72136,578 @@
         <v>52</v>
       </c>
     </row>
+    <row r="2967" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2967" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2967" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2967" s="1">
+        <v>104</v>
+      </c>
+      <c r="D2967" s="1">
+        <v>23</v>
+      </c>
+      <c r="E2967" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2967" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2967" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2967" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2968" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2968" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2968" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2968" s="1">
+        <v>152</v>
+      </c>
+      <c r="D2968" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2968" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2968" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2968" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2968" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2969" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2969" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2969" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2969" s="1">
+        <v>46</v>
+      </c>
+      <c r="D2969" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2969" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2969" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2969" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2969" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2970" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2970" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2970" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2970" s="1">
+        <v>12</v>
+      </c>
+      <c r="D2970" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2970" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2970" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2970" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2970" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2971" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2971" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2971" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2971" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2971" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2971" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2971" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2971" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2971" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2972" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2972" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2972" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2972" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2972" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2972" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2972" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2972" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2972" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2973" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2973" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2973" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2973" s="1">
+        <v>24</v>
+      </c>
+      <c r="D2973" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2973" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2973" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2973" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2973" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2974" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2974" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2974" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2974" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2974" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2974" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2974" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2974" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2974" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2975" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2975" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2975" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2975" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2975" s="1">
+        <v>7</v>
+      </c>
+      <c r="E2975" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2975" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2975" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2975" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2976" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2976" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2976" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2976" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2976" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2976" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2976" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2976" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2976" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2977" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2977" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2977" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2977" s="1">
+        <v>7</v>
+      </c>
+      <c r="D2977" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2977" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2977" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2977" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2977" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2978" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2978" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2978" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C2978" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2978" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2978" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2978" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2978" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2978" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2979" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2979" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2979" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2979" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2979" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2979" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F2979" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2979" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2979" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2980" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2980" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2980" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2980" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2980" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2980" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2980" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2980" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2980" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2981" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2981" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2981" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2981" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2981" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2981" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2981" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2981" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2981" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2982" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2982" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2982" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C2982" s="1">
+        <v>4</v>
+      </c>
+      <c r="D2982" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2982" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2982" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2982" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2982" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2983" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2983" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2983" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2983" s="1">
+        <v>6</v>
+      </c>
+      <c r="D2983" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2983" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2983" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2983" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2983" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2984" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2984" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2984" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2984" s="1">
+        <v>35</v>
+      </c>
+      <c r="D2984" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2984" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2984" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2984" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2984" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2985" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2985" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2985" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2985" s="1">
+        <v>2</v>
+      </c>
+      <c r="D2985" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2985" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2985" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2985" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2985" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2986" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2986" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2986" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2986" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2986" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2986" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2986" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2986" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2986" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2987" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2987" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2987" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C2987" s="1">
+        <v>8</v>
+      </c>
+      <c r="D2987" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2987" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2987" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2987" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2987" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2988" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2988" s="2">
+        <v>44082</v>
+      </c>
+      <c r="B2988" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2988" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2988" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2988" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2988" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2988" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2988" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.09.08
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1398011-D655-47C6-9FCA-D901A693960A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C07FAE-E437-4F2D-B914-0525E00127C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1044" yWindow="1044" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1392" yWindow="1392" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11950" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12038" uniqueCount="55">
   <si>
     <t>fecha</t>
   </si>
@@ -190,6 +190,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200907 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200908 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -592,10 +595,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J2988"/>
+  <dimension ref="A1:J3010"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2968" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2968" sqref="A2968:A2988"/>
+    <sheetView tabSelected="1" topLeftCell="A2990" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A2990" sqref="A2990:A3010"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -72708,6 +72711,578 @@
         <v>53</v>
       </c>
     </row>
+    <row r="2989" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2989" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2989" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2989" s="1">
+        <v>103</v>
+      </c>
+      <c r="D2989" s="1">
+        <v>24</v>
+      </c>
+      <c r="E2989" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2989" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2989" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2989" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2990" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2990" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2990" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C2990" s="1">
+        <v>151</v>
+      </c>
+      <c r="D2990" s="1">
+        <v>22</v>
+      </c>
+      <c r="E2990" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2990" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2990" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2990" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2991" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2991" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2991" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C2991" s="1">
+        <v>41</v>
+      </c>
+      <c r="D2991" s="1">
+        <v>4</v>
+      </c>
+      <c r="E2991" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2991" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2991" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2991" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2992" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2992" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2992" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2992" s="1">
+        <v>14</v>
+      </c>
+      <c r="D2992" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2992" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2992" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2992" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2992" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2993" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2993" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2993" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2993" s="1">
+        <v>16</v>
+      </c>
+      <c r="D2993" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2993" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2993" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2993" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2993" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2994" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2994" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2994" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2994" s="1">
+        <v>21</v>
+      </c>
+      <c r="D2994" s="1">
+        <v>2</v>
+      </c>
+      <c r="E2994" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2994" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2994" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2994" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2995" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2995" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2995" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2995" s="1">
+        <v>28</v>
+      </c>
+      <c r="D2995" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2995" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2995" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2995" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H2995" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2996" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2996" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2996" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2996" s="1">
+        <v>11</v>
+      </c>
+      <c r="D2996" s="1">
+        <v>3</v>
+      </c>
+      <c r="E2996" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F2996" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2996" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2996" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2997" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2997" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2997" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2997" s="1">
+        <v>29</v>
+      </c>
+      <c r="D2997" s="1">
+        <v>6</v>
+      </c>
+      <c r="E2997" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2997" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2997" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2997" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2998" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2998" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2998" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C2998" s="1">
+        <v>0</v>
+      </c>
+      <c r="D2998" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2998" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2998" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2998" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H2998" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2999" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2999" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B2999" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2999" s="1">
+        <v>3</v>
+      </c>
+      <c r="D2999" s="1">
+        <v>0</v>
+      </c>
+      <c r="E2999" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2999" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2999" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H2999" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3000" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3000" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3000" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3000" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3000" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3000" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3000" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3000" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3000" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3001" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3001" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3001" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3001" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3001" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3001" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3001" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3001" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3001" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3002" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3002" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3002" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3002" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3002" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3002" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3002" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3002" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3002" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3003" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3003" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3003" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3003" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3003" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3003" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3003" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3003" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3003" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3004" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3004" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3004" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3004" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3004" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3004" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3004" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3004" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3004" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3005" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3005" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3005" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3005" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3005" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3005" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3005" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3005" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3005" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3006" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3006" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3006" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3006" s="1">
+        <v>38</v>
+      </c>
+      <c r="D3006" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3006" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3006" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3006" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3006" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3007" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3007" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3007" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3007" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3007" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3007" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3007" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3007" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3007" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3008" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3008" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3008" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3008" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3008" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3008" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3008" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3008" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3008" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3009" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3009" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3009" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3009" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3009" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3009" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3009" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3009" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3009" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3010" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3010" s="2">
+        <v>44083</v>
+      </c>
+      <c r="B3010" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3010" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3010" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3010" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3010" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3010" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3010" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces data-charts 2020.09.09
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44C07FAE-E437-4F2D-B914-0525E00127C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803BE59-4AD0-4056-B931-4347D932CB13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1392" yWindow="1392" windowWidth="10596" windowHeight="5124" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10608" yWindow="732" windowWidth="10596" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12038" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12126" uniqueCount="56">
   <si>
     <t>fecha</t>
   </si>
@@ -193,6 +193,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200908 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200909 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -595,10 +598,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3010"/>
+  <dimension ref="A1:J3032"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2990" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2990" sqref="A2990:A3010"/>
+    <sheetView tabSelected="1" topLeftCell="A3006" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3012" sqref="A3012:A3032"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -73283,6 +73286,578 @@
         <v>54</v>
       </c>
     </row>
+    <row r="3011" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3011" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3011" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3011" s="1">
+        <v>97</v>
+      </c>
+      <c r="D3011" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3011" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3011" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3011" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3011" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3012" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3012" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3012" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3012" s="1">
+        <v>147</v>
+      </c>
+      <c r="D3012" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3012" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3012" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3012" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3012" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3013" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3013" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3013" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3013" s="1">
+        <v>38</v>
+      </c>
+      <c r="D3013" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3013" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3013" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3013" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3013" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3014" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3014" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3014" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3014" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3014" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3014" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3014" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3014" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3014" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3015" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3015" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3015" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3015" s="1">
+        <v>16</v>
+      </c>
+      <c r="D3015" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3015" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3015" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3015" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3015" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3016" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3016" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3016" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3016" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3016" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3016" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3016" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3016" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3016" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3017" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3017" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3017" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3017" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3017" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3017" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3017" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3017" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3017" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3018" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3018" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3018" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3018" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3018" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3018" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3018" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3018" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3018" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3019" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3019" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3019" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3019" s="1">
+        <v>29</v>
+      </c>
+      <c r="D3019" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3019" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3019" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3019" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3019" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3020" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3020" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3020" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3020" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3020" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3020" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3020" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3020" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3020" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3021" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3021" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3021" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3021" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3021" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3021" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3021" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3021" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3021" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3022" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3022" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3022" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3022" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3022" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3022" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3022" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3022" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3022" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3023" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3023" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3023" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3023" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3023" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3023" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3023" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3023" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3023" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3024" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3024" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3024" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3024" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3024" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3024" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3024" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3024" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3024" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3025" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3025" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3025" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3025" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3025" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3025" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3025" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3025" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3025" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3026" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3026" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3026" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3026" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3026" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3026" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3026" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3026" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3026" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3027" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3027" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3027" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3027" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3027" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3027" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3027" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3027" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3027" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3028" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3028" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3028" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3028" s="1">
+        <v>32</v>
+      </c>
+      <c r="D3028" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3028" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3028" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3028" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3028" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3029" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3029" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3029" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3029" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3029" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3029" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3029" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3029" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3029" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3030" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3030" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3030" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3030" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3030" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3030" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3030" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3030" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3030" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3031" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3031" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3031" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3031" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3031" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3031" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3031" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3031" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3031" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3032" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3032" s="2">
+        <v>44084</v>
+      </c>
+      <c r="B3032" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3032" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3032" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3032" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3032" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3032" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3032" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts FR IT 2020.09.10
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5803BE59-4AD0-4056-B931-4347D932CB13}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E741F3-D88E-49B1-9F04-2209677B0339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10608" yWindow="732" windowWidth="10596" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10956" yWindow="1080" windowWidth="10596" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12126" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12214" uniqueCount="57">
   <si>
     <t>fecha</t>
   </si>
@@ -196,6 +196,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200909 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200910 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -598,10 +601,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3032"/>
+  <dimension ref="A1:J3054"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3006" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3012" sqref="A3012:A3032"/>
+    <sheetView tabSelected="1" topLeftCell="A3028" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3034" sqref="A3034:A3054"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -73858,6 +73861,578 @@
         <v>55</v>
       </c>
     </row>
+    <row r="3033" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3033" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3033" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3033" s="1">
+        <v>97</v>
+      </c>
+      <c r="D3033" s="1">
+        <v>23</v>
+      </c>
+      <c r="E3033" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3033" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3033" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3033" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3034" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3034" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3034" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3034" s="1">
+        <v>144</v>
+      </c>
+      <c r="D3034" s="1">
+        <v>18</v>
+      </c>
+      <c r="E3034" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3034" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3034" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3034" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3035" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3035" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3035" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3035" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3035" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3035" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3035" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3035" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3035" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3036" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3036" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3036" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3036" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3036" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3036" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3036" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3036" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3036" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3037" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3037" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3037" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3037" s="1">
+        <v>13</v>
+      </c>
+      <c r="D3037" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3037" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3037" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3037" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3037" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3038" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3038" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3038" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3038" s="1">
+        <v>19</v>
+      </c>
+      <c r="D3038" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3038" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3038" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3038" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3038" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3039" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3039" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3039" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3039" s="1">
+        <v>32</v>
+      </c>
+      <c r="D3039" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3039" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3039" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3039" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3039" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3040" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3040" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3040" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3040" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3040" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3040" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3040" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3040" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3040" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3041" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3041" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3041" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3041" s="1">
+        <v>28</v>
+      </c>
+      <c r="D3041" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3041" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3041" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3041" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3041" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3042" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3042" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3042" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3042" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3042" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3042" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3042" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3042" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3042" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3043" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3043" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3043" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3043" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3043" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3043" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3043" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3043" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3043" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3044" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3044" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3044" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3044" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3044" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3044" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3044" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3044" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3044" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3045" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3045" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3045" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3045" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3045" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3045" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3045" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3045" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3045" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3046" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3046" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3046" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3046" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3046" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3046" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3046" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3046" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3046" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3047" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3047" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3047" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3047" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3047" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3047" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3047" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3047" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3047" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3048" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3048" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3048" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3048" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3048" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3048" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3048" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3048" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3048" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3049" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3049" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3049" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3049" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3049" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3049" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3049" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3049" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3049" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3050" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3050" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3050" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3050" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3050" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3050" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3050" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3050" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3050" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3051" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3051" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3051" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3051" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3051" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3051" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3051" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3051" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3051" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3052" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3052" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3052" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3052" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3052" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3052" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3052" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3052" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3052" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3053" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3053" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3053" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3053" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3053" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3053" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3053" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3053" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3053" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3054" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3054" s="2">
+        <v>44085</v>
+      </c>
+      <c r="B3054" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3054" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3054" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3054" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3054" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3054" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3054" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.09.11
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13E741F3-D88E-49B1-9F04-2209677B0339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D53D03-B0AC-44E1-B885-7CFB48E7FDB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10956" yWindow="1080" windowWidth="10596" windowHeight="7800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="288" yWindow="228" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12214" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12302" uniqueCount="58">
   <si>
     <t>fecha</t>
   </si>
@@ -199,6 +199,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200910 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200911 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -601,10 +604,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3054"/>
+  <dimension ref="A1:J3076"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3028" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3034" sqref="A3034:A3054"/>
+    <sheetView tabSelected="1" topLeftCell="A3044" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3056" sqref="A3056:A3076"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -74433,6 +74436,578 @@
         <v>56</v>
       </c>
     </row>
+    <row r="3055" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3055" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3055" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3055" s="1">
+        <v>94</v>
+      </c>
+      <c r="D3055" s="1">
+        <v>23</v>
+      </c>
+      <c r="E3055" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3055" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3055" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3055" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3056" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3056" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3056" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3056" s="1">
+        <v>137</v>
+      </c>
+      <c r="D3056" s="1">
+        <v>18</v>
+      </c>
+      <c r="E3056" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3056" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3056" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3056" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3057" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3057" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3057" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3057" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3057" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3057" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3057" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3057" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3057" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3058" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3058" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3058" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3058" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3058" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3058" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3058" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3058" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3058" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3059" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3059" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3059" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3059" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3059" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3059" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3059" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3059" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3059" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3060" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3060" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3060" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3060" s="1">
+        <v>16</v>
+      </c>
+      <c r="D3060" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3060" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3060" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3060" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3060" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3061" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3061" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3061" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3061" s="1">
+        <v>33</v>
+      </c>
+      <c r="D3061" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3061" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3061" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3061" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3061" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3062" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3062" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3062" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3062" s="1">
+        <v>13</v>
+      </c>
+      <c r="D3062" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3062" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3062" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3062" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3062" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3063" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3063" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3063" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3063" s="1">
+        <v>25</v>
+      </c>
+      <c r="D3063" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3063" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3063" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3063" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3063" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3064" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3064" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3064" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3064" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3064" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3064" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3064" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3064" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3064" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3065" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3065" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3065" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3065" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3065" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3065" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3065" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3065" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3065" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3066" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3066" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3066" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3066" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3066" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3066" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3066" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3066" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3066" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3067" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3067" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3067" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3067" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3067" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3067" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3067" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3067" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3067" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3068" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3068" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3068" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3068" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3068" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3068" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3068" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3068" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3068" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3069" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3069" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3069" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3069" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3069" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3069" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3069" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3069" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3069" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3070" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3070" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3070" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3070" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3070" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3070" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3070" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3070" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3070" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3071" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3071" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3071" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3071" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3071" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3071" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3071" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3071" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3071" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3072" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3072" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3072" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3072" s="1">
+        <v>29</v>
+      </c>
+      <c r="D3072" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3072" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3072" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3072" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3072" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3073" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3073" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3073" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3073" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3073" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3073" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3073" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3073" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3073" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3074" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3074" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3074" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3074" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3074" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3074" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3074" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3074" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3074" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3075" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3075" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3075" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3075" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3075" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3075" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3075" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3075" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3075" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3076" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3076" s="2">
+        <v>44086</v>
+      </c>
+      <c r="B3076" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3076" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3076" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3076" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3076" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3076" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3076" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020-09-12
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3D53D03-B0AC-44E1-B885-7CFB48E7FDB5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F445569C-7A03-47C6-A830-3BB078D9907B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="288" yWindow="228" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12302" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12390" uniqueCount="59">
   <si>
     <t>fecha</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200911 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200912 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -604,10 +607,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3076"/>
+  <dimension ref="A1:J3098"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3044" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3056" sqref="A3056:A3076"/>
+    <sheetView tabSelected="1" topLeftCell="A3066" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3078" sqref="A3078:A3098"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -75008,6 +75011,578 @@
         <v>57</v>
       </c>
     </row>
+    <row r="3077" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3077" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3077" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3077" s="1">
+        <v>94</v>
+      </c>
+      <c r="D3077" s="1">
+        <v>23</v>
+      </c>
+      <c r="E3077" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3077" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3077" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3077" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3078" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3078" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3078" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3078" s="1">
+        <v>130</v>
+      </c>
+      <c r="D3078" s="1">
+        <v>16</v>
+      </c>
+      <c r="E3078" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3078" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3078" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3078" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3079" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3079" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3079" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3079" s="1">
+        <v>39</v>
+      </c>
+      <c r="D3079" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3079" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3079" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3079" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3079" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3080" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3080" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3080" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3080" s="1">
+        <v>13</v>
+      </c>
+      <c r="D3080" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3080" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3080" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3080" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3080" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3081" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3081" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3081" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3081" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3081" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3081" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3081" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3081" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3081" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3082" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3082" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3082" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3082" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3082" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3082" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3082" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3082" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3082" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3083" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3083" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3083" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3083" s="1">
+        <v>40</v>
+      </c>
+      <c r="D3083" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3083" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3083" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3083" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3083" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3084" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3084" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3084" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3084" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3084" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3084" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3084" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3084" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3084" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3085" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3085" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3085" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3085" s="1">
+        <v>28</v>
+      </c>
+      <c r="D3085" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3085" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3085" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3085" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3085" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3086" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3086" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3086" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3086" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3086" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3086" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3086" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3086" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3086" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3087" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3087" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3087" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3087" s="1">
+        <v>9</v>
+      </c>
+      <c r="D3087" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3087" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3087" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3087" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3087" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3088" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3088" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3088" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3088" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3088" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3088" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3088" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3088" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3088" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3089" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3089" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3089" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3089" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3089" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3089" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3089" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3089" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3089" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3090" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3090" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3090" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3090" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3090" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3090" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3090" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3090" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3090" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3091" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3091" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3091" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3091" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3091" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3091" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3091" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3091" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3091" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3092" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3092" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3092" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3092" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3092" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3092" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3092" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3092" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3092" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3093" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3093" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3093" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3093" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3093" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3093" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3093" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3093" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3093" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3094" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3094" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3094" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3094" s="1">
+        <v>30</v>
+      </c>
+      <c r="D3094" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3094" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3094" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3094" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3094" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3095" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3095" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3095" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3095" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3095" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3095" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3095" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3095" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3095" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3096" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3096" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3096" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3096" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3096" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3096" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3096" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3096" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3096" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3097" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3097" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3097" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3097" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3097" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3097" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3097" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3097" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3097" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3098" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3098" s="2">
+        <v>44087</v>
+      </c>
+      <c r="B3098" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3098" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3098" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3098" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3098" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3098" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3098" s="1" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain provinces 2020.09.13
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F445569C-7A03-47C6-A830-3BB078D9907B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0208806E-B365-44DA-8433-6C904143FE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="288" yWindow="228" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="636" yWindow="576" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12390" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12478" uniqueCount="60">
   <si>
     <t>fecha</t>
   </si>
@@ -205,6 +205,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200912 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200913 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -607,10 +610,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3098"/>
+  <dimension ref="A1:J3120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3066" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3078" sqref="A3078:A3098"/>
+    <sheetView tabSelected="1" topLeftCell="A3088" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3100" sqref="A3100:A3120"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -75583,6 +75586,578 @@
         <v>58</v>
       </c>
     </row>
+    <row r="3099" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3099" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3099" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3099" s="1">
+        <v>99</v>
+      </c>
+      <c r="D3099" s="1">
+        <v>24</v>
+      </c>
+      <c r="E3099" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3099" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3099" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3099" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3100" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3100" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3100" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3100" s="1">
+        <v>130</v>
+      </c>
+      <c r="D3100" s="1">
+        <v>16</v>
+      </c>
+      <c r="E3100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3100" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3100" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3100" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3101" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3101" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3101" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3101" s="1">
+        <v>44</v>
+      </c>
+      <c r="D3101" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3101" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3101" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3101" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3102" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3102" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3102" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3102" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3102" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3102" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3102" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3102" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3102" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3103" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3103" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3103" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3103" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3103" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3103" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3103" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3103" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3103" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3104" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3104" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3104" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3104" s="1">
+        <v>18</v>
+      </c>
+      <c r="D3104" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3104" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3104" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3104" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3105" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3105" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3105" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3105" s="1">
+        <v>41</v>
+      </c>
+      <c r="D3105" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3105" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3105" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3105" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3105" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3106" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3106" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3106" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3106" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3106" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3106" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3106" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3106" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3106" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3107" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3107" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3107" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3107" s="1">
+        <v>29</v>
+      </c>
+      <c r="D3107" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3107" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3107" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3107" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3108" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3108" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3108" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3108" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3108" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3108" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3108" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3108" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3109" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3109" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3109" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3109" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3109" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3109" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3109" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3109" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3109" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3110" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3110" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3110" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3110" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3110" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3110" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3110" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3110" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3111" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3111" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3111" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3111" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3111" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3111" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3111" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3111" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3111" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3112" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3112" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3112" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3112" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3112" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3112" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3112" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3112" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3112" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3113" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3113" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3113" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3113" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3113" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3113" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3113" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3113" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3114" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3114" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3114" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3114" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3114" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3114" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3114" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3114" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3115" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3115" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3115" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3115" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3115" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3115" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3115" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3115" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3116" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3116" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3116" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3116" s="1">
+        <v>29</v>
+      </c>
+      <c r="D3116" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3116" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3116" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3116" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3117" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3117" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3117" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3117" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3117" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3117" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3117" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3117" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3117" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3118" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3118" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3118" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3118" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3118" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3118" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3118" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3118" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3118" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3119" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3119" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3119" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3119" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3119" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3119" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3119" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3119" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3119" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="3120" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3120" s="2">
+        <v>44088</v>
+      </c>
+      <c r="B3120" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3120" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3120" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3120" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3120" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3120" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3120" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.09.14
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0208806E-B365-44DA-8433-6C904143FE71}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B62670-E353-4AC1-AD82-AC661F121A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="636" yWindow="576" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="984" yWindow="924" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12478" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12566" uniqueCount="61">
   <si>
     <t>fecha</t>
   </si>
@@ -208,6 +208,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200913 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200914 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -610,10 +613,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3120"/>
+  <dimension ref="A1:J3142"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3088" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3100" sqref="A3100:A3120"/>
+    <sheetView tabSelected="1" topLeftCell="A3110" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3122" sqref="A3122:A3142"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76158,6 +76161,578 @@
         <v>59</v>
       </c>
     </row>
+    <row r="3121" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3121" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3121" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3121" s="1">
+        <v>99</v>
+      </c>
+      <c r="D3121" s="1">
+        <v>23</v>
+      </c>
+      <c r="E3121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3121" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3121" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3121" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3122" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3122" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3122" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3122" s="1">
+        <v>142</v>
+      </c>
+      <c r="D3122" s="1">
+        <v>19</v>
+      </c>
+      <c r="E3122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3122" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3122" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3122" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3123" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3123" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3123" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3123" s="1">
+        <v>43</v>
+      </c>
+      <c r="D3123" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3123" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3123" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3123" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3124" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3124" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3124" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3124" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3124" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3124" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3124" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3124" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3124" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3125" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3125" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3125" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3125" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3125" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3125" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3125" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3125" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3126" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3126" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3126" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3126" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3126" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3126" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3126" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3126" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3127" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3127" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3127" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3127" s="1">
+        <v>39</v>
+      </c>
+      <c r="D3127" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3127" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3127" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3127" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3127" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3128" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3128" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3128" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3128" s="1">
+        <v>16</v>
+      </c>
+      <c r="D3128" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3128" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3128" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3128" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3128" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3129" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3129" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3129" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3129" s="1">
+        <v>30</v>
+      </c>
+      <c r="D3129" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3129" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3129" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3129" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3129" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3130" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3130" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3130" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3130" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3130" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3130" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3130" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3130" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3131" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3131" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3131" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3131" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3131" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3131" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3131" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3131" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3131" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3132" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3132" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3132" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3132" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3132" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3132" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3132" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3132" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3133" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3133" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3133" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3133" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3133" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3133" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3133" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3133" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3133" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3134" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3134" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3134" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3134" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3134" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3134" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3134" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3134" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3134" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3135" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3135" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3135" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3135" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3135" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3135" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3135" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3135" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3135" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3136" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3136" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3136" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3136" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3136" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3136" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3136" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3136" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3136" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3137" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3137" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3137" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3137" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3137" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3137" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3137" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3137" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3137" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3138" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3138" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3138" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3138" s="1">
+        <v>33</v>
+      </c>
+      <c r="D3138" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3138" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3138" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3138" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3138" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3139" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3139" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3139" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3139" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3139" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3139" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3139" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3139" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3139" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3140" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3140" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3140" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3140" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3140" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3140" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3140" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3140" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3140" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3141" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3141" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3141" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3141" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3141" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3141" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3141" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3141" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3141" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="3142" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3142" s="2">
+        <v>44089</v>
+      </c>
+      <c r="B3142" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3142" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3142" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3142" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3142" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3142" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3142" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.09.15
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9B62670-E353-4AC1-AD82-AC661F121A6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7743D46-78A7-47E4-B62F-CCE28C09B7A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="984" yWindow="924" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12566" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12654" uniqueCount="62">
   <si>
     <t>fecha</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200914 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200915 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -613,10 +616,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3142"/>
+  <dimension ref="A1:J3164"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3110" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3122" sqref="A3122:A3142"/>
+    <sheetView tabSelected="1" topLeftCell="A3132" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3144" sqref="A3144:A3164"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -76733,6 +76736,578 @@
         <v>60</v>
       </c>
     </row>
+    <row r="3143" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3143" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3143" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3143" s="1">
+        <v>98</v>
+      </c>
+      <c r="D3143" s="1">
+        <v>24</v>
+      </c>
+      <c r="E3143" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3143" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3143" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3143" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3144" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3144" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3144" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3144" s="1">
+        <v>138</v>
+      </c>
+      <c r="D3144" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3144" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3144" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3144" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3144" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3145" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3145" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3145" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3145" s="1">
+        <v>43</v>
+      </c>
+      <c r="D3145" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3145" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3145" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3145" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3145" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3146" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3146" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3146" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3146" s="1">
+        <v>9</v>
+      </c>
+      <c r="D3146" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3146" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3146" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3146" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3146" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3147" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3147" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3147" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3147" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3147" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3147" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3147" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3147" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3147" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3148" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3148" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3148" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3148" s="1">
+        <v>13</v>
+      </c>
+      <c r="D3148" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3148" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3148" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3148" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3149" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3149" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3149" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3149" s="1">
+        <v>39</v>
+      </c>
+      <c r="D3149" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3149" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3149" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3149" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3149" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3150" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3150" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3150" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3150" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3150" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3150" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3150" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3150" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3150" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3151" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3151" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3151" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3151" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3151" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3151" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3151" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3151" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3151" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3152" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3152" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3152" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3152" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3152" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3152" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3152" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3152" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3152" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3153" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3153" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3153" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3153" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3153" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3153" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3153" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3153" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3153" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3154" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3154" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3154" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3154" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3154" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3154" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3154" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3154" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3155" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3155" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3155" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3155" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3155" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3155" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3155" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3155" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3155" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3156" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3156" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3156" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3156" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3156" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3156" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3156" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3156" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3157" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3157" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3157" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3157" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3157" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3157" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3157" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3157" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3157" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3158" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3158" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3158" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3158" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3158" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3158" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3158" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3158" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3158" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3159" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3159" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3159" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3159" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3159" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3159" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3159" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3159" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3159" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3160" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3160" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3160" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3160" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3160" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3160" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3160" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3160" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3160" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3161" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3161" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3161" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3161" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3161" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3161" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3161" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3161" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3162" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3162" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3162" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3162" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3162" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3162" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3162" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3162" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3162" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3163" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3163" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3163" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3163" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3163" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3163" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3163" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3163" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3163" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="3164" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3164" s="2">
+        <v>44090</v>
+      </c>
+      <c r="B3164" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3164" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3164" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3164" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3164" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3164" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3164" s="1" t="s">
+        <v>61</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain data-charts 2020.09.16
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7743D46-78A7-47E4-B62F-CCE28C09B7A0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823E915A-A7DC-4F23-B39E-E1B18B64F357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="984" yWindow="924" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="804" yWindow="84" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12654" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12742" uniqueCount="63">
   <si>
     <t>fecha</t>
   </si>
@@ -214,6 +214,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200915 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200916 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -616,10 +619,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3164"/>
+  <dimension ref="A1:J3186"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3144" sqref="A3144:A3164"/>
+      <selection activeCell="A3166" sqref="A3166:A3186"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -77308,6 +77311,578 @@
         <v>61</v>
       </c>
     </row>
+    <row r="3165" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3165" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3165" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3165" s="1">
+        <v>99</v>
+      </c>
+      <c r="D3165" s="1">
+        <v>23</v>
+      </c>
+      <c r="E3165" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3165" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3165" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3165" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3166" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3166" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3166" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3166" s="1">
+        <v>135</v>
+      </c>
+      <c r="D3166" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3166" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3166" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3166" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3166" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3167" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3167" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3167" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3167" s="1">
+        <v>42</v>
+      </c>
+      <c r="D3167" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3167" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3167" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3167" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3168" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3168" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3168" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3168" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3168" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3168" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3168" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3168" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3169" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3169" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3169" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3169" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3169" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3169" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3169" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3169" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3170" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3170" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3170" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3170" s="1">
+        <v>17</v>
+      </c>
+      <c r="D3170" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3170" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3170" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3170" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3171" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3171" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3171" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3171" s="1">
+        <v>39</v>
+      </c>
+      <c r="D3171" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3171" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3171" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3171" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3171" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3172" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3172" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3172" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3172" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3172" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3172" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3172" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3172" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3172" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3173" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3173" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3173" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3173" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3173" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3173" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3173" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3173" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3173" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3174" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3174" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3174" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3174" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3174" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3174" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3174" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3174" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3174" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3175" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3175" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3175" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3175" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3175" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3175" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3175" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3175" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3175" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3176" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3176" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3176" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3176" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3176" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3176" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3176" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3176" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3177" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3177" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3177" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3177" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3177" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3177" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3177" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3177" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3177" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3178" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3178" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3178" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3178" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3178" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3178" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3178" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3178" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3179" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3179" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3179" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3179" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3179" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3179" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3179" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3179" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3179" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3180" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3180" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3180" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3180" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3180" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3180" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3180" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3180" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3181" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3181" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3181" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3181" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3181" s="1">
+        <v>1</v>
+      </c>
+      <c r="E3181" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3181" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3181" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3181" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3182" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3182" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3182" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3182" s="1">
+        <v>38</v>
+      </c>
+      <c r="D3182" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3182" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3182" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3182" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3182" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3183" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3183" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3183" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3183" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3183" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3183" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3183" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3183" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3183" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3184" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3184" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3184" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3184" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3184" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3184" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3184" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3184" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3184" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3185" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3185" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3185" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3185" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3185" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3185" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3185" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3185" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3185" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="3186" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3186" s="2">
+        <v>44091</v>
+      </c>
+      <c r="B3186" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3186" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3186" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3186" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3186" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3186" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3186" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain IT FR data-charts 2020-09-18
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823E915A-A7DC-4F23-B39E-E1B18B64F357}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A28610A-FD1A-40B5-846F-47A2EF4836E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="804" yWindow="84" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="804" yWindow="84" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12742" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12830" uniqueCount="64">
   <si>
     <t>fecha</t>
   </si>
@@ -217,6 +217,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200916 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200917 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -619,10 +622,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3186"/>
+  <dimension ref="A1:J3208"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3166" sqref="A3166:A3186"/>
+    <sheetView tabSelected="1" topLeftCell="A3176" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3188" sqref="A3188:A3208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -77883,6 +77886,578 @@
         <v>62</v>
       </c>
     </row>
+    <row r="3187" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3187" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3187" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3187" s="1">
+        <v>98</v>
+      </c>
+      <c r="D3187" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3187" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3187" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3187" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3187" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3188" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3188" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3188" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3188" s="1">
+        <v>139</v>
+      </c>
+      <c r="D3188" s="1">
+        <v>20</v>
+      </c>
+      <c r="E3188" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3188" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3188" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3188" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3189" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3189" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3189" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3189" s="1">
+        <v>48</v>
+      </c>
+      <c r="D3189" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3189" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3189" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3189" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3189" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3190" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3190" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3190" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3190" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3190" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3190" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3190" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3190" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3190" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3191" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3191" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3191" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3191" s="1">
+        <v>8</v>
+      </c>
+      <c r="D3191" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3191" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3191" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3191" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3191" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3192" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3192" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3192" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3192" s="1">
+        <v>17</v>
+      </c>
+      <c r="D3192" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3192" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3192" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3192" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3192" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3193" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3193" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3193" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3193" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3193" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3193" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3193" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3193" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3193" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3194" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3194" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3194" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3194" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3194" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3194" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3194" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3194" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3194" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3195" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3195" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3195" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3195" s="1">
+        <v>31</v>
+      </c>
+      <c r="D3195" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3195" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3195" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3195" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3195" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3196" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3196" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3196" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3196" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3196" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3196" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3196" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3196" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3196" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3197" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3197" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3197" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3197" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3197" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3197" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3197" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3197" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3197" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3198" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3198" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3198" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3198" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3198" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3198" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3198" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3198" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3199" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3199" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3199" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3199" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3199" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3199" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3199" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3199" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3199" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3200" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3200" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3200" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3200" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3200" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3200" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3200" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3200" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3200" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3201" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3201" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3201" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3201" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3201" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3201" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3201" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3201" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3201" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3202" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3202" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3202" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3202" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3202" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3202" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3202" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3202" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3202" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3203" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3203" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3203" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3203" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3203" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3203" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3203" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3203" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3203" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3204" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3204" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3204" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3204" s="1">
+        <v>37</v>
+      </c>
+      <c r="D3204" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3204" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3204" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3204" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3204" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3205" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3205" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3205" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3205" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3205" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3205" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3205" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3205" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3205" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3206" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3206" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3206" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3206" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3206" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3206" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3206" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3206" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3206" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3207" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3207" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3207" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3207" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3207" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3207" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3207" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3207" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3207" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3208" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3208" s="2">
+        <v>44092</v>
+      </c>
+      <c r="B3208" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3208" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3208" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3208" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3208" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3208" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3208" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
update Spain IT FR data-charts 2020.09.18
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ParaCovid\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A28610A-FD1A-40B5-846F-47A2EF4836E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6757560-53C8-4E4C-8624-0B0C84042DD4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="804" yWindow="84" windowWidth="10608" windowHeight="11316" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12830" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12918" uniqueCount="65">
   <si>
     <t>fecha</t>
   </si>
@@ -220,6 +220,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200917 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200918 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -622,10 +625,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J3208"/>
+  <dimension ref="A1:J3230"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3176" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3188" sqref="A3188:A3208"/>
+    <sheetView tabSelected="1" topLeftCell="A3198" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3210" sqref="A3210:A3230"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -78458,6 +78461,578 @@
         <v>63</v>
       </c>
     </row>
+    <row r="3209" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3209" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3209" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3209" s="1">
+        <v>94</v>
+      </c>
+      <c r="D3209" s="1">
+        <v>21</v>
+      </c>
+      <c r="E3209" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3209" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3209" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3209" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3210" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3210" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3210" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3210" s="1">
+        <v>124</v>
+      </c>
+      <c r="D3210" s="1">
+        <v>19</v>
+      </c>
+      <c r="E3210" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3210" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3210" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3210" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3211" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3211" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3211" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3211" s="1">
+        <v>46</v>
+      </c>
+      <c r="D3211" s="1">
+        <v>5</v>
+      </c>
+      <c r="E3211" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3211" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3211" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3211" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3212" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3212" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3212" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3212" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3212" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3212" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3212" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3212" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3212" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3213" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3213" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3213" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3213" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3213" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3213" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3213" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3213" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3213" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3214" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3214" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3214" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3214" s="1">
+        <v>19</v>
+      </c>
+      <c r="D3214" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3214" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3214" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3214" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3214" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3215" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3215" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3215" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3215" s="1">
+        <v>38</v>
+      </c>
+      <c r="D3215" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3215" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3215" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3215" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3215" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3216" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3216" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3216" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3216" s="1">
+        <v>14</v>
+      </c>
+      <c r="D3216" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3216" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3216" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3216" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3216" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3217" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3217" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3217" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3217" s="1">
+        <v>30</v>
+      </c>
+      <c r="D3217" s="1">
+        <v>6</v>
+      </c>
+      <c r="E3217" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3217" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3217" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3217" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3218" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3218" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3218" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3218" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3218" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3218" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3218" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3218" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3218" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3219" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3219" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3219" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3219" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3219" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3219" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3219" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3219" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3219" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3220" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3220" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3220" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3220" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3220" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3220" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3220" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3220" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3220" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3221" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3221" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3221" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3221" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3221" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3221" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3221" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3221" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3221" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3222" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3222" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3222" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3222" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3222" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3222" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3222" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3222" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3222" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3223" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3223" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3223" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3223" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3223" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3223" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3223" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3223" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3223" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3224" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3224" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3224" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3224" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3224" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3224" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3224" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3224" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3224" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3225" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3225" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3225" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3225" s="1">
+        <v>7</v>
+      </c>
+      <c r="D3225" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3225" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3225" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3225" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3225" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3226" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3226" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3226" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3226" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3226" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3226" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3226" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3226" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3226" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3227" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3227" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3227" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3227" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3227" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3227" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3227" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3227" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3227" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3228" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3228" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3228" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3228" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3228" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3228" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3228" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3228" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3228" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3229" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3229" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3229" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3229" s="1">
+        <v>6</v>
+      </c>
+      <c r="D3229" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3229" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3229" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3229" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3229" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3230" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3230" s="2">
+        <v>44093</v>
+      </c>
+      <c r="B3230" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3230" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3230" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3230" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3230" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3230" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3230" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
udpate Spain FR IT data-charts 2020.09.22
</commit_message>
<xml_diff>
--- a/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
+++ b/data/original/spain/aragon/casos_coronavirus_hospitales.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13182" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13270" uniqueCount="69">
   <si>
     <t>fecha</t>
   </si>
@@ -231,6 +231,9 @@
   </si>
   <si>
     <t>Fuente Servcio Aragonés de Salud - 20200921 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
+  </si>
+  <si>
+    <t>Fuente Servcio Aragonés de Salud - 20200922 COVID-19 SITUACION HOSPITALIZACION.xlsx</t>
   </si>
 </sst>
 </file>
@@ -633,10 +636,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3296"/>
+  <dimension ref="A1:J3318"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3264" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3276" sqref="A3276:A3296"/>
+    <sheetView tabSelected="1" topLeftCell="A3287" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A3298" sqref="A3298:A3318"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -80757,6 +80760,578 @@
         <v>67</v>
       </c>
     </row>
+    <row r="3297" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3297" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3297" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C3297" s="1">
+        <v>87</v>
+      </c>
+      <c r="D3297" s="1">
+        <v>21</v>
+      </c>
+      <c r="E3297" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3297" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3297" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3297" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3298" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3298" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3298" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3298" s="1">
+        <v>150</v>
+      </c>
+      <c r="D3298" s="1">
+        <v>22</v>
+      </c>
+      <c r="E3298" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3298" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3298" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3298" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3299" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3299" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3299" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3299" s="1">
+        <v>51</v>
+      </c>
+      <c r="D3299" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3299" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3299" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3299" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3299" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3300" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3300" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3300" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3300" s="1">
+        <v>12</v>
+      </c>
+      <c r="D3300" s="1">
+        <v>3</v>
+      </c>
+      <c r="E3300" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3300" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3300" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3300" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3301" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3301" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3301" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3301" s="1">
+        <v>11</v>
+      </c>
+      <c r="D3301" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3301" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3301" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3301" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3301" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3302" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3302" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3302" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3302" s="1">
+        <v>15</v>
+      </c>
+      <c r="D3302" s="1">
+        <v>4</v>
+      </c>
+      <c r="E3302" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3302" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3302" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3302" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3303" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3303" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3303" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3303" s="1">
+        <v>42</v>
+      </c>
+      <c r="D3303" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3303" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3303" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3303" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3303" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3304" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3304" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3304" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3304" s="1">
+        <v>13</v>
+      </c>
+      <c r="D3304" s="1">
+        <v>2</v>
+      </c>
+      <c r="E3304" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3304" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3304" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3304" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3305" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3305" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3305" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3305" s="1">
+        <v>33</v>
+      </c>
+      <c r="D3305" s="1">
+        <v>7</v>
+      </c>
+      <c r="E3305" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3305" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3305" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3305" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3306" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3306" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3306" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3306" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3306" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3306" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3306" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3306" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3306" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3307" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3307" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3307" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3307" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3307" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3307" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3307" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3307" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3307" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3308" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3308" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3308" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3308" s="1">
+        <v>4</v>
+      </c>
+      <c r="D3308" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3308" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3308" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G3308" s="1">
+        <v>44216</v>
+      </c>
+      <c r="H3308" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3309" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3309" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3309" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3309" s="1">
+        <v>9</v>
+      </c>
+      <c r="D3309" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3309" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3309" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3309" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3309" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3310" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3310" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3310" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3310" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3310" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3310" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3310" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3310" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3310" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3311" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3311" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3311" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3311" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3311" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3311" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3311" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3311" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3311" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3312" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3312" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3312" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3312" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3312" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3312" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3312" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3312" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3312" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3313" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3313" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3313" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3313" s="1">
+        <v>5</v>
+      </c>
+      <c r="D3313" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3313" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3313" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3313" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3313" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3314" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3314" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3314" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C3314" s="1">
+        <v>35</v>
+      </c>
+      <c r="D3314" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3314" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3314" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3314" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3314" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3315" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3315" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3315" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3315" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3315" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3315" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3315" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3315" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3315" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3316" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3316" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3316" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="C3316" s="1">
+        <v>2</v>
+      </c>
+      <c r="D3316" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3316" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F3316" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3316" s="1">
+        <v>50297</v>
+      </c>
+      <c r="H3316" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3317" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3317" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3317" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C3317" s="1">
+        <v>3</v>
+      </c>
+      <c r="D3317" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3317" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3317" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3317" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3317" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="3318" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3318" s="2">
+        <v>44097</v>
+      </c>
+      <c r="B3318" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3318" s="1">
+        <v>0</v>
+      </c>
+      <c r="D3318" s="1">
+        <v>0</v>
+      </c>
+      <c r="E3318" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3318" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3318" s="1">
+        <v>22125</v>
+      </c>
+      <c r="H3318" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>